<commit_message>
Add further history of public law cards
</commit_message>
<xml_diff>
--- a/flashcards/Memcode - VL Geschichte des Öffentlichen Rechts (JKU, Austria).xlsx
+++ b/flashcards/Memcode - VL Geschichte des Öffentlichen Rechts (JKU, Austria).xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="298">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="416">
   <si>
     <t>Question</t>
   </si>
@@ -19,892 +19,1246 @@
     <t>Answer</t>
   </si>
   <si>
+    <t>&lt;p&gt;Wo sehen Sie die Ungerechtigkeiten im Kurienwahlrecht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Widerspricht &lt;strong&gt;Gleichheitsprinzip&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unterschiedliche &lt;strong&gt;Kurien&lt;/strong&gt; hatten &lt;strong&gt;unterschiedliche Mandatszahlen &lt;/strong&gt;-&amp;gt; mehr/weniger "Wahlmacht" pro Wähler&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Gesetze wurden 1935 in D beschlossen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nürnberger Gesetze &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Dezemberverfassung - &lt;strong&gt;Wer &lt;/strong&gt;darf wählen/&lt;strong&gt;wie &lt;/strong&gt;wird &lt;strong&gt;gewählt&lt;/strong&gt; - was waren die &lt;strong&gt;Streitpunkte&lt;/strong&gt;? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Zensus&lt;/em&gt;: Wahlrecht abhängig von &lt;strong&gt;Steuerleistung &lt;/strong&gt;-&amp;gt; &lt;strong&gt;privilegiert&lt;/strong&gt; &lt;strong&gt;Oberschicht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kurien&lt;/em&gt;: &lt;strong&gt;Wählerklassen &lt;/strong&gt;mit &lt;strong&gt;unterschiedlichen&lt;/strong&gt; &lt;strong&gt;Mandatszahlen &lt;/strong&gt;-&amp;gt; &lt;strong&gt;kein&lt;/strong&gt; &lt;strong&gt;gleiches &lt;/strong&gt;Wahlrecht&lt;/li&gt;&lt;li&gt;&lt;em&gt;Ausschluss der Frau&lt;/em&gt; -&amp;gt; da &lt;strong&gt;kein Militärdienst&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was passierte mit der K u K Monarchie nach dem 1. WK?&lt;/p&gt;&lt;p&gt;Was sind die &lt;strong&gt;Nachfolgestaaten?&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Monarchie ist in &lt;strong&gt;&lt;em&gt;Nationalstaaten &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;zerfallen&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Republik &lt;strong&gt;Deutschösterreich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Republik &lt;strong&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Republik &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Tschechoslowakei&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Republik &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Polen&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Königreich &lt;strong&gt;Jugoslawien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rumänien&lt;/strong&gt;, &lt;strong&gt;Bulgarien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Warum kam die Bezeichnung "Deutschösterreich zustande"?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;nach &lt;/strong&gt;dem &lt;strong&gt;Krieg &lt;/strong&gt;sahen fast &lt;strong&gt;alle polit. Lager&lt;/strong&gt; den neuen, &lt;strong&gt;kleineren&lt;/strong&gt; &lt;strong&gt;Staat &lt;/strong&gt;als &lt;strong&gt;nicht überlebensfähig &lt;/strong&gt;an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Daher der &lt;strong&gt;Wunsch&lt;/strong&gt; nach &lt;strong&gt;Anschluss &lt;/strong&gt;an D&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; Name &lt;strong&gt;Deutschösterreich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Gesetz vom 12. November 1918 über die Staats- und Regierungsform &lt;/em&gt;erkärte &lt;strong&gt;DÖ &lt;/strong&gt;zum &lt;strong&gt;Bestandteil Ds&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Bedeutung hat das Freiteilsrecht für die Entstehung der gewillkürten Erbfolge?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;MA hatte &lt;strong&gt;nur geborene Erben &lt;/strong&gt;-&amp;gt; &lt;em&gt;keine Letztwillige &lt;/em&gt;Verfügung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Freiteil &lt;/strong&gt;war eine &lt;strong&gt;Schenkung &lt;/strong&gt;(Rechtsgeschäft unter lebenden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schuf aber die &lt;strong&gt;Möglichkeit &lt;/strong&gt;einer &lt;strong&gt;quasi-letztwilligen Verfügung &lt;/strong&gt;&lt;em&gt;ohne Zustimmung&lt;/em&gt; von &lt;em&gt;Söhnen&lt;/em&gt;/&lt;em&gt;Frau&lt;/em&gt;&lt;/li&gt;&lt;li&gt;War also ein &lt;strong&gt;Schritt Richtung&lt;/strong&gt; echter &lt;strong&gt;Testierfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Polizei in der NS Zeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Verselbständigung der politischen Polizei: &lt;strong&gt;Gestapo &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;strong&gt;erforschen&lt;/strong&gt;" und "&lt;strong&gt;bekämpfen&lt;/strong&gt;" aller &lt;strong&gt;staatsgefährlichen Bestrebungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine Kontrolle &lt;/strong&gt;durch &lt;strong&gt;Verwaltungsgerichte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Errichtung &lt;/em&gt;der &lt;em&gt;KZs &lt;/em&gt;und &lt;em&gt;Verschleppung &lt;/em&gt;der &lt;em&gt;Opfer &lt;/em&gt;basierte auf dieser &lt;strong&gt;Ermächtigung&lt;/strong&gt; der &lt;strong&gt;Gestapo&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Gesetzgebungsprozess nach der Dezemberverfassung 1867?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Geregelt im &lt;strong&gt;Grundgesetz über Reichsvertretung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Reichsrat &lt;/em&gt;&lt;/strong&gt;aus &lt;strong&gt;Herren&lt;/strong&gt;+ &lt;strong&gt;Abgeordnetenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Abgeordnete &lt;/em&gt;von &lt;em&gt;Landtag &lt;/em&gt;entsandt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Kaiser jährlich &lt;/strong&gt;einberufen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzgebungskompetenzen&lt;/strong&gt; &lt;strong&gt;taxativ &lt;/strong&gt;aufgezählt&lt;/li&gt;&lt;li&gt;Gültiger &lt;strong&gt;&lt;em&gt;Gesetzesbeschluss&lt;/em&gt;&lt;/strong&gt; &lt;em&gt;bedurfte&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zustimmung &lt;strong&gt;beider Häuser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sanktion des &lt;strong&gt;Kaisers &lt;/strong&gt;(&lt;strong&gt;absolutes &lt;/strong&gt;Veto)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Außerordentliche&lt;/strong&gt; &lt;strong&gt;Gesetzgebung &lt;/strong&gt;mittels &lt;strong&gt;Notverordnung &lt;/strong&gt;des Kaisers&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung des Frauenwahlrechts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Becksche Wahlrechtsreform 1907&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Rückschritt -&amp;gt; reines &lt;strong&gt;Männerwahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong&gt;nach 1907 &lt;/strong&gt;gestellten &lt;strong&gt;Anträge&lt;/strong&gt; wurden &lt;strong&gt;nie im Plenum &lt;/strong&gt;diskutiert&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Februar 1919&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erste &lt;/strong&gt;Wahl mit &lt;strong&gt;Frauenwahlrecht&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wahl zur &lt;strong&gt;Konstituierenden Nationalversammlung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Basierend auf dem &lt;em&gt;Gesetz vom 18. Dezember 918 über die Wahlordnung der konstituierenden Nationalversammlung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Handelsgesetzbuch 1861?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Als Entwurf eines &lt;strong&gt;gemeinsamen Handelsrechts&lt;/strong&gt; &lt;strong&gt;1861 &lt;/strong&gt;von der &lt;strong&gt;Bundesversammlung &lt;/strong&gt;des &lt;strong&gt;dt. Bundes&lt;/strong&gt; verabschiedet.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ziel: &lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Einheitlichkeit &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;bei &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Handelsgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Trat in Ö &lt;strong&gt;1863 &lt;/strong&gt;als &lt;strong&gt;Allgemeines Handelsgesetzbuch &lt;/strong&gt;in Kraft&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die ordentliche und außerordentliche Gesetzgebung i&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;m Konstitutionalismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Ordentliche&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;Kaiser&lt;/strong&gt; &lt;strong&gt;einberufener&lt;/strong&gt; &lt;strong&gt;Reichsrat &lt;/strong&gt;arbeitet &lt;strong&gt;Gesetze&lt;/strong&gt; aus&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Außerordentliche&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Kriegsabsolutismus &lt;em&gt;1914-1917&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;für &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;KWEG 1917&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Rassenhygiene?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;NS Zeit&lt;/em&gt;&lt;/p&gt;&lt;p&gt;Umsetzung durch &lt;em&gt;Nürnberger Rassengesetze &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Eheverbote&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zwangssterilisationen &lt;/strong&gt;und &lt;strong&gt;Zwangsabtreibungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bei verschiedenen &lt;strong&gt;Krankheiten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bestimmte &lt;strong&gt;Bevölkerungsgruppen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Schlussendlich &lt;em&gt;Mordprogramm T4&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Rechts-Überleitungsgesetz 1945?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Verfassungs-Überleitungsgesetz&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Setzt &lt;strong&gt;Verfassungsgesetze &lt;/strong&gt;wieder in Kraft&lt;/li&gt;&lt;li&gt;Stand &lt;strong&gt;1933&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Rechts-Überleitungsgesetz&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Setzt &lt;strong&gt;einfachgesetzl&lt;/strong&gt;. &lt;strong&gt;Normen&lt;/strong&gt; wieder in Kraft&lt;/li&gt;&lt;li&gt;Stand &lt;strong&gt;1938&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Behörden-Überleitungsgesetz&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wiederherstellung &lt;strong&gt;Verwaltungs&lt;/strong&gt;- und &lt;strong&gt;Justizbehörden &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1938&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Zweites Verfassungs-Überleitungsgesetz&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Übertragung &lt;strong&gt;Gesetzgebung&lt;/strong&gt;+&lt;strong&gt;Regierungsgewalt &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;von prov&lt;/strong&gt;. &lt;strong&gt;Staatsregierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;auf &lt;strong&gt;Parlament&lt;/strong&gt; + &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wirtschaft im 19. JH?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;&lt;em&gt;Industrielle Revolution&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wandel &lt;strong&gt;Agrar &lt;/strong&gt;zu &lt;strong&gt;Industriegesellschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;&lt;em&gt;In Ö&lt;/em&gt;&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Textil, Metall, Papierindustrie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Urbanisierung &lt;/strong&gt;der Bevölkerung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wohnungsknappheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Arbeitslosigkeit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pauperismus &lt;/strong&gt;- Massenverarmung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Wirtschaftsliberalismus&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Wirtschaftsaufschwung &lt;/strong&gt;durch&lt;strong&gt; Reduktion&lt;/strong&gt; von &lt;strong&gt;Richtlinien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Frage des Zentralistischen/Dezentralistischen Einheitsstaat&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Einigkeit&lt;/strong&gt; über &lt;strong&gt;Staatsform &lt;/strong&gt;der Republik &lt;strong&gt;DÖ&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;em&gt;Eine Ansicht: &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;zentralistischer &lt;/strong&gt;Einheitsstaat&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;prov. Landesversammlungen&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nahmen aber &lt;strong&gt;Recht&lt;/strong&gt; der &lt;strong&gt;Gesetzgebung &lt;/strong&gt;für &lt;strong&gt;Landesbereich &lt;/strong&gt;in Anspruch und &lt;strong&gt;bildeten bundesstaatliches Element&lt;/strong&gt; -&amp;gt; &lt;em&gt;Dezentralisiert&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Rätebewegung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;Bewegung der &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;Arbeiter&lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;- und &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;Soldatenräte&lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt; in den Jahren &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;1918-1924&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;Orientiert an russischen &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(57, 56, 56);"&gt;Sowjets &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Prärogativen der Krone?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Angelegeheiten &lt;/strong&gt;die &lt;strong&gt;auschließlich &lt;/strong&gt;dem &lt;strong&gt;Kaiser &lt;/strong&gt;zustanden&lt;/li&gt;&lt;li&gt;&lt;em&gt;Religion, Strafrecht, Außeres, Krieg&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Hexenverfolgung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Strafprozesse &lt;strong&gt;ohne Straftaten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;ab &lt;strong&gt;16 JH Massenhinrichtungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ziel: &lt;strong&gt;Disziplinierung &lt;/strong&gt;der Frau&lt;/li&gt;&lt;li&gt;Basierend auf &lt;strong&gt;Hexenbulle &lt;/strong&gt;+ &lt;strong&gt;Hexenhammer&lt;/strong&gt;,&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie &lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Constitutio Criminalis Carolina&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Entnazifizierungsgesetze?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Verbotsgesetz&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;NSDAP aufgelöst&lt;/strong&gt; und &lt;strong&gt;verboten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederbetätigungsverbot&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Kriegsverbrechergesetz&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ahndung der &lt;strong&gt;NS-Verbrechen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Staatsvertrag 1955?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Staatsvertrag von Wien&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;15.05.&lt;strong&gt;1955&lt;/strong&gt; in Wien unterzeichnet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beendete Besatzungszeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt: &lt;strong&gt;4 Teile&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Teil I&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Wiederherstellung Ö als &lt;strong&gt;unabhängiger demokratischer Staat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anschlussverbot&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Schutz der &lt;strong&gt;Menschenrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Sicherung der &lt;strong&gt;Demokratie&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Teil II:&lt;/em&gt; &lt;strong&gt;militärische &lt;/strong&gt;Bestimmungen&lt;/p&gt;&lt;p&gt;&lt;em&gt;Teil III&lt;/em&gt;: &lt;strong&gt;Zurückziehen &lt;/strong&gt;der &lt;strong&gt;alliierten &lt;/strong&gt;Streitkräfte bis&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Jahresende 1955&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Teil IV:&lt;/em&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ansprüche &lt;/strong&gt;der &lt;strong&gt;Alliierten &lt;/strong&gt;aus dem Krieg ggü. Ö:&lt;/li&gt;&lt;li&gt;Grundsatz: &lt;strong&gt;keine Reparationszahlungen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Reformation?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1517 Luthers 95 Thesen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Gegen &lt;em&gt;Ablasshandel &lt;/em&gt;gerichtet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;allgemeines Priestertum &lt;/strong&gt;- &lt;em&gt;Laienkelch&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Priesterehe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;löste &lt;/strong&gt;die &lt;strong&gt;Kirche &lt;/strong&gt;aus Amtsgewalt des &lt;strong&gt;Papstes &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gab &lt;strong&gt;Landesherren kirchliche &lt;/strong&gt;Regierungsgewalt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das ius reformandi?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das Recht der &lt;strong&gt;Fürsten &lt;/strong&gt;über die &lt;strong&gt;Religion&lt;/strong&gt; in ihrem &lt;strong&gt;Territorium &lt;/strong&gt;zu &lt;strong&gt;Entscheiden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;aus &lt;strong&gt;Augsburger Religionsfrieden 1555 &lt;/strong&gt;hervorgegangen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vergleich der wichtigsten Inhalte der Verfassungen:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Pillersdorfer 1848&lt;/li&gt;&lt;li&gt;Kremsierer Entwurf 1848/49&lt;/li&gt;&lt;li&gt;Oktroyierte Märzverfassung 1849&lt;/li&gt;&lt;li&gt;Dezemberverfassung 1867&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;img src="https://memcode-production.s3.us-west-2.amazonaws.com/1613752475085"&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Reformen und Patente Joseph II?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Toleranzpatent 1781&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Regelung zur &lt;strong&gt;freien Religionsausübung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Siehe Karte&lt;/li&gt;&lt;li&gt;&lt;em&gt;Agrarreform 1781&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aufhebung&lt;/strong&gt; &lt;strong&gt;Leibeigenschaft&lt;/strong&gt; -&amp;gt; &lt;strong&gt;&lt;em&gt;persönlicher Bezug &lt;/em&gt;&lt;/strong&gt;zu &lt;strong&gt;Grund &lt;/strong&gt;und &lt;strong&gt;Boden Fehlte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Ehegesetzgebung 1783&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Trennung &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ehesakrament &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ehevertrag &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Erbfolgepatent 1786&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einheitliche gesetzl&lt;/strong&gt;. &lt;strong&gt;Erbfolge &lt;/strong&gt;für alle dt. Länder&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;6-Parentel&lt;/strong&gt; System&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die wichtigsten Inhalte der Dezemberverfassung von 1867?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Inhalt&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Frühkonstitutionell&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;/&lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Hochkonstitutionell &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gemischt&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gesetzgebung&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reich&lt;em&gt;rat&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Herren &lt;/strong&gt;+ &lt;strong&gt;Abgeordneten&lt;/strong&gt;haus&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;kein Selbstversammlungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Absolutes &lt;/strong&gt;&lt;strong&gt;Veto &lt;/strong&gt;des Kaisers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Notverordnungsrecht&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wahlrecht&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Wahlmänner&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;volle &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Gewaltenteilung&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichtsbarkeit&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;unabhängig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundrechte&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;StGG&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: konnten in &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Krise ausgesetzt&lt;/strong&gt; werden&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Geltungsbereich&lt;/em&gt;: &lt;strong&gt;nicht &lt;/strong&gt;für &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Reichsgericht ist Vorläufer welches österreichischen Gerichts?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;VfGH&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Aber: &lt;strong&gt;Reichsgericht &lt;/strong&gt;nur &lt;strong&gt;deklaratorische&lt;/strong&gt; Prüfung der Gesetze&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;VfGH kassatorisch&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Bundesexekution im dt. Bund?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ermöglichte &lt;strong&gt;Mitglied &lt;/strong&gt;zur &lt;strong&gt;Einhaltung&lt;/strong&gt; von &lt;strong&gt;Bundesversammlung &lt;/strong&gt;beschlossenen &lt;strong&gt;Verpflichtungen&lt;/strong&gt; zu &lt;strong&gt;zwingen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Bundesintervention im dt. Bund?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Instrument der &lt;strong&gt;Bundesversammlung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ermöglichte in einem &lt;strong&gt;Land &lt;/strong&gt;in dem ein &lt;strong&gt;Aufstand ausgebrochen &lt;/strong&gt;war, auch &lt;strong&gt;ohne Ersuchen &lt;/strong&gt;des &lt;strong&gt;betroffenen Herrschers &lt;/strong&gt;&lt;em&gt;einzugreifen&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Warum wollte DÖ, dass der Vertrag von St. Germain Staatsvertrag heißt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;wegen der &lt;strong&gt;Kriegsschuldfrage&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Nach der &lt;strong&gt;Ansicht &lt;/strong&gt;der &lt;strong&gt;politischen&lt;/strong&gt; &lt;strong&gt;Vertreter DÖs &lt;/strong&gt;befand sich die &lt;strong&gt;Republik &lt;/strong&gt;mit &lt;strong&gt;niemandem&lt;/strong&gt; im &lt;strong&gt;Krieg&lt;/strong&gt; und &lt;em&gt;konnte &lt;/em&gt;daher gar &lt;em&gt;keinen Friedensvertrag &lt;/em&gt;schließen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Warum waren die Toleranzbestimmungen bzgl. Religion von Joseph II notwendig?&lt;/p&gt;&lt;p&gt;Es gab ja den Augsburger Religionsfrieden/Westfälischen Frieden.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;die Duldung&lt;strong&gt; Andersgläubiger &lt;/strong&gt;die im &lt;strong&gt;Westfälischen&lt;/strong&gt; &lt;strong&gt;Frieden &lt;/strong&gt;festgeschrieben wurde &lt;strong&gt;galt für Ö nicht&lt;/strong&gt;! &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Habsburger&lt;/strong&gt; &lt;strong&gt;forcierten &lt;/strong&gt;weiterhin in ihren Erblanden die &lt;strong&gt;katholische Gegenreformation&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;-&amp;gt; Daher&lt;em&gt; Toleranzpatent&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wurde das KWEG 1917 zum Verfassungsgesetz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;mit dem B-VG 1920&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Paktierte Gesetze im Rahmen des Ö-U Ausgleichs?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gesetze zur Regelung dualistischer Angelegenheiten &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welchen Zeitraum umfasst das Mittelalter?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;500-1500 n. Chr.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;libertas affectandi?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Freie Wahl des Erben bei Kinderlosigkeit&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Kurfürsten (in Hinsicht auf die Goldene Bulle)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Ein bevorrechteter Kreis von &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Königswählern &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Erzbischofe&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Pfalzgrafen&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Herzoge &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;ohne Bayern)&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die goldene Bulle?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die goldene Bulle war ein in Urkundenform verfasstes &lt;strong&gt;kaiserliches Gesetzbuch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von &lt;strong&gt;1356-1806&lt;/strong&gt; das &lt;strong&gt;wichtigste der Grundgesetze &lt;/strong&gt;des Heiligen Römischen Reichs&lt;/li&gt;&lt;li&gt;Es regelte vor allem die Modalitäten der &lt;strong&gt;Wahl und der Krönung der römisch-deutschen Könige und Kaiser&lt;/strong&gt; durch die Kurfürsten. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;schriftliche&lt;/strong&gt; &lt;strong&gt;Fixierung &lt;/strong&gt;des sich gewohnheitsrechtlich herausgebildeten Wahlrechts. &lt;/li&gt;&lt;li&gt;Aktiv &lt;strong&gt;wahlberechtigt &lt;/strong&gt;waren ausschließlich die drei geistlichen und die vier weltlichen Kurfürsten. &lt;/li&gt;&lt;li&gt;Festgelegt wurden das &lt;strong&gt;Majoritätsprinzip &lt;/strong&gt;und der Grundsatz der &lt;strong&gt;örtlichen und zeitlichen Einheit&lt;/strong&gt; der Wahl.&lt;/li&gt;&lt;li&gt;Dieses Gesetz machte das Reich zu einem&lt;strong&gt; föderalen Staatsgebilde&lt;/strong&gt; und blieb bis zum Ende 1806 bestehen. &lt;/li&gt;&lt;li&gt;Die Goldene Bulle diente vor allem dazu, das römische bzw. &lt;strong&gt;päpstliche Einmischen zu unterbinden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;König war oberster Lehnsherr&lt;/strong&gt; des Reiches, führte den Oberbefehl über das Reichsheer und verfügte über die Regalien (nutzbare königliche Hoheitsrechte).&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;&amp;nbsp;Wie war das Wahlrecht vor der Goldenen Bulle? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Das Wahlrecht bewegte sich im Spannungsfeld zwischen dem &lt;strong&gt;Wahlrecht des hohen Adels, Geblütsrecht einer bestimmten Dynastie und kirchlichen Ansprüchen&lt;/strong&gt;. Vor der Goldenen Bulle wurde der Kaiser vom Papst in Rom gekrönt, dem deutschen König kam eine Anwartschaft auf diese Kaiserkrönung zu. Daraus leitete das Papsttum eine Reihe umstrittener Rechte ab&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Approbation der deutschen Kaiserwahl&lt;/li&gt;&lt;li&gt;Reichsvikariat solange der Thron unbesetzt war&lt;/li&gt;&lt;li&gt;Depositionsrecht bzgl. des Königs/Kaisers&lt;/li&gt;&lt;li&gt;Recht, das Imperium auf ein anderes Reich zu übertragen&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war der Augsburger Religionsfriede?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1517 Martin Luthers 95 Thesen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reform &lt;/strong&gt;der &lt;strong&gt;Kirche -&amp;gt; &lt;/strong&gt;v.a. gegen &lt;strong&gt;Ablasshandel&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;u.a. &lt;strong&gt;Kirchliche Regierungsgewalt &lt;/strong&gt;für &lt;strong&gt;Landesherren&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Karl V&lt;/strong&gt; verhängt &lt;strong&gt;Reichsacht &lt;/strong&gt;über Luther&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Protestanten &lt;/strong&gt;(evangelische Reichsstände) formen &lt;strong&gt;Schmalkaldischen Bund -&amp;gt; Krieg &lt;/strong&gt;mit Kaiser und Katholiken&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kaiser &lt;/strong&gt;erkennt, dass &lt;strong&gt;Protestantismus nicht militärisch &lt;/strong&gt;besiegt werden kann&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1552 &lt;/strong&gt;vorläufiger Frieden mit &lt;strong&gt;Passauer Vertrag &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1555 Augsburger Reichstag&lt;/strong&gt;: &lt;strong&gt;Langfristiger Friede &lt;/strong&gt;nach langen Verhandlungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Freie Religionsausübung &lt;/strong&gt;für jeden &lt;strong&gt;Fürsten &lt;/strong&gt;in &lt;strong&gt;seinem Land &lt;/strong&gt;(&lt;em&gt;Cuius regio, eius religio&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Untertanen&lt;/strong&gt; dürfen &lt;strong&gt;auswandern&lt;/strong&gt;, wenn sie mit &lt;strong&gt;Bekenntnis &lt;/strong&gt;des Fürsten&lt;strong&gt; &lt;/strong&gt;nicht einverstanden sind&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Hielt &lt;strong&gt;bis 1618 &lt;/strong&gt;→ 30-Jähriger Krieg&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der geistliche Vorbehalt im Zusammenhang mit dem Augsburger Religionsfrieden? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der &lt;strong&gt;reservatum ecclesiasticium &lt;/strong&gt;verhängte über die den Katholizismus aufgebenden geistlichen Territorialherren (Erzbischöfe, Bischöfe, Äbte, Prälaten) den ipso facto (durch diese Tatsache) eintretenden Verlust ihrer Territorien und Kirchenämter.&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das &lt;strong&gt;ius foederis&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Das Recht der Fürsten, Bündnisse zu schließen, sofern sie sich nicht gegen den Kaiser richten&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext des Ermächtigungsgesetzes von 1933? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kontext&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Grundsätze der &lt;strong&gt;Weimarer Reichsverfassung &lt;/strong&gt;sollten &lt;strong&gt;beseitigt &lt;/strong&gt;werden&lt;/li&gt;&lt;li&gt;Am 27. Februar &lt;strong&gt;1933 brannte &lt;/strong&gt;der &lt;strong&gt;Reichstag &lt;/strong&gt;und Marinus van der Lubbe wurde als vermeintlicher Täter verhaftet.&lt;/li&gt;&lt;li&gt;Die Nationalsozialisten nahmen dies zum Anlass, um das &lt;strong&gt;Schreckensbild einer kommunistischen Revolution &lt;/strong&gt;heraufzubeschwören.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Name:&lt;em&gt; Gesetz zur Behebung der Not von Volk und Reich&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Übertragung der &lt;strong&gt;Gesetzgebung &lt;/strong&gt;an die &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesetze &lt;/strong&gt;konnten &lt;strong&gt;Verfassungsändern &lt;/strong&gt;sein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufhebung &lt;/strong&gt;der&lt;strong&gt; Gewaltenteilung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufhebung &lt;/strong&gt;der &lt;strong&gt;Rechtsstaatlichkeit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Unter welchem &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Rechtsmakel &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ist das Ermächtigungsgesetz von 1933 zustande gekommen? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gem. &lt;strong&gt;Artikel 76 der Weimarer Reichsverfassung&lt;/strong&gt; mussten mindestens &lt;strong&gt;2/3&lt;/strong&gt; der Abgeordneten für eine &lt;strong&gt;Verfassungsänderung &lt;/strong&gt;stimmen. &lt;/li&gt;&lt;li&gt;Dieses erhöhte Konsensquorum wurde auch bei der Abstimmung erzielt, allerdings verhinderte die &lt;strong&gt;vorangegangene Verhaftungswelle der gewählten KPD-Mitglieder&lt;/strong&gt; ein rechtskonformes Zustandekommen dieses Gesetzes.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext des Ermächtigungsgesetzes von 1934? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Die &lt;strong&gt;Verfassung von 1934 &lt;/strong&gt;wurde &lt;strong&gt;zwei Mal erlassen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1. Mal:&lt;/em&gt; &lt;strong&gt;VO&lt;/strong&gt; gestützt auf &lt;strong&gt;KWEG&lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; &lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;(Kriegswirtschaftlichen Ermächtigungsgesetz)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;gesamte &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Verfassung&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Inhalt der VO&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Verfassungswidrig: &lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;KWEG ermächtigt nicht &lt;/strong&gt;zum Erlass neuer &lt;strong&gt;Verfassungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Volksabstimmung&lt;/strong&gt; Art 44 (2) &lt;strong&gt;nicht stattgefunden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;2. Mal: &lt;/em&gt;&lt;strong&gt;Geschäftsordnung &lt;/strong&gt;des &lt;strong&gt;NR &lt;/strong&gt;mit &lt;strong&gt;Notverordnung &lt;/strong&gt;basierend auf &lt;strong&gt;KWEG &lt;/strong&gt;geändert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;NR einberufen &lt;/strong&gt;- "&lt;em&gt;Rumpfparlament&lt;/em&gt;" mit &lt;strong&gt;76 Abgeordneten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erlassen das &lt;strong&gt;ErmächtigungsG 1934&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Verfassungswidrig&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Min &lt;strong&gt;83 &lt;/strong&gt;NR &lt;strong&gt;Abgeordnete notwendig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Volksabstimmung nicht &lt;/strong&gt;stattgefunden &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Inhalt&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Art 44 (2) aufgehoben &lt;/strong&gt;-&amp;gt; &lt;strong&gt;keine Volksabstimmung &lt;/strong&gt;bei Gesamtänderung&lt;/li&gt;&lt;li&gt;Die zuvor &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;erlassene&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;VO &lt;/strong&gt;wird zur &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verfassung erhoben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Funktionen von &lt;em&gt;NR &lt;/em&gt;und &lt;em&gt;BR &lt;/em&gt;galten als &lt;em&gt;erloschen &lt;/em&gt;-&amp;gt; &lt;em&gt;Befugnisse &lt;/em&gt;gehen an BReg&lt;/li&gt;&lt;li&gt;&lt;strong&gt;BReg &lt;/strong&gt;erhält &lt;strong&gt;Befugnis Übergang &lt;/strong&gt;zur &lt;strong&gt;neuen Verfassung &lt;/strong&gt;zu regeln und Zeitpunkt der Wirksamkeit festzulegen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext der Dezemberverfassung 1867?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kein Bekenntnis &lt;/strong&gt;zum &lt;strong&gt;Konstitutionalismus&lt;/strong&gt;: Es wurde &lt;strong&gt;keine Verfassung &lt;/strong&gt;erlassen.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sammlung aus &lt;strong&gt;mehreren Gesetzen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Viele &lt;em&gt;Rückgriffe &lt;/em&gt;zur &lt;em&gt;Verfassung &lt;/em&gt;von &lt;em&gt;1849&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Die vom Reichsrat ausgearbeiteten Gesetze stellten einen &lt;strong&gt;Kompromiss &lt;/strong&gt;zwischen den &lt;strong&gt;monarchischen Ansprüchen&lt;/strong&gt; des &lt;strong&gt;Kaisers&lt;/strong&gt; und den &lt;strong&gt;liberalen-konstitutionellen Ideen &lt;/strong&gt;der &lt;strong&gt;Abgeordneten&lt;/strong&gt; dar.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Gesetz über die Verantwortlichkeit der Minister&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierungsakte&lt;/strong&gt; &lt;strong&gt;des Kaisers &lt;/strong&gt;waren von dem &lt;strong&gt;verantwortlichen&lt;/strong&gt; &lt;strong&gt;Minister&lt;/strong&gt; &lt;strong&gt;gegenzuzeichnen&lt;/strong&gt;. Dieser konnte durch vorsätzliche oder grob fahrlässige Verletzung der Verfassung sowie sonstiger Gesetze vom &lt;strong&gt;Reichsrat &lt;/strong&gt;zur &lt;strong&gt;Verantwortung gezogen &lt;/strong&gt;werden (&lt;strong&gt;Ministerialklage&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Grundgesetz über die Reichsvertretung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Das Grundgesetz über die Reichsvertretung&lt;strong&gt; änderte die Form von 1861 ab&lt;/strong&gt;, wodurch der Ausgleich praktisch vorweggenommen wurde:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Reichsrat bestand wie bisher aus &lt;strong&gt;Herren- und Abgeordnetenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Reichsrat sollte j&lt;strong&gt;ährlich vom Kaiser einberufen&lt;/strong&gt; werden&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gesetzgebungskompetenzen&lt;/strong&gt; wurden taxativ &lt;strong&gt;aufgezählt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gesetzesbeschluss bedurfte Zustimmung beider Häuser&lt;/strong&gt; und der &lt;strong&gt;Sanktion durch den Kaiser (=absolutes Veto)&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die allgemeinen Rechte der Staatsbürger&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechtskatalog der Dezemberverfassung, wobei eine Reihe von &lt;strong&gt;liberalen Freiheitsrechten&lt;/strong&gt; normiert wurden, jedoch&lt;strong&gt; keine sozialen oder politischen &lt;/strong&gt;Grundrechte.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;Möglichkeit der Aussetzung der Grundrechte&lt;/strong&gt; stellte eine gravierende Schwäche dar.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über Einsetzung eines Reichsgerichtes&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schuf erstmals die Möglichkeit &lt;strong&gt;Kompetenzkonflikte &lt;/strong&gt;zwischen &lt;strong&gt;Gerichten&lt;/strong&gt; &lt;strong&gt;und Verwaltungsbehörden &lt;/strong&gt;bzw &lt;strong&gt;Ländervertretern und Regierung &lt;/strong&gt;durch verbindlichen &lt;strong&gt;Beschluss des Reichsrates &lt;/strong&gt;zu &lt;strong&gt;lösen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Durch die &lt;strong&gt;Judikatur des Reichsgerichts &lt;/strong&gt;kam es zu einer Präzisierung der Grundrechte. Allerdings besaßen diese Erkenntnisse nur deklaratorischen Charakter, eine &lt;strong&gt;Aufhebung des verfassungswidrigen Aktes konnte nicht angeordnet werden&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die richterliche Gewalt &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stellte die Grundsätze der Gerichtsbarkeit dar (&lt;strong&gt;garantierte richterliche Unabhängigkeit&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kündigte&lt;strong&gt; Regelungen zur Amtshaftung&lt;/strong&gt; an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;legte &lt;strong&gt;Öffentlichkeit der Verfahren &lt;/strong&gt;fest&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;und &lt;strong&gt;Verwaltung &lt;/strong&gt;bestätigt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die Ausübung der Regierungs- und Vollzugsgewalt&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/em&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beschäftigte sich mit der&lt;strong&gt; Person des Kaisers (geheiligt, unverletzlich, unverantwortlich)&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Legalitätsprinzip &lt;em&gt;erstmals &lt;/em&gt;&lt;/strong&gt;festgelegt&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Ausübung der Verwaltung nur aufgrund der Gesetze&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Delegationsgesetz &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ist die &lt;strong&gt;Vollzugsnorm des Ausgleichs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompetenzverteilung zwischen &lt;/strong&gt;den &lt;strong&gt;Reichshälften &lt;/strong&gt;und deren Finanzierung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gemeinsame Organe &lt;/strong&gt;und deren &lt;strong&gt;Handlungsbefugnisse&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie zeigte sich die Ministerverantwortlichkeit in der Dezemberverfassung von 1867?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Jeder der &lt;strong&gt;Kammern &lt;/strong&gt;hatte die Möglichkeit, einen &lt;strong&gt;Minister &lt;/strong&gt;wegen &lt;strong&gt;behaupteter&lt;/strong&gt; &lt;strong&gt;Gesetzesverletzung vor &lt;/strong&gt;einem neu einzurichtenden &lt;strong&gt;Staatsgerichtshof anzuklagen&lt;/strong&gt;.&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie wurde das Notverordnungsrecht in der Dezemberverfassung von 1867 geregelt? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&amp;nbsp;Noch im Juli 1867 wurde das Notverordnungsrecht des Grundgesetzes über die Reichsvertretung präzisiert und die &lt;strong&gt;Geltung der Notverordnungen &lt;/strong&gt;auf den &lt;strong&gt;Zeitraum&lt;/strong&gt; &lt;strong&gt;bis &lt;/strong&gt;zum nächsten &lt;strong&gt;Zusammentritt&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Reichsrates beschränkt&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wenn die &lt;strong&gt;Notverordnungen nicht&lt;/strong&gt; &lt;strong&gt;binnen&lt;/strong&gt; &lt;strong&gt;vier Wochen&lt;/strong&gt; &lt;strong&gt;vorgelegt &lt;/strong&gt;wurden, &lt;strong&gt;erlosch&lt;/strong&gt; die Rechtskraft.&lt;/li&gt;&lt;li&gt;Dem &lt;strong&gt;kaiserlichen&lt;/strong&gt; &lt;strong&gt;Notverordnungsrecht&lt;/strong&gt; wurden &lt;strong&gt;materielle Schranken &lt;/strong&gt;gesetzt. So durften keine Verordnungen erlassen werden, die &lt;strong&gt;Staatsgrundgesetze verändern&lt;/strong&gt;, den &lt;strong&gt;Staatsschatz&lt;/strong&gt; dauernd &lt;strong&gt;belasten &lt;/strong&gt;oder &lt;strong&gt;Staatsgut veräußern&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Das Notverordnungsrecht wurde in der Folge &lt;strong&gt;immer extensiver genutzt &lt;/strong&gt;und mündete zur Zeit des Austrofaschismus in einer Überspannung des Anwendungsrahmens. Allerdings &lt;strong&gt;diente &lt;/strong&gt;es in der Zeit &lt;strong&gt;nach &lt;/strong&gt;der &lt;strong&gt;Dezemberverfassung &lt;/strong&gt;dazu, &lt;strong&gt;unaufschiebbare Materien &lt;/strong&gt;möglichst &lt;strong&gt;zeitnah &lt;/strong&gt;zu &lt;strong&gt;regeln&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die &lt;strong&gt;konstitutionellen &lt;/strong&gt;Elemente der Dezemberverfassung von 1867?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;In Anknüpfung an die Verfassung von 1849 wies die Dezemberverfassung einige konstitutionelle Elemente auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ministerverantwortlichkeit &lt;/strong&gt;(politische und rechtliche Kontrolle)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gewaltentrennung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verbindung der &lt;strong&gt;Volkssouveränität &lt;/strong&gt;mit der &lt;strong&gt;monarchischen&lt;/strong&gt; &lt;strong&gt;Legitimität&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Notverordnungen &lt;/strong&gt;mussten &lt;strong&gt;genehmigt &lt;/strong&gt;werden&amp;nbsp;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des Kaisers &lt;strong&gt;materiellen Schranken &lt;/strong&gt;unterworfen&lt;/li&gt;&lt;li&gt;Auch wenn nur &lt;strong&gt;deklaratorischer &lt;/strong&gt;Charakter, &lt;strong&gt;Überprüfung der Gesetze&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Skizzieren Sie die Entwicklung des Wahlrechts&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Februarpatent 1861&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einrichtung von Reichsrat, eine Art Parlament aus &lt;strong&gt;Abgeordneten&lt;/strong&gt; und &lt;strong&gt;Herrenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herrenhaus von Kaiser &lt;/strong&gt;bestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abgeordnetenhaus von Landtagen &lt;/strong&gt;bestellt, dies gewählt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landtagswahlrecht&lt;/strong&gt;: &lt;strong&gt;Kurienwahlrecht &lt;/strong&gt;(4: Großgrundbesitzer, Städte + Märkte + Industriestandorte, Handels + Gewerbekammern, Landgemeinden) + &lt;strong&gt;Zensuswahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Kurienwahlrecht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Zusammenfassung der&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; Wähler in Wählerklassen&lt;/span&gt;, denen unterschiedliche Mandate zukommen.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Zensuswahlrecht&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Wahlrecht von der &lt;strong&gt;Steuerleistung abhängig&lt;/strong&gt;, da politische Mitwirkungsrechte wirtschaftliche Unabhängigkeit voraussetzten. Dahinter stand die politische Zielsetzung, die &lt;strong&gt;feudale &lt;/strong&gt;und &lt;strong&gt;bürgerliche&lt;/strong&gt; &lt;strong&gt;Oberschicht &lt;/strong&gt;zu &lt;strong&gt;privilegieren&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Frauen nicht ausgeschlossen,&lt;/strong&gt; wenn Steuerleistung erfüllt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1873 &lt;/em&gt;&lt;strong&gt;&lt;em&gt;direkte Wahl der Abgeordneten&lt;/em&gt;&lt;/strong&gt; (ohne Umweg via Landtag), Wahlrecht nur mehr für Männer, außer Großgrundbesitzer&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1882: Taaffe'sche Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zensus &lt;/strong&gt;auf 5 Gulden &lt;strong&gt;gesenkt &lt;/strong&gt;-&amp;gt; mehr Wahlberechtigte &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verschiebung von Wahlbezirken &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1896: Badenische Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;5. Kurie: Allgemeine Wählerklasse&lt;/strong&gt; -&amp;gt; nur Männer&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Erfordert 1 Jahr Sesshaftigkeit &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Senkung von Steuerzensus&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pluralwahlrecht&lt;/strong&gt;: Mitglieder anderer Kurien konnten auch hier wählen. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wenig Einfluss:&lt;/strong&gt; 5. Kurie wählte nur 72/425 Abgeordnete&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1907: Beck’sche Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abschaffung von Kurien+Zensuswahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Allgemeines, gleiches, direktes und geheimes Wahlrecht &lt;strong&gt;für Männer &lt;/strong&gt;→ jetzt gar keine Frauen mehr wählen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Erfordert 1 Jahr Sesshaftigkeit &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aufstockung der Mandate&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1918: Allgemeines Wahlrecht auch für Frauen &lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Von 1933 (Ständestaat) über 1938 (Anschluss) bis 1945 (Republik Österreich) kein Wahlrecht, erst danach wieder. &lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was kennzeichnet die Verfassungsnovelle von 1929?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Auslöser&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;BVG 1920 &lt;/strong&gt;war parteipolitischer &lt;strong&gt;Kompromiss &lt;/strong&gt;zw. &lt;strong&gt;Sozialdemokraten &lt;/strong&gt;und &lt;strong&gt;Christlichsozialen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;die &lt;strong&gt;bürgerlichen&lt;/strong&gt; Lager waren &lt;strong&gt;unzufrieden&lt;/strong&gt; damit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Insb. &lt;strong&gt;Stellung/Wahl&lt;/strong&gt; des &lt;strong&gt;BPräs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Inhalt&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzverschiebung &lt;/strong&gt;zugunsten &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;BPRäs &lt;/strong&gt;hat Recht zu &lt;strong&gt;Einberufung &lt;/strong&gt;und &lt;strong&gt;Auflösung &lt;/strong&gt;des &lt;strong&gt;NR&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie &lt;em&gt;Neuwahlen&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;BReg nicht &lt;/strong&gt;mehr &lt;strong&gt;von NR &lt;/strong&gt;gewählt&lt;/li&gt;&lt;li&gt;BP&lt;/li&gt;&lt;li class="ql-indent-1"&gt;BP vom &lt;strong&gt;Volk gewählt &lt;/strong&gt;(Statt Bundesversammlung)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Absetzung &lt;/strong&gt;durch &lt;strong&gt;Volksabstimmung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ernennt &lt;strong&gt;BK&lt;/strong&gt;, und auf &lt;strong&gt;dessen Vorschlag BReg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Entlässt BReg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des BP nur auf &lt;em&gt;Vorschlag &lt;/em&gt;der &lt;em&gt;BReg &lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bundesrat &lt;/strong&gt;durch &lt;strong&gt;Länder&lt;/strong&gt;- und &lt;strong&gt;Ständerat ersetzt &lt;/strong&gt;-&amp;gt; eigenes B-VG &lt;em&gt;nie erlassen&lt;/em&gt; (also alte Rechtslage)&lt;/li&gt;&lt;li&gt;&lt;em&gt;Neuordnung &lt;/em&gt;der obersten Bundesorgane&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;NR &lt;/strong&gt;und &lt;strong&gt;BPräs gleichgestellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BReg von NR &lt;/strong&gt;und &lt;strong&gt;BPräs abhängig &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;gewünschte &lt;strong&gt;Entpolitisierung &lt;/strong&gt;des &lt;strong&gt;VfGH &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;NR &lt;/strong&gt;nur mehr &lt;strong&gt;Vorschlagsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BReg &lt;/strong&gt;auch &lt;strong&gt;Vorschlagsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ernennung&lt;/strong&gt; durch &lt;strong&gt;BPräs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Folge: &lt;em&gt;nur Umpolitisierung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wurde der BP vor der Verfassungsnovelle 1929 gewählt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Durch die Bundesversammlung&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der Westfälische Friede?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;beendete &lt;/strong&gt;&lt;em&gt;1648 &lt;/em&gt;&lt;strong&gt;den 30-jährigen Krieg &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Zwei Verhandlungsorte:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Münster: &lt;/strong&gt;zwischen Kaiser, den Reichsständen&lt;strong&gt; &lt;/strong&gt;und &lt;strong&gt;Frankreich&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Osnabrück: &lt;/strong&gt;zwischen Kaiser, den Reichsständen&lt;strong&gt; &lt;/strong&gt;und &lt;strong&gt;Schweden&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Ergebnis&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zwei getrennte&lt;/strong&gt;, aber &lt;strong&gt;juristisch &lt;/strong&gt;als &lt;strong&gt;Einheit &lt;/strong&gt;betrachtete &lt;strong&gt;Urkunden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;trat &lt;em&gt;1649 &lt;/em&gt;in &lt;strong&gt;Kraft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Konfessionelle Bestimmungen:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das &lt;strong&gt;reformierte Bekenntnis &lt;/strong&gt;(&lt;strong&gt;Calvin&lt;/strong&gt;) wurde dem &lt;strong&gt;augsburgischen &lt;/strong&gt;(&lt;strong&gt;Luther&lt;/strong&gt;) &lt;strong&gt;gleichgestellt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Augsburger &lt;/strong&gt;Religionsfriede &lt;strong&gt;bestätigt &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Toleranzklausel für Andersgläubige&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Normaltags- &lt;/strong&gt;und &lt;strong&gt;Normaljahrsregelung &lt;/strong&gt;ergänzt:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederherstellung &lt;/strong&gt;des &lt;strong&gt;Besitzstandes &lt;/strong&gt;von Protestanten und Katholiken von&lt;strong&gt; 1. Januar 1624 &lt;/strong&gt;-&amp;gt; Vor allem Rückgängigmachung des &lt;strong&gt;Restitutionsedikts &lt;/strong&gt;von 1629, bei dem Kaiser Protestanten enteignete.&lt;/li&gt;&lt;li&gt;Der&lt;strong&gt; geistliche Vorbehalt&lt;/strong&gt; wurde auch &lt;strong&gt;auf protestantische Bistumsadministratoren ausgedehnt&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;In &lt;strong&gt;Religionsfragen &lt;/strong&gt;hatte der &lt;strong&gt;Reichstag &lt;/strong&gt;nicht in der &lt;strong&gt;Kuriengliederung&lt;/strong&gt;, &lt;strong&gt;sondern &lt;/strong&gt;getrennt nach &lt;strong&gt;Religionsgruppen &lt;/strong&gt;zu beraten.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Allgemeine Verfassungsfragen:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Territorialherrschaft der Reichsstände &lt;/strong&gt;wurde anerkannt.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Struktur an der Reichsspitze&lt;/strong&gt; verändert: &lt;strong&gt;bayrischen&lt;/strong&gt; &lt;strong&gt;Kurwürde&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beratendes Stimmrecht &lt;/strong&gt;der &lt;strong&gt;Reichsstände &lt;/strong&gt;in &lt;strong&gt;volles &lt;/strong&gt;umgewandelt&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;obersten&lt;/strong&gt; &lt;strong&gt;Reichsgerichte &lt;/strong&gt;sollten &lt;strong&gt;paritätisch &lt;/strong&gt;(Konfessionen zahlenmäßig gleich vertreten) besetzt werden.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was unterscheidet den &lt;strong&gt;Augsburger Religionsfrieden &lt;/strong&gt;vom &lt;strong&gt;Westfälischen Frieden&lt;/strong&gt;? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Augsburger Religionsfrieden &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;bezog sich lediglich auf die &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Augsburger&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Konfession&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Luther&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;). &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;westfälische Friede &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;bezog sich nun auch auf das &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;reformierte Bekenntnis&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Calvin&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der österreichisch-ungarische Ausgleich? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;1867&lt;/li&gt;&lt;li&gt;Verfassungsrechtliche Vereinbarung, durch die das Kaisertum Österreich zur &lt;strong&gt;österreichisch-ungarischen Monarchie&lt;/strong&gt; wurde.&lt;/li&gt;&lt;li&gt;Rechtliche Grundlagen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pragmatische Sanktion&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesetzesartikel XII von 1867 für Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Delegationsgesetz 1867&lt;/strong&gt; für Österreich. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ungarn ging dabei von einer abänderbaren Verpflichtung aus, Österreich von einem Vertrag.&lt;/li&gt;&lt;li&gt;Die Rechtsnatur „&lt;strong&gt;Realunion besonderer Art zweier ansonsten selbstständiger Staaten&lt;/strong&gt;“ .&lt;/li&gt;&lt;li class="ql-indent-1"&gt;2 Staaten&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;pragmatischen &lt;/strong&gt;Angelegenheiten &lt;strong&gt;gemeinsam&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;dualistische &lt;/strong&gt;nach &lt;strong&gt;regelmäßig&lt;/strong&gt; zu &lt;strong&gt;vereinbarenden Grundätzen &lt;/strong&gt;zu behandeln waren.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichshälften: Cisleithanien (Österreich), Transleithanien (Ungarn)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt; Pragmatische Angelegenheiten&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Äußeres, Kriegswesen, Finanzen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;gemeinsame &lt;strong&gt;Minister&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Gesetze durch &lt;strong&gt;übereinstimmende&lt;/strong&gt; &lt;strong&gt;Beschlüsse Delegationen &lt;/strong&gt;der beiden &lt;strong&gt;Parlamente &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Militärischer &lt;/strong&gt;Oberbefehl&lt;strong&gt; &lt;/strong&gt;beim &lt;strong&gt;Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Finanzierung aufgeteilt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zustimmung&lt;/strong&gt; von &lt;strong&gt;Reichsrat &lt;/strong&gt;und &lt;strong&gt;Reichstag &lt;/strong&gt;notwendig&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Dualistische Angelegenheiten&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;insb. &lt;strong&gt;Wirtschaftsfragen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Getrennte Gesetze f&lt;/strong&gt;ür je eine Reichshälfte&lt;/li&gt;&lt;li&gt;Von &lt;strong&gt;Ö und U Behörden&lt;/strong&gt; &lt;strong&gt;getrennt &lt;/strong&gt;ausgeführt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht &lt;/strong&gt;von &lt;strong&gt;gemeinsamen Ministerien &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Reichstag, was der Reichsrat in Österreich-Ungarn?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Reichstag: Parlament in Ungarn&lt;/p&gt;&lt;p&gt;Reichsrat: Parlament in Österreich (Eselsbrücke: Öste&lt;strong&gt;rr&lt;/strong&gt;eichs&lt;strong&gt;r&lt;/strong&gt;at)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist eine&lt;strong&gt; Real&lt;/strong&gt;union?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Völkerrechtliche Verbindung selbständiger Staaten durch ein &lt;strong&gt;gemeinsames Staatsoberhaupt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Mit &lt;strong&gt;weiteren gemeinsamen&lt;/strong&gt; &lt;strong&gt;Institutionen&lt;/strong&gt;, also Staatsorganen und Verwaltungseinrichtungen&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Investiturstreit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1076 &lt;/strong&gt;bis &lt;strong&gt;1122 &lt;/strong&gt;(Wormser Konkordat)&lt;/li&gt;&lt;li&gt;Die Durchsetzung des &lt;strong&gt;libertas ecclasiae&lt;/strong&gt; (Kirchenfreiheit) durch &lt;strong&gt;Papst Gregor VII&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konflikt zwischen geistlicher und weltlicher Macht bzgl. &lt;strong&gt;Amtseinsetzungen von Geistlichen durch die weltliche Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kirche gegen Laieninvestitur&lt;/strong&gt;, Heinrich IV für.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eskalation: Heinrich IV lässt &lt;strong&gt;Papst&lt;/strong&gt; &lt;strong&gt;durch Bischofsversammlung in Worms absetzen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;1076&lt;/em&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;&lt;strong&gt;Papst &lt;/strong&gt;Gregor VII &lt;strong&gt;exkommuniziert Heinrich IV&lt;/strong&gt;, u&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ntersagt Regierung und löst Treueeide -&amp;gt;&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; schränkt politische Handlungsfähigkeit stark ein&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Canossagang&lt;/strong&gt;: Heinrich IV geht zu Papst und bittet um &lt;strong&gt;Aufhebung der Exkommunizierung &lt;/strong&gt;-&amp;gt; &lt;strong&gt;erfolgreich&lt;/strong&gt;, beendet Streit aber nicht.&lt;strong&gt; &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1084&lt;/em&gt;: Erhebung des &lt;strong&gt;Gegenpapstes Klemens III &lt;/strong&gt;-&amp;gt; krönt Heinrich zu &lt;strong&gt;Kaiser&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertrag von Sutri (strikte Trennung von REich und Kirche) gescheitert&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Beendet &lt;/span&gt;&lt;em style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;1122 &lt;/em&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;mit &lt;/span&gt;&lt;strong&gt;Wormser Konkordat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Wormser Konkordat? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;1122&lt;/em&gt;: &lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Wormser Konkordat &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zwischen &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Heinrich V&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und Papst &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Calixt II&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterscheidung von &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Temporalien &lt;/strong&gt;(weltliche/materielle Güter) und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Spiritualien &lt;/strong&gt;(geistliches Amt)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Heinrich verzichtet&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;auf&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Investitur mit Ring und Stab&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;(Ehe mit Kirche + priesterliches Hirtentum) -&amp;gt; &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;keine Laieninvestitur &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;in geistliche Ämter &lt;/span&gt;mehr.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Papst&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gestand&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;zu&lt;/strong&gt;: Wahl von Bischöfen&lt;strong&gt; &lt;/strong&gt;und Äbten &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;des &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;deutschen Reiches in Gegenwart des Kaisers &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Konsequenzen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kaiser verliert &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Personalhoheit &lt;/strong&gt;über Reichskirche&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Bischöfe &lt;/strong&gt;und&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Äbte&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unabhängig &lt;/strong&gt;von Kaiser, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Territorien&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bleiben &lt;/strong&gt;in Kaisers Hand&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Reichskirche &lt;/strong&gt;wird &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;feudalisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geistliche &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Reichsfürsten &lt;/strong&gt;(in der Lehenspyramide über weltlichen) nutzen Doppelstellung als geistliche+weltliche Herrscher um &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;kirchliche Landherrschaft&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;auszubauen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Königtum &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;büßt religiöses Prestige&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(sakraler Nimbus) &lt;strong&gt;ein&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das &lt;strong&gt;Rumpfparlament &lt;/strong&gt;in Österreich 1934?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Stark verkleinertes Parlament da:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sozialdemokraten&lt;/strong&gt; aufgrund von &lt;strong&gt;Parteiverbot &lt;/strong&gt;nicht teilnehmen konnten &lt;/li&gt;&lt;li&gt;&lt;strong&gt;großdeutsche &lt;/strong&gt;(Nationaler Wirtschaftsblock) größtenteils aus Protest &lt;strong&gt;boykottierten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Genfer-Protokolle? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;1922 &lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ö Wirtschaft -&amp;gt; starke &lt;strong&gt;Inflation&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Lösungsansatz: &lt;strong&gt;Auslandskredite &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;650 Mio Goldkronen&lt;/strong&gt; vom &lt;strong&gt;Völkerbund &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verbürgt von &lt;strong&gt;England,&lt;/strong&gt; &lt;strong&gt;Italien, Tschechoslovakei, Frankreich&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Drei Genfer Protokolle: &lt;/strong&gt;enthalten Bedingungen der Anleihe&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erneute Verpflichtung von Ö zur&lt;strong&gt; Unabhängigkeit iSd Vertrag von St Germain&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anschlussverbot &lt;/strong&gt;bekräftigt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;20 Jahre&lt;/strong&gt; &lt;strong&gt;keine &lt;/strong&gt;finanzielle/wirtschaftliche Verpflichtungen die &lt;strong&gt;Unabhängigkeit konterkarieren&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Reform&lt;/em&gt;- &lt;/strong&gt;und &lt;strong&gt;&lt;em&gt;Sanierungs&lt;/em&gt;&lt;/strong&gt;&lt;em&gt;programm&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verwaltungs&lt;strong&gt;reform&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einnahmeerhöhung &lt;/strong&gt;durch diverse &lt;strong&gt;Steuern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einsparungsmaßnahmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;niedrige &lt;/strong&gt;Investitionen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;rigorose Ausgabenreduktion&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Zollunionsplan?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;ab &lt;strong&gt;1929 &lt;/strong&gt;wurde die Schaffung eines&lt;strong&gt; einheitlichen deutsch-österreichischen Zoll- und Wirtschaftsgebietes &lt;/strong&gt;gefordert.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von Deutscher Seite als Reaktion auf &lt;strong&gt;französischen Vorschlag eines europäischen Staatenbundes &lt;/strong&gt;vertreten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eine solche europ. Verbindung hätte den &lt;strong&gt;politischen und territorialen Status der europ. Staaten festgesetzt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Ende der Deutschen Revisions- und Großmachtpolitk&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Um dies zu verhindern: &lt;strong&gt;Deutschland&lt;/strong&gt; strebt &lt;strong&gt;Großmachtstellung &lt;/strong&gt;an, &lt;strong&gt;Ö als Sprungbrett&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Geheime Verhandlungen&lt;/strong&gt; werden &lt;strong&gt;publik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;französische Regierung sieht&lt;strong&gt; Zollunion als Vorstufe des Anschlusses&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stellt  Ö ein &lt;strong&gt;Ultimatum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;IGH in Den Haag entscheidet: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zollunion &lt;strong&gt;nicht gegen Anschlussverbot&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;gegen Genfer Protokolle&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Als &lt;strong&gt;1931 &lt;/strong&gt;zur &lt;strong&gt;politischen Krise &lt;/strong&gt;die &lt;strong&gt;Bankenkrise &lt;/strong&gt;kam, &lt;strong&gt;verzichtete &lt;/strong&gt;Ö auf den Plan.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist das Toleranzpatent von Joseph II? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Am 13.10.&lt;strong&gt;1781&lt;/strong&gt; von&lt;strong&gt; Joseph II&lt;/strong&gt; für Ö erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur&lt;strong&gt; eines von vielen&lt;/strong&gt;, da die &lt;strong&gt;Maßnahmen &lt;/strong&gt;auch &lt;strong&gt;Länderweise erlassen &lt;/strong&gt;werden mussten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Betraf:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;evangelische Bekenntnisse &lt;/strong&gt;(&lt;em&gt;Augsburgerisch &lt;/em&gt;und &lt;em&gt;Helvetisch&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht unierte&lt;/strong&gt;, &lt;strong&gt;orthodoxe &lt;/strong&gt;Christen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erlaubt &lt;/strong&gt;wurde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;das &lt;strong&gt;Privatexercicium &lt;/strong&gt;(nicht-öffentliche Religionsausübung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Errichtung &lt;/strong&gt;von &lt;strong&gt;Bethäusern &lt;/strong&gt;und &lt;strong&gt;Kirchen&lt;/strong&gt;, solange &lt;strong&gt;nicht nach außen als solche erkennbar&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weitere &lt;strong&gt;Ausübung &lt;/strong&gt;und &lt;strong&gt;regulative Eingriffe &lt;/strong&gt;in &lt;strong&gt;Ausgstaltung&lt;/strong&gt; der &lt;strong&gt;Religion &lt;/strong&gt;wurden unter &lt;strong&gt;staatliche Aufsicht &lt;/strong&gt;gestellt, z.B.: die &lt;strong&gt;Schulmeister&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Juden&lt;/strong&gt; waren &lt;strong&gt;nicht umfasst&lt;/strong&gt;, wurden a&lt;strong&gt;ber besser gestellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Niederlassung &lt;/strong&gt;in &lt;strong&gt;Gemeinden &lt;/strong&gt;die ihnen bisher verboten waren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zugang zu vielen &lt;strong&gt;Gewerben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Möglichkeit des &lt;strong&gt;Studiums&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Joseph &lt;/strong&gt;II verstand (gegenüber kath. Kirche) sich als &lt;strong&gt;oberster&lt;/strong&gt; &lt;strong&gt;Kirchenherr &lt;/strong&gt;des Staates&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wollte &lt;strong&gt;staatliche Verwaltung &lt;/strong&gt;und &lt;strong&gt;Kontrolle &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;= Josephinisches Staatskirchentum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gründe &lt;/strong&gt;für Toleranzpatent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur &lt;strong&gt;teilweise &lt;/strong&gt;aus &lt;strong&gt;liberaler&lt;/strong&gt; &lt;strong&gt;religiöser Haltung &lt;/strong&gt;von Joseph II&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;vielmehr&lt;/strong&gt;: &lt;strong&gt;wirtschaftliche Wachstumschancen &lt;/strong&gt;durch Anpassungen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Beseitigung &lt;/strong&gt;des &lt;strong&gt;kirchlichen Einflusses &lt;/strong&gt;auf die &lt;strong&gt;Ehe&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Auflösung &lt;/strong&gt;von &lt;strong&gt;Klöstern &lt;/strong&gt;die sich&lt;strong&gt; nicht Unterricht, Krankenpflege, Landwirtschaft oder Gewerbe &lt;/strong&gt;widmeten&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Das &lt;strong&gt;Vermögen &lt;/strong&gt;ging in &lt;strong&gt;Religionsfond&lt;/strong&gt;, der die &lt;strong&gt;Pfarren &lt;/strong&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;finanzierte &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;bis ins 20. Jahrhundert bestand&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was versteht man unter der Stagnation im Vormärz und was erhofften sich die Menschen und worin wurden sie enttäuscht? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Vormärz: &lt;strong&gt;1792 &lt;/strong&gt;bis &lt;strong&gt;1848 &lt;/strong&gt;- &lt;strong&gt;Französische Revolution &lt;/strong&gt;bis &lt;strong&gt;Märzrevolution&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Motivation der franz. Revolution: Befreiung von autoritären Herrschern, Einkehr der Grundsätze der Aufklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;In Ö gaben sich &lt;strong&gt;Joseph II und Leopold II&lt;/strong&gt; als &lt;strong&gt;aufgeklärt &lt;/strong&gt;und konnten sich mit &lt;strong&gt;Teilen &lt;/strong&gt;der &lt;strong&gt;revolutionären Ideen identifizieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Franz II&lt;/strong&gt; - &lt;strong&gt;Gegner der Revolution&lt;/strong&gt; und der &lt;strong&gt;innerstaatlichen&lt;/strong&gt; &lt;strong&gt;Öffnungstendenzen seiner Vorgänger&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Amtsantritt &lt;/strong&gt;startete &lt;strong&gt;Stagnation &lt;/strong&gt;(Ende der Zeit der Reformen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Striktes Festhalten an der &lt;strong&gt;monarchischen Legitimität &lt;/strong&gt;zur &lt;strong&gt;Unterdrückung liberaler, konstitutioneller &lt;/strong&gt;und &lt;strong&gt;nationaler Bewegungen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Österreich als &lt;strong&gt;Obrigkeits&lt;/strong&gt;-, &lt;strong&gt;Zensur&lt;/strong&gt;-, &lt;strong&gt;Überwachungsstaat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Reformzeit&lt;/strong&gt; unter Joseph II und Leopold II &lt;strong&gt;folgte&lt;/strong&gt; also der &lt;strong&gt;Vormärz &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem die &lt;strong&gt;Neuordnung&lt;/strong&gt; &lt;strong&gt;Europas &lt;/strong&gt;am &lt;strong&gt;Wiener&lt;/strong&gt; &lt;strong&gt;Kongress 1815 &lt;/strong&gt;mit &lt;strong&gt;Metternich's Stabilitätssystem (U&lt;/strong&gt;nterdrückung der&lt;strong&gt; &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Demokratie, Presse-, Meinungs- und Versammlungsfreiheit&lt;/span&gt;&lt;strong&gt;) &lt;/strong&gt;prägte die Zeit bis zur Revolution 1848 &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Worin wurden die Leute enttäuscht?&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung der autoritären&lt;/strong&gt; &lt;strong&gt;Strukturen&lt;/strong&gt; und &lt;strong&gt;Einführung eines Verfassungsstaates&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung&lt;/strong&gt; des &lt;strong&gt;Pauperismus &lt;/strong&gt;und des &lt;strong&gt;Massenelends&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung &lt;/strong&gt;der &lt;strong&gt;drangsalierenden Auflagen&lt;/strong&gt;, die durch das &lt;strong&gt;Metternichsche Stabilitätssystem &lt;/strong&gt;über ganz Europa lagen&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der &lt;span style="background-color: rgb(255, 255, 255); color: rgba(0, 0, 0, 0.87);"&gt;Pauperismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;Verelendung &lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;großer &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;Bevölkerungsteile &lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;unmittelbar &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;vor der Industrialisierung &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;zunehmender Verarmung &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;vor allem der Arbeiterschicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Jakobinerverschwörung?&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1793/1794&amp;nbsp;&lt;/strong&gt;formierten sich in Ö die &lt;strong&gt;Jakobiner&lt;/strong&gt; aus &lt;strong&gt;Schriftstellern&lt;/strong&gt;, &lt;strong&gt;Intellektuellen &lt;/strong&gt;und &lt;strong&gt;Beamten &lt;/strong&gt;die &lt;strong&gt;Joseph II &lt;/strong&gt;und &lt;strong&gt;Leopold II wohlgesonnen &lt;/strong&gt;gegenüberstanden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem &lt;strong&gt;diejenigen&lt;/strong&gt;, die an den &lt;strong&gt;Reformen &lt;/strong&gt;von &lt;strong&gt;Joseph II mitgewirkt &lt;/strong&gt;haben und von der &lt;strong&gt;Restaurationspolitik&lt;/strong&gt; &lt;strong&gt;von Franz II enttäuscht&lt;/strong&gt; waren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sie organisierten sich im &lt;strong&gt;geheimen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Standen im &lt;strong&gt;Austausch mit französischen&lt;/strong&gt; Jakobinern&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;Komplotte &lt;/strong&gt;kamen aber&lt;strong&gt; nie zur Ausführung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;österr&lt;/strong&gt;. &lt;strong&gt;Jakobiner &lt;/strong&gt;versuchten (anders als Josephinismus) die &lt;strong&gt;Revolution&lt;/strong&gt; &lt;strong&gt;von Unten &lt;/strong&gt;(mittels unterer Gesellschaftsschichten) vorzubereiten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Auch in &lt;strong&gt;Ungarn &lt;/strong&gt;gab es eine &lt;strong&gt;Bewegung &lt;/strong&gt;für &lt;strong&gt;politisch-soziale Reformen im Habsburgerreich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie für &lt;strong&gt;nationale Unabhängigkeit&lt;/strong&gt; &lt;strong&gt;Ungarns&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;von &lt;strong&gt;Machtübernahme &lt;/strong&gt;durch &lt;strong&gt;Franz II &lt;/strong&gt;enttäuscht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;→ Forderungen radikaler: vollständige Umgestaltung der Gesellschaft&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Jakobinerprozesse?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Trotz &lt;strong&gt;Bemühungen&lt;/strong&gt; &lt;strong&gt;um Geheimhaltung &lt;/strong&gt;der österr. und ungar. &lt;strong&gt;Jakobiner &lt;/strong&gt;konnten die &lt;strong&gt;Polizei Spitzel &lt;/strong&gt;einschleusen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verhaftungswelle &lt;/strong&gt;im Juli &lt;strong&gt;1794 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Führende Köpfe wie &lt;strong&gt;Martinovics &lt;/strong&gt;und &lt;strong&gt;Riedel&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Exempel statuieren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anzeige wegen &lt;strong&gt;Majestätsbeleidigung &lt;/strong&gt;oder &lt;strong&gt;Landesverrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Todesstrafe &lt;/strong&gt;für &lt;strong&gt;ungarische Bürger &lt;/strong&gt;und &lt;strong&gt;Militärpersonen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Für &lt;strong&gt;österreichische Zivilisten &lt;/strong&gt;war &lt;strong&gt;keine Todesstrafe &lt;/strong&gt;möglich&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sondergericht &lt;/strong&gt;um &lt;strong&gt;Todesstrafe &lt;/strong&gt;zu &lt;strong&gt;ermöglichen von  &lt;/strong&gt;&lt;em&gt;Jurist &lt;/em&gt;&lt;strong&gt;Karl Anton von Martini&lt;/strong&gt; &lt;strong&gt;&lt;em&gt;verhindert &lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stattdessen: schwerer Festungsarrest&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die innenpolitischen Folgen der Jakobinerprozesse?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Aufdeckung der Verschwörung&lt;/strong&gt; gemeinsam mit &lt;strong&gt;Hinrichtung Ludwig XVI und Marie Antionette &lt;/strong&gt;führte endgültig zu &lt;strong&gt;reaktionärer Linie&lt;/strong&gt; Franz II&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hetze &lt;/strong&gt;gegen alle, die &lt;strong&gt;nicht seiner Meinung &lt;/strong&gt;folgten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Intellektuelle &lt;/strong&gt;und &lt;strong&gt;Beamte&lt;/strong&gt; denen man &lt;strong&gt;Sympathie für&lt;/strong&gt; &lt;strong&gt;Aufklärung &lt;/strong&gt;nachsagte -&amp;gt; aus &lt;strong&gt;öffentlichem Leben entfernt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionäre Propaganda&lt;/strong&gt; und &lt;strong&gt;Geheimbünde verboten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Jakobinerprozesse &lt;/strong&gt;waren eine &lt;strong&gt;Bruchstelle &lt;/strong&gt;in der &lt;strong&gt;aufgeklärten&lt;/strong&gt; &lt;strong&gt;Entwicklung der Ö. Politik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Wiedereinführung &lt;/em&gt;&lt;strong&gt;Todesstrafe&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1795 &lt;/strong&gt;neue &lt;strong&gt;General-Zensurverordnung&lt;/strong&gt; um &lt;strong&gt;öffentliche Meinungsbildung &lt;/strong&gt;zu &lt;strong&gt;beeinflussen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was wurde auf dem Wiener Kongress geregelt?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;territoriale &lt;/strong&gt;und &lt;strong&gt;politische&lt;/strong&gt; &lt;strong&gt;Neuordnung Kontinentaleuropas&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;revolutionären Bestrebungen &lt;/strong&gt;+ &lt;strong&gt;napoleonischen Kriege &lt;/strong&gt;-&amp;gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;&lt;em&gt;kleinere&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Mächte&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;untergegangen, &lt;em&gt;Europa &lt;/em&gt;in &lt;em&gt;Chaos&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nach &lt;strong&gt;Niederlage Napoleons&lt;/strong&gt;: &lt;strong&gt;Aufteilung &lt;/strong&gt;der Gebiete unter Siegermächten.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zur Lösung: &lt;strong&gt;Wiener Kongress &lt;/strong&gt;unter &lt;strong&gt;Leitung&lt;/strong&gt; &lt;strong&gt;Metternichs &lt;/strong&gt;von &lt;strong&gt;November 1814 bis Juni 1815&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Neben territorialer Neuordnung &lt;strong&gt;auch&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionäre Ideen &lt;/strong&gt;(Freiheit, Gleichheit, Brüderlichkeit) &lt;strong&gt;klein &lt;/strong&gt;halten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Absolutistische Machtgefüge stabilisieren &lt;/strong&gt;/ neu aufbauen.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Auseinandersetzung mit Gedankengut &lt;/strong&gt;der Aufklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber mit &lt;strong&gt;Ziel&lt;/strong&gt; des &lt;strong&gt;Neuaufbaus &lt;/strong&gt;des &lt;strong&gt;Absolutismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;strong&gt;Verwerfen &lt;/strong&gt;der &lt;strong&gt;Ziele &lt;/strong&gt;und &lt;strong&gt;Methoden &lt;/strong&gt;der Revolution&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;strong&gt;freiwillige Übernahme &lt;/strong&gt;weniger &lt;strong&gt;Resultate &lt;/strong&gt;um erneute &lt;strong&gt;Revolution &lt;/strong&gt;zu &lt;strong&gt;verhindern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aber: &lt;strong&gt;Erstes Mal &lt;/strong&gt;"&lt;em&gt;europäischer Gedanke&lt;/em&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Lösung&lt;/strong&gt; der Probleme &lt;strong&gt;durch Gemeinschaft &lt;/strong&gt;/ &lt;strong&gt;Zusammenhelfen &lt;/strong&gt;der &lt;strong&gt;Staaten&lt;/strong&gt;/Königshäuser&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war der Rheinbund? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1806&lt;/strong&gt;: Zusammenschluss von &lt;strong&gt;16 deutschen Fürsten&lt;/strong&gt; unter dem &lt;strong&gt;Protektorat Napoleons&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit Gründung des Staatenbundes &lt;strong&gt;Austritt aus Hl. Röm Reich Deutscher Nation&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rheinbund blieb &lt;/strong&gt;faktisch ein &lt;strong&gt;militärisches Zweckbündnis &lt;/strong&gt;zwischen &lt;strong&gt;Rheinbundstaaten&lt;/strong&gt; und &lt;strong&gt;Napoleons Frankreich&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausbau in &lt;strong&gt;Bundesstaat &lt;/strong&gt;mit gemeinsamen Organen &lt;strong&gt;scheitert &lt;/strong&gt;am &lt;strong&gt;Widerstand &lt;/strong&gt;der Mitglieder&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ende &lt;strong&gt;1813 &lt;/strong&gt;nach &lt;strong&gt;Niederlage Napoleons &lt;/strong&gt;in &lt;strong&gt;Völkerschlacht&lt;/strong&gt; &lt;strong&gt;bei Leipzig&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Mediatisierung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;"&lt;strong&gt;Mittelbarmachung&lt;/strong&gt;" im Hl. Röm Reich&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verlust der selbständigen Herrschaft&lt;/strong&gt; (&lt;em&gt;Souveränität&lt;/em&gt;) der Grafen und Fürsten, v.A. kleinerer Reichsstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unterordnung &lt;/strong&gt;unter &lt;strong&gt;größere Territorien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Reichsdeputationshauptschluss?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abfindung &lt;/strong&gt;der &lt;strong&gt;weltlichen &lt;/strong&gt;Fürsten für &lt;strong&gt;linksrheinische Gebietsverluste &lt;/strong&gt;an&lt;strong&gt; Frankreich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Geschah durch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Säkularisation kirchlicher &lt;/strong&gt;Herrschaften&lt;/li&gt;&lt;li class="ql-indent-1"&gt;und &lt;strong&gt;Mediatisierung&lt;/strong&gt; &lt;strong&gt;kleinerer&lt;/strong&gt; &lt;strong&gt;weltlicher &lt;/strong&gt;Herrschaften &lt;/li&gt;&lt;li class="ql-indent-1"&gt;bisheriger Reichsstände &lt;strong&gt;rechts&lt;/strong&gt; &lt;strong&gt;des  Rheins&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1804/1806 im Detail &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1804 &lt;/strong&gt;erklärte sich &lt;strong&gt;Franz II &lt;/strong&gt;unter Eindruck der Kaiserkrönung Napoleons zum&lt;strong&gt; Kaiser von Österreich&lt;/strong&gt;, da er einen Machtverlust im Hl. Röm. Reich antizipierte.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Juli 1806&lt;/strong&gt;: &lt;strong&gt;Rheinbund &lt;/strong&gt;zwischen 16 deutsche Fürsten unter Protektorat Napoleons geschlossen.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;August 1806&lt;/strong&gt;: &lt;strong&gt;Napoleon fordert Niederlegung &lt;/strong&gt;der &lt;strong&gt;Kaiserkrone des Hl. Röm. Reichs &lt;/strong&gt;von Franz II -&amp;gt; &lt;strong&gt;Franz II kommt dem nach &lt;/strong&gt;-&amp;gt; Bleibt aber Kaiser von Ö!&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit Niederlegung des Kaiseramts:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Entbindung &lt;/strong&gt;der &lt;strong&gt;Reichsstände &lt;/strong&gt;vom &lt;strong&gt;Reich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Institutionelles&lt;/strong&gt; &lt;strong&gt;Ende &lt;/strong&gt;des &lt;strong&gt;HRRDN &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Rechtlich &lt;/strong&gt;war das Ende&lt;strong&gt; unzulässig&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-3"&gt;Erfordert &lt;strong&gt;Abdankung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-3"&gt;Erfordert &lt;strong&gt;Einbindung &lt;/strong&gt;des &lt;strong&gt;Reichstages&lt;/strong&gt;/der &lt;strong&gt;Kurfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Folge: &lt;strong&gt;de facto&lt;/strong&gt; Untergang, aber &lt;strong&gt;nicht&lt;em&gt; &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;de iure&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die Märzrevolution 1848&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Märzrevolution 1848 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Studenten&lt;/strong&gt; + &lt;strong&gt;Bürger &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Petition &lt;/strong&gt;an Kaiser für überfällige &lt;strong&gt;Reformen &lt;/strong&gt;wie &lt;strong&gt;Aufhebung der Zensur&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Demonstranten stürmen &lt;/strong&gt;nach Enttäuschung über Behandlung durch &lt;strong&gt;NÖ Landtag &lt;/strong&gt;das &lt;strong&gt;Landhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Staatsmacht &lt;/strong&gt;versucht &lt;strong&gt;Metternichs&lt;/strong&gt; &lt;strong&gt;Repressionspolitik&lt;/strong&gt; aufrechtzuerhalten -&amp;gt; &lt;strong&gt;direkter&lt;/strong&gt; &lt;strong&gt;Widerspruch &lt;/strong&gt;zu den &lt;strong&gt;Forderungen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Nachdem &lt;strong&gt;Arbeiter &lt;/strong&gt;sich dem &lt;strong&gt;Protest&lt;/strong&gt; &lt;strong&gt;angeschlossen &lt;/strong&gt;haben -&amp;gt; &lt;strong&gt;Druck &lt;/strong&gt;auf &lt;strong&gt;Kaiser &lt;/strong&gt;steigt -&amp;gt; bringt &lt;strong&gt;Metternich &lt;/strong&gt;zum &lt;strong&gt;Rücktritt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiser &lt;/strong&gt;verspricht Konstitution zu erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beteiligung &lt;/strong&gt;des &lt;strong&gt;Bürgertums &lt;/strong&gt;in Form von Beratungen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;-&amp;gt; &lt;em&gt;Pillersdorfersche Verfassung&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie wurde die aufgezwungene Märzverfassung 1849 bezeichnet?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Oktroyierte &lt;/strong&gt;Märzverfassung 1849&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Neoabsolutismus?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1851-1867&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Genauer Beginn &lt;/strong&gt;hängt ab was als &lt;strong&gt;entscheidend angesehen &lt;/strong&gt;wird:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verfassungswirklichkeit 1851&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für Patente von April und August spricht: &lt;strong&gt;offener Widerspruch &lt;/strong&gt;zur &lt;strong&gt;Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für Silvesterpatente spricht: &lt;strong&gt;Heben &lt;/strong&gt;formell von &lt;strong&gt;Verfassung 1849 auf&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Oktroyierte Märzverfassung&lt;/strong&gt; &lt;strong&gt;1849&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für diese spricht: wurde &lt;strong&gt;nie umgesetzt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das Neue: &lt;strong&gt;Scheinkonstitutionelle &lt;/strong&gt;Elemente und teilweise &lt;strong&gt;inhaltlich liberale Gesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;→ &lt;strong&gt;Absolutheit &lt;/strong&gt;der Herrschaftsmacht &lt;strong&gt;gemildert&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;br&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Merkmale:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zentralismus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Versuch &lt;strong&gt;Nationalitätskonflikt einzuschränken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;deutsche Amtssprache&lt;/strong&gt;, &lt;strong&gt;Betonung &lt;/strong&gt;der &lt;strong&gt;Länder&lt;/strong&gt; und ihrer &lt;strong&gt;Verfassungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtig &lt;strong&gt;neben &lt;/strong&gt;dem &lt;strong&gt;Kaiser&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beamtentum&lt;/strong&gt;, &lt;strong&gt;Heer&lt;/strong&gt;, &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Endgültiges Ende&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Dezemberverfassung &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;1867&lt;/em&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Silvesterpatente von 1851?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;31.12.1851&lt;/strong&gt; vom Kaiser erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;endete&lt;/strong&gt; formell die &lt;strong&gt;frühkonstitutionelle &lt;/strong&gt;Phase →&lt;strong&gt; keine&lt;/strong&gt; &lt;strong&gt;Verfassung&lt;/strong&gt; mehr → &lt;strong&gt;Absolutismus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ol&gt;&lt;li&gt;Patent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Märzverfassung &lt;/strong&gt;von 1849 &lt;strong&gt;außer Kraft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausdrücklich&lt;/strong&gt; &lt;strong&gt;bestätigt:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gleichheit &lt;/strong&gt;aller Bürger vor dem Gesetz&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Aufhebung&lt;/strong&gt; der &lt;strong&gt;Untertänigkeit&lt;/strong&gt; der &lt;strong&gt;Bauern&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Patent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aufhebung &lt;/strong&gt;des &lt;strong&gt;Grundrechtspatents &lt;/strong&gt;von &lt;strong&gt;1849&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bestätigt &lt;/strong&gt;aber &lt;strong&gt;ausdrücklich religiöse Grundrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;allerhöchstes Kabinettsschreiben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schreiben &lt;/strong&gt;von Kaiser &lt;strong&gt;an Ministerpräsident Schwarzenberg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;36 Grundsätze &lt;/strong&gt;für organisatorische Einrichtungen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Umstrukturierung &lt;/strong&gt;der &lt;strong&gt;internen Verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Machtkonzentration &lt;/strong&gt;auf den &lt;strong&gt;Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Jurisdiktion &lt;/strong&gt;und &lt;strong&gt;Grundrechtsschutz&lt;/strong&gt; &lt;strong&gt;untergraben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Mitbestimmung &lt;/strong&gt;des &lt;strong&gt;Volkes ausgeschlossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Einzug &lt;/strong&gt;von &lt;strong&gt;organisatorischen Ebenen &lt;/strong&gt;in der &lt;strong&gt;Verwaltung &lt;/strong&gt;von Stadt, Kreis, Bezirks- und Länderebene → Verringerung der Länder- und Gemeindeautonomie&lt;/li&gt;&lt;/ol&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Justizreformen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Richter&lt;/strong&gt; und &lt;strong&gt;Justizbeamte nicht &lt;/strong&gt;mehr &lt;strong&gt;unabhängig &lt;/strong&gt;→ befolgen allgemeine Vorschriften für Staatsbeamte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Verwaltung&lt;/strong&gt; und &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;in erster &lt;strong&gt;Instanz aufgehoben&lt;/strong&gt; → Bezirksämter Entscheiden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strafprozess: &lt;strong&gt;Inquisitorisches &lt;/strong&gt;Verfahren und &lt;strong&gt;keine öffentlichen&lt;/strong&gt; &lt;strong&gt;Prozesse&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber:&lt;strong&gt; Geplant &lt;/strong&gt;möglichst &lt;strong&gt;schnell einheitliches Strafrecht &lt;/strong&gt;für alle &lt;strong&gt;Kronländer &lt;/strong&gt;zu schaffen, sowie &lt;strong&gt;ABGB&lt;/strong&gt; in allen &lt;strong&gt;Kronländern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zusammengefasst:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Rückkehr zu &lt;strong&gt;absoluter Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine&lt;/strong&gt; repräsentative &lt;strong&gt;Mitbestimmung &lt;/strong&gt;des&lt;strong&gt; Volkes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Länder&lt;/strong&gt;- und &lt;strong&gt;Gemeindeautonomie&lt;/strong&gt; &lt;strong&gt;zurückgedrängt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Justizreformen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Grundrechten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie ist &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(im Neoabsolutismus)&lt;/span&gt; die Stellung des Reichsrates?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Militärische Niederlagen&lt;/strong&gt; und &lt;strong&gt;Widerstand &lt;/strong&gt;gegen &lt;strong&gt;Silvesterpatente 1851 &lt;/strong&gt;zwingen &lt;strong&gt;Kaiser&lt;/strong&gt; zum &lt;strong&gt;erneuten Eingriff &lt;/strong&gt;in &lt;strong&gt;Organisation &lt;/strong&gt;der &lt;strong&gt;Staatsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Entgegen erwarteter innenpolitischer Wende erweitert &lt;/strong&gt;er mit &lt;strong&gt;Patent &lt;/strong&gt;von &lt;strong&gt;März 1860 &lt;/strong&gt;den &lt;strong&gt;Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;außerordentliche &lt;/strong&gt;Reichsräte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle der &lt;strong&gt;Monarchie&lt;/strong&gt; &lt;strong&gt;wohlgesonnen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;= &lt;strong&gt;verstärkter Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Aufgaben:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Agenden &lt;/strong&gt;des &lt;strong&gt;Staatshaushaltes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;allgemeine &lt;strong&gt;wichtige&lt;/strong&gt; &lt;strong&gt;Gesetzesangelegenheiten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von &lt;strong&gt;Landtagen eingebrachte Vorlagen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erneute Kompetenzerweiterung &lt;/strong&gt;im &lt;strong&gt;Juli 1860 &lt;/strong&gt;erlaubt &lt;strong&gt;Sanierung &lt;/strong&gt;des schwer verschuldeten &lt;strong&gt;Staatshaushaltes gegen &lt;/strong&gt;den &lt;strong&gt;Willen der Länder&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die Stützen von Franz Joseph im Neoabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beamtentum&lt;/li&gt;&lt;li&gt;Heer&lt;/li&gt;&lt;li&gt;Kirche&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer war (im Neoabsolutismus) die Zentralfigur der öffentlichen Verwaltung?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Der &lt;strong&gt;Gendarm&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Dem &lt;strong&gt;Einfluss des Innenministers entzogen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Umfassende &lt;/strong&gt;Rechte an Gendarm &lt;strong&gt;übertragen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Rolle spielte die Kirche im Neoabsolutismus? (gedrucktes Canossa)&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konkordat&lt;/strong&gt; von &lt;strong&gt;1855 &lt;/strong&gt;um sich in Europa als &lt;strong&gt;katholische Großmacht &lt;/strong&gt;zu &lt;strong&gt;profilieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erhoffte Prestigegewinn &lt;/strong&gt;bei &lt;strong&gt;katholischen Fürsten &lt;/strong&gt;im Deutschen Bund, als &lt;strong&gt;Gegengewicht&lt;/strong&gt; zu &lt;strong&gt;Preußen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schulterschluss mit Kirche &lt;/strong&gt;soll &lt;strong&gt;legitimatorische Mängel &lt;/strong&gt;des &lt;strong&gt;Reichszentralismus verstecken &lt;/strong&gt;und über &lt;strong&gt;fehlende &lt;/strong&gt;demokratische/&lt;strong&gt;konstitutionelle Legitimation hinwegtäuschen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Katholischer Klerus ursprünglich &lt;/strong&gt;für &lt;strong&gt;nationale Bewegungen&lt;/strong&gt;, erst &lt;strong&gt;nach Konkordat &lt;/strong&gt;für &lt;strong&gt;absolutistischen Gesamtstaat&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Durch &lt;strong&gt;betonten Katholizismus &lt;/strong&gt;sollen &lt;strong&gt;nationale&lt;/strong&gt; &lt;strong&gt;Interessen negiert &lt;/strong&gt;werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Länder &lt;/strong&gt;der Monarchie &lt;strong&gt;durch neue &lt;/strong&gt;Form des &lt;strong&gt;Patriotismus verbunden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kirche &lt;/strong&gt;in der &lt;strong&gt;Ausgestaltung &lt;/strong&gt;des &lt;strong&gt;Glaubens freie Hand&lt;/strong&gt; gelassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eheangelegenheiten &lt;/strong&gt;der &lt;strong&gt;kirchlichen Gerichtsbarkeit &lt;/strong&gt;vorbehalten&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das handelspolitische Königgrätz? &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Die &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Konkurrenz &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zwischen &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Österreich&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Preußen &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;fügte Österreich &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;schwere wirtschaftliche Schäden &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zu.&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Preußen&lt;/strong&gt; zwang &lt;strong&gt;Staaten&lt;/strong&gt; des &lt;strong&gt;Deutschen Bundes &lt;/strong&gt;ab &lt;strong&gt;1862&lt;/strong&gt; in &lt;strong&gt;Zollverein &lt;/strong&gt;mit &lt;strong&gt;Frankreich &lt;/strong&gt;und &lt;strong&gt;Großbritannien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Kulturkampf in Österreich?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Befasst sich mit der &lt;strong&gt;öffentlichen Austragung&lt;/strong&gt; über die &lt;strong&gt;Kritik &lt;/strong&gt;am &lt;strong&gt;Konkordat von 1855&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kritik&lt;strong&gt; aus bürgerlich-liberalen Kreise&lt;/strong&gt;n&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verstärkt&lt;/strong&gt; durch die &lt;strong&gt;Niederlage &lt;/strong&gt;von &lt;strong&gt;1859 &lt;/strong&gt;im Sardinischen Krieg (2. Ital. Unabhängigkeitskrieg)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Machte &lt;strong&gt;Notwendigkeit staatlicher Reformen&lt;/strong&gt; klar&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;weiterer&lt;/strong&gt; &lt;strong&gt;Niederlage&lt;/strong&gt; &lt;strong&gt;1866 (&lt;em&gt;Königgrätz&lt;/em&gt;)&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;klar, dass &lt;strong&gt;reaktionäre&lt;/strong&gt; und &lt;strong&gt;klerikale Linie nicht&lt;/strong&gt; &lt;strong&gt;haltbar&lt;/strong&gt; ist&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;außenpolitischer Misserfolg &lt;/strong&gt;kann &lt;strong&gt;nicht mehr &lt;/strong&gt;hinter &lt;strong&gt;Beschützerrolle &lt;/strong&gt;für &lt;strong&gt;deutsches Katholikentum versteckt &lt;/strong&gt;werden &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung &lt;/strong&gt;versucht &lt;strong&gt;Heiligen&lt;/strong&gt; &lt;strong&gt;Stuhl &lt;/strong&gt;von einer Lösung zu &lt;strong&gt;überzeugen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Praktische&lt;/strong&gt; &lt;strong&gt;Abkehr &lt;/strong&gt;vom &lt;strong&gt;Konkordat 1867 &lt;/strong&gt;durch &lt;strong&gt;Festlegung &lt;/strong&gt;der &lt;strong&gt;Staatsbürgerrechte &lt;/strong&gt;und &lt;strong&gt;Bestimmungen&lt;/strong&gt; über die &lt;strong&gt;richterliche Gewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vorrangstellung &lt;/strong&gt;der Kirche &lt;strong&gt;de facto unmöglich &lt;/strong&gt;gemacht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Maigesetzen &lt;/strong&gt;von &lt;strong&gt;1868&lt;/strong&gt; &lt;strong&gt;endgültig beendet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie gliederte sich die Gewerbeordnung im Neoabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gewerbeordnung von &lt;strong&gt;1859&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zeigte weiten Bogen &lt;/strong&gt;zwischen &lt;strong&gt;konservativer&lt;/strong&gt; und &lt;strong&gt;liberaler&lt;/strong&gt; &lt;strong&gt;Legislative &lt;/strong&gt;auf, da sie die &lt;strong&gt;Zunftordnung aufhob.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sollte &lt;strong&gt;Betriebsamkeit &lt;/strong&gt;erleichtern.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompromiss. Zunächst &lt;/strong&gt;von &lt;strong&gt;beiden Seiten angefeindet&lt;/strong&gt;, aber &lt;strong&gt;zunehmend &lt;/strong&gt;mit &lt;strong&gt;Wohlwollen &lt;/strong&gt;begrüßt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Rechtszersplitterung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beseitigung &lt;/strong&gt;des &lt;strong&gt;Konzessionssystems&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nicht alle &lt;/strong&gt;wurden &lt;strong&gt;gewerbefrei&lt;/strong&gt;, &lt;strong&gt;aber nur &lt;/strong&gt;noch &lt;strong&gt;14 &lt;/strong&gt;im &lt;strong&gt;Gesetz&lt;/strong&gt; &lt;strong&gt;taxativ aufgezählte &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kaum &lt;/strong&gt;noch &lt;strong&gt;gesetzliche Preisbindung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Arbeitsverhältnisse &lt;/strong&gt;(Lehrlinge etc.; freie Vereinbarkeit)&lt;/li&gt;&lt;li&gt;Erste &lt;strong&gt;Ansätze &lt;/strong&gt;von &lt;strong&gt;Arbeitnehmerschutz &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Genossenschaftswesen&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Reichsrat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;In &lt;strong&gt;Märzverfassung&lt;/strong&gt; &lt;strong&gt;1849 &lt;/strong&gt;vorgesehen &lt;strong&gt;Reichstag &lt;/strong&gt;wurde &lt;strong&gt;nie umgesetzt &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeigte &lt;strong&gt;fehlenden Willen &lt;/strong&gt;des Kaisers für &lt;strong&gt;konstitutionell Staatsführung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ursprünglich &lt;/strong&gt;als &lt;strong&gt;Beratungsorgan &lt;/strong&gt;vorgesehener &lt;strong&gt;Reichsrat &lt;/strong&gt;wurde &lt;strong&gt;verfassungswidrig aufgewertet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;hatte &lt;strong&gt;kein Initiativrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Stattdessen &lt;/strong&gt;konnten &lt;strong&gt;Kaiser &lt;/strong&gt;und &lt;strong&gt;Minister &lt;/strong&gt;die Kompetenz des &lt;strong&gt;Reichsrates in Anspruch nehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;durfte zur &lt;strong&gt;Vorbereitung &lt;/strong&gt;der &lt;strong&gt;Beratung &lt;/strong&gt;um &lt;strong&gt;Mitwirkung&lt;/strong&gt; der &lt;strong&gt;Minister ersuchen&lt;/strong&gt;, diese waren aber &lt;strong&gt;nicht verpflichtet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war das Oktoberdiplom von 1860? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Verwaltungsreform &lt;/strong&gt;ohne &lt;strong&gt;tatsächlich &lt;/strong&gt;was &lt;strong&gt;zu ändern&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ziel: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarische Adelige &lt;/strong&gt;auf Seite des &lt;strong&gt;Kaisers &lt;/strong&gt;bringen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarische &lt;/strong&gt;Länder &lt;strong&gt;beruhigen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verweis auf die &lt;strong&gt;Erbfolgeordnung &lt;/strong&gt;der &lt;strong&gt;pragmatischen Sanktion&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unteilbarkeit &lt;/strong&gt;der habsburgischen Länder&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beteiligung &lt;/strong&gt;der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Völker&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;in &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Gesetzgebung &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zusammenwachsen &lt;/strong&gt;der &lt;strong&gt;Völker &lt;/strong&gt;durch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Staatsbürgerliche &lt;strong&gt;Gleichheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gleiche Wehr&lt;/strong&gt;- und &lt;strong&gt;Steuerpflicht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Religionsfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gleicher &lt;strong&gt;Ämterzugang&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Weitere Info: Eher weniger wichtig &lt;/p&gt;&lt;p&gt;Kontext:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Versuch &lt;/strong&gt;durch &lt;strong&gt;Verweis auf &lt;/strong&gt;die &lt;strong&gt;Landtage&lt;/strong&gt;, die &lt;strong&gt;ungarischen &lt;/strong&gt;Länder zu &lt;strong&gt;beruhigen&lt;/strong&gt; und die &lt;strong&gt;Einheit &lt;/strong&gt;der Monarchie zu &lt;strong&gt;festigen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;Differenzierter&lt;/strong&gt;" &lt;strong&gt;Föderalismus &lt;/strong&gt;in der Monarchie:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarische Angelegenheiten &lt;/strong&gt;mit &lt;strong&gt;Landtag &lt;/strong&gt;behandelt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht&lt;/strong&gt;-&lt;strong&gt;Ungarische &lt;/strong&gt;Länder beziehen zusätzlich &lt;strong&gt;weiterhin Reichstag&lt;/strong&gt; ein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufstockung &lt;/strong&gt;der von den &lt;strong&gt;Landtagen &lt;/strong&gt;zu entsendenden &lt;strong&gt;Reichsratsmitgliedern&lt;/strong&gt; auf &lt;strong&gt;100&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ankündigung &lt;/strong&gt;von &lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Justiz &lt;/strong&gt;und &lt;strong&gt;Verwaltung&lt;/strong&gt; und &lt;strong&gt;Stärkung &lt;/strong&gt;der &lt;strong&gt;Selbstverwaltung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ungarn &lt;/strong&gt;erhielt zurück:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Historische &lt;strong&gt;Verfassung &lt;/strong&gt;(Vor 1848)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hofkanzlei&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;oberster&lt;/strong&gt; &lt;strong&gt;Gerichtshof&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Sollte&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ungarischen Adel &lt;/strong&gt;auf &lt;strong&gt;Seite&lt;/strong&gt; des &lt;strong&gt;Kaisers &lt;/strong&gt;bringen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zentralismus durch &lt;/strong&gt;neue Form des &lt;strong&gt;Föderalismus kaschieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Änderungen&lt;/strong&gt; wurden in &lt;strong&gt;Ungarn&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;Feudaladel&lt;/strong&gt; &lt;strong&gt;begrüßt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Von der &lt;strong&gt;Mehrheit&lt;/strong&gt; der &lt;strong&gt;Bevölkerung&lt;/strong&gt; &lt;strong&gt;abgelehnt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Für die &lt;strong&gt;westlichen Länder&lt;/strong&gt; ergab es &lt;strong&gt;keine richtigen Änderungen&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was war der Februarpatent von 1861? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ausführungsgesetz &lt;/strong&gt;zum &lt;strong&gt;Oktoberdiplom&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Änderte das Oktoberdiplom &lt;strong&gt;inhaltlich weitgehend&lt;/strong&gt; &lt;strong&gt;ab&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kombination&lt;/strong&gt; der Beilagen (&lt;strong&gt;Grundgesetze&lt;/strong&gt; + &lt;strong&gt;Wahlordnungen&lt;/strong&gt;) wurde als &lt;strong&gt;Verfassung&lt;/strong&gt; &lt;strong&gt;verkündet&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste Verfassung &lt;/strong&gt;seit &lt;strong&gt;1849&lt;/strong&gt;, aber nur auf &lt;strong&gt;Gesetzgebung bezogen &lt;/strong&gt;(keine anderen konstitutionellen Elemente)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zuständigkeit&lt;/strong&gt; der &lt;strong&gt;Landesgesetzgebung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landesfinanzen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;Landwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Öffentliches &lt;strong&gt;Bauwesen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Weitere Aufgaben &lt;/strong&gt;konnten den Ländern zugewiesen werden, &lt;strong&gt;wenn&lt;/strong&gt; &lt;strong&gt;Landesinteressen berührt &lt;/strong&gt;wurden&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Landtage &lt;/strong&gt;wurden aus &lt;strong&gt;4 Kurien&lt;/strong&gt; gewählt (Großgrundbesitz, Handel+Gewerbe, Städte+Märkte, Landgemeinden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;hoher Steuerzensus &lt;/strong&gt;-&amp;gt; nur wohlhabende Schichten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgeordnete &lt;strong&gt;deutscher&lt;/strong&gt; &lt;strong&gt;Nationalität&lt;/strong&gt; wurden &lt;strong&gt;gefördert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reichsvertretung&lt;/strong&gt;: &lt;strong&gt;Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Besteht aus: &lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Herrenhaus&lt;/strong&gt;: Adel + Kleriker, vom &lt;strong&gt;Kaiser &lt;/strong&gt;ernannt&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Abgeordnetenhaus&lt;/strong&gt;: Aus &lt;strong&gt;Landtagen &lt;/strong&gt;entsandt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vom &lt;strong&gt;Kaiser&lt;/strong&gt; &lt;strong&gt;einberufen &lt;/strong&gt;1x &lt;strong&gt;Jährlich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompetenzbereich &lt;/strong&gt;des Reichsrates &lt;strong&gt;bestätigt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beratende &lt;/strong&gt;Funktion zu &lt;strong&gt;beschließender Funktion &lt;/strong&gt;gewandelt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abhängig von &lt;strong&gt;Sanktion &lt;/strong&gt;des &lt;strong&gt;Kaisers &lt;/strong&gt;(Veto)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Weitere&lt;/strong&gt; &lt;strong&gt;Reichsvertretung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;engerer&lt;/strong&gt; &lt;strong&gt;Reichstag &lt;/strong&gt;für Angelegenheiten in &lt;strong&gt;nicht ungarische &lt;/strong&gt;Länder&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des &lt;strong&gt;Kaisers &lt;/strong&gt;(Gesetze ohne Reichstag)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Alleinige Entscheidungsmacht &lt;/strong&gt;des &lt;strong&gt;Kaises &lt;/strong&gt;in Agenden wie &lt;strong&gt;Äußeres&lt;/strong&gt;, &lt;strong&gt;Kriegswesen&lt;/strong&gt;, &lt;strong&gt;Religion&lt;/strong&gt;, &lt;strong&gt;Strafrecht &lt;/strong&gt;(&lt;em&gt;Prärogativen der Krone)&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie war die Rolle der Grundrechte im Neoabsolutismus? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundrechte&lt;/strong&gt;/Grundfreiheiten &lt;strong&gt;von Bürgern &lt;/strong&gt;immer wieder &lt;strong&gt;durch Kaiser&lt;/strong&gt; &lt;strong&gt;betont&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber &lt;strong&gt;kein Katalog &lt;/strong&gt;aufgezählter Rechte, sondern &lt;strong&gt;eher Staatsziele &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Inhaltlich&lt;/strong&gt; entweder gar &lt;strong&gt;nicht garantiert&lt;/strong&gt;, &lt;strong&gt;oder &lt;/strong&gt;mittels &lt;strong&gt;einfacher&lt;/strong&gt; &lt;strong&gt;Gesetze&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Obstruktionspolitik?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trotz&lt;/strong&gt; &lt;strong&gt;Betonung&lt;/strong&gt; der &lt;strong&gt;Landtage &lt;/strong&gt;und &lt;strong&gt;Zugeständnisse &lt;/strong&gt;des &lt;strong&gt;Monarchen&lt;/strong&gt;, &lt;strong&gt;verweigerten&lt;/strong&gt; die &lt;strong&gt;Ungarn &lt;/strong&gt;die &lt;strong&gt;Beschickung &lt;/strong&gt;des &lt;strong&gt;Reichsrates&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarischer Landtag &lt;/strong&gt;(auf &lt;strong&gt;Basis &lt;/strong&gt;von &lt;strong&gt;Februarpatent&lt;/strong&gt; 1861 &lt;strong&gt;gewählt&lt;/strong&gt;) &lt;strong&gt;lehnt Zentralparlament ab &lt;/strong&gt;-&amp;gt; fordert &lt;strong&gt;Rückkehr &lt;/strong&gt;zur &lt;strong&gt;revolutionären Verfassung&lt;/strong&gt; von &lt;strong&gt;1848&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kroatien &lt;/strong&gt;und &lt;strong&gt;Siebenbürgerische Rumänen erhoffen &lt;/strong&gt;sich durch &lt;strong&gt;Annäherung&lt;/strong&gt; an &lt;strong&gt;Ungarn&lt;/strong&gt; &lt;strong&gt;Vorteile&lt;/strong&gt;, und &lt;strong&gt;tragen Obstruktionspolitik&lt;/strong&gt; &lt;strong&gt;mit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Auf Dauer schrumpfte Reichsrat&lt;/strong&gt; (mangels Entsendung) auf &lt;strong&gt;Versammlung &lt;/strong&gt;von Politikern der &lt;strong&gt;deutschen Verfassungspartei&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Monarch&lt;/strong&gt; &lt;strong&gt;bevorzugt &lt;/strong&gt;dann &lt;strong&gt;staatliche&lt;/strong&gt; &lt;strong&gt;Neugestaltung&lt;/strong&gt;, &lt;strong&gt;statt Zentralismus &lt;/strong&gt;oder &lt;strong&gt;Föderalismus&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Dualismus &lt;/strong&gt;mit Ungarn&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1865 Erklärung an &lt;/strong&gt;seine &lt;strong&gt;Völker&lt;/strong&gt;: &lt;strong&gt;Enttäuschung &lt;/strong&gt;über &lt;strong&gt;Verweigerung &lt;/strong&gt;der Entsendung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Deshalb&lt;/strong&gt;: &lt;strong&gt;Überarbeitung &lt;/strong&gt;von &lt;strong&gt;Februarpatent notwendig &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sowie &lt;strong&gt;Verhandlungen &lt;/strong&gt;mit &lt;strong&gt;Landtagen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundgesetz &lt;/strong&gt;über die &lt;strong&gt;Reichsvertretung &lt;/strong&gt;wurde daher in allen &lt;strong&gt;Ländern sistiert &lt;/strong&gt;(&lt;strong&gt;stillgelegt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weil: &lt;strong&gt;Kann nicht gelten&lt;/strong&gt;, &lt;strong&gt;während &lt;/strong&gt;es in einem anderen Land &lt;strong&gt;verhandelt wird&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einigung &lt;/strong&gt;mit den &lt;strong&gt;Landtagen&lt;/strong&gt; &lt;strong&gt;verzögerte &lt;/strong&gt;sich aufgrund &lt;strong&gt;militärischer Niederlage &lt;/strong&gt;gegen &lt;strong&gt;Preußen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Faktisch &lt;/strong&gt;kehrte &lt;strong&gt;Franz Joseph &lt;/strong&gt;damit zu &lt;strong&gt;absolutistischer &lt;/strong&gt;Herrschaft zurück&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der aufgeklärte Absolutismus?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verbindung&lt;/strong&gt; von &lt;strong&gt;Absolutismus &lt;/strong&gt;und &lt;strong&gt;Aufklärung &lt;/strong&gt;im &lt;strong&gt;18. Jahrhundert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herrscher &lt;/strong&gt;handeln &lt;strong&gt;nach Grundsätzen&lt;/strong&gt; der &lt;strong&gt;Vernunft &lt;/strong&gt;und zum &lt;strong&gt;Wohl &lt;/strong&gt;der &lt;strong&gt;Untertanen&lt;/strong&gt; und des &lt;strong&gt;Landes&lt;/strong&gt;, &lt;strong&gt;nicht &lt;/strong&gt;nach &lt;strong&gt;eigenem Willen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reformen&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;soziale Missstände &lt;/strong&gt;beseitigen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Wissenschaft&lt;/strong&gt;, &lt;strong&gt;Kultur&lt;/strong&gt;, &lt;strong&gt;Bildung&lt;/strong&gt;, &lt;strong&gt;Handel &lt;/strong&gt;und &lt;strong&gt;Gewerbe&lt;/strong&gt; &lt;strong&gt;fördern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erster Diener des Staates&lt;/strong&gt; - Kontrast zum Gottesgnadendum &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;In Ö&lt;/strong&gt; vor allem gezeigt durch &lt;strong&gt;Toleranzpolitik Joseph &lt;/strong&gt;II.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Obwohl &lt;strong&gt;Liberalisierung&lt;/strong&gt; der &lt;strong&gt;Religionspolitik weniger &lt;/strong&gt;aus &lt;strong&gt;idealistischen Gründen&lt;/strong&gt;, &lt;strong&gt;eher&lt;/strong&gt; zur &lt;strong&gt;Steigerung &lt;/strong&gt;der &lt;strong&gt;Wirtschaftskraft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann bestand die konstitutionelle Doppelmonarchie? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Auch &lt;strong&gt;Konstitutionalismus &lt;/strong&gt;genannt&lt;/li&gt;&lt;li&gt;Von&lt;strong&gt; Ö-U Ausgleich 1867&lt;/strong&gt; bis Zusammenbruch nach 1. WK &lt;strong&gt;1918&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die pragmatische Sanktion? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Von &lt;strong&gt;Kaiser Karl VI&lt;/strong&gt; &lt;strong&gt;1713 &lt;/strong&gt;veröffentlichte Urkunde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unteilbarkeit &lt;/strong&gt;und &lt;strong&gt;Untrennbarkeit &lt;/strong&gt;der habsburgerischen &lt;strong&gt;Erbländer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;gemeinsamer &lt;strong&gt;Landesfürst &lt;/strong&gt;als &lt;strong&gt;Monarch &lt;/strong&gt;der &lt;strong&gt;Union&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erbfolge: Primogenitur &lt;/strong&gt;im &lt;strong&gt;Mannesstamm&lt;/strong&gt;, falls keine männlichen Nachfolger &lt;strong&gt;subsidiär Erbrecht &lt;/strong&gt;der &lt;strong&gt;Töchter&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;ab &lt;strong&gt;1720 &lt;/strong&gt;Karl VI &lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;Hoffnung &lt;/strong&gt;auf &lt;strong&gt;männl&lt;/strong&gt;. &lt;strong&gt;Nachkommen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bemühte &lt;/strong&gt;sich um &lt;strong&gt;innen&lt;/strong&gt;+&lt;strong&gt;außenpolitische&lt;/strong&gt; &lt;strong&gt;Anerkennung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;zugunsten&lt;/strong&gt; Tochter: &lt;strong&gt;Maria Theresia&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;außenpolitische &lt;strong&gt;Vorgeschichte&lt;/strong&gt;: der &lt;strong&gt;Spanische Erbfolgekrieg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Spanische &lt;strong&gt;männliche Linie &lt;/strong&gt;ausgestorben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Konfliktierende Ansprüche&lt;/strong&gt;: &lt;strong&gt;testamentarischer Nachfolger &lt;/strong&gt;&lt;em&gt;Bourbone&lt;/em&gt;, sowie &lt;em&gt;Habsburger&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wodurch wurde der Konstitutionalismus geprägt? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Parlamentarismus &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Massenparteien &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kampf&lt;/strong&gt; um ein &lt;strong&gt;allgemeines&lt;/strong&gt; &lt;strong&gt;Wahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nationale Forderungen &lt;/strong&gt;(größte &lt;strong&gt;Belastung &lt;/strong&gt;der &lt;strong&gt;Innenpolitik&lt;/strong&gt;)&lt;/li&gt;&lt;/ol&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie hängen die Maigesetze von 1868 und das Konkordat von 1855 zusammen? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Maigesetze &lt;/strong&gt;von &lt;strong&gt;1868 &lt;/strong&gt;sowie damit &lt;strong&gt;verbundene&lt;/strong&gt; &lt;strong&gt;Änderungen&lt;/strong&gt; des &lt;strong&gt;ABGB beendeten &lt;/strong&gt;das &lt;strong&gt;Konkordat &lt;/strong&gt;von &lt;strong&gt;1855&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eherecht &lt;/strong&gt;für Katholiken &lt;strong&gt;wiederhergestellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehesachen&lt;/strong&gt; wieder &lt;strong&gt;weltlicher&lt;/strong&gt; &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;zugeordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notzivilehe&lt;/strong&gt;, wenn&lt;strong&gt; &lt;/strong&gt;Kirche &lt;strong&gt;Trauung verweigert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reaktion &lt;/strong&gt;der &lt;strong&gt;Bevölkerung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bürgerlich&lt;/strong&gt;-&lt;strong&gt;liberal&lt;/strong&gt;: &lt;strong&gt;Zustimmung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ländliche &lt;/strong&gt;Regionen: &lt;strong&gt;Kritik&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1874 weitere Maigesetze: Verhältnis &lt;/strong&gt;von &lt;strong&gt;Staat &lt;/strong&gt;und &lt;strong&gt;Kirche &lt;/strong&gt;weiter &lt;strong&gt;zugunsten&lt;/strong&gt; l&lt;strong&gt;iberaler Öffnung konkretisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Katholikengesetz &lt;/strong&gt;zur Regelung der &lt;strong&gt;äußeren Rechtsverhältnisse &lt;/strong&gt;der &lt;strong&gt;Kirche &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Religionsfonds&lt;/strong&gt;gesetz &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anerkennungs&lt;/strong&gt;gesetz &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der eiserne Ring?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Regierung &lt;/strong&gt;unter Eduard Graf von &lt;strong&gt;Taaffe &lt;/strong&gt;bildete &lt;strong&gt;gestützt &lt;/strong&gt;auf &lt;strong&gt;feudale&lt;/strong&gt; &lt;strong&gt;Kreise&lt;/strong&gt; den&lt;strong&gt; Eisernen Ring, &lt;/strong&gt;ab &lt;strong style="background-color: rgb(230, 238, 248); color: rgb(51, 51, 51);"&gt;1879&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Suchte &lt;strong&gt;Annäherung &lt;/strong&gt;an die &lt;strong&gt;katholisch&lt;/strong&gt;-&lt;strong&gt;konservativen Rechten&lt;/strong&gt; im &lt;strong&gt;Parlament&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neue &lt;strong&gt;Gesprächsbasis &lt;/strong&gt;mit &lt;strong&gt;österr&lt;/strong&gt;. &lt;strong&gt;Bischöfen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer war Teil der Mittelmächte?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;K+K&lt;/li&gt;&lt;li&gt;Deutsches Kaiserreich&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wer waren die Entente-Mächte?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Frankreich&lt;/li&gt;&lt;li&gt;Russland&lt;/li&gt;&lt;li&gt;Großbritannien&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der Panslawismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Streben &lt;/strong&gt;nach &lt;strong&gt;kulturellem&lt;/strong&gt; und &lt;strong&gt;politischem Zusammenschluss &lt;/strong&gt;aller &lt;strong&gt;slawischen&lt;/strong&gt; &lt;strong&gt;Völker&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zerschlagung &lt;/strong&gt;von &lt;strong&gt;Österreich-Ungarn&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind frühkonstitutionelle Elemente der Dezemberverfassung 1867?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Macht &lt;/strong&gt;beim &lt;strong&gt;Kaiser &lt;/strong&gt;konzentriert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;oberster Träger &lt;/strong&gt;von &lt;strong&gt;Regierungs &lt;/strong&gt;+ &lt;strong&gt;Vollzugsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;absolutes &lt;/strong&gt;Veto&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Herrenhaus &lt;/strong&gt;von &lt;strong&gt;Kaiser ernannt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abgeordnetenhaus Ausschusslandtag &lt;/strong&gt;-&amp;gt; &lt;strong&gt;keine Volksvertretung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Monarchie auf Widerruf?&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Budget &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Wirtschaftspolitik&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;in &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;K. u. K Monarchie &lt;/strong&gt;benötigte &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;ständige&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Verhandlungen&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;zwischen&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Ö und U&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;und war vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Versuch &lt;/strong&gt;der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Aufrechterhaltung &lt;/strong&gt;einer &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;gemeinsamen&lt;/strong&gt; &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Wirtschaft &lt;/strong&gt;geprägt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Diese &lt;strong&gt;Verhandlungen &lt;/strong&gt;in &lt;strong&gt;Konferenzen &lt;/strong&gt;und &lt;strong&gt;Deputationen &lt;/strong&gt;waren oft Austragungsort von &lt;strong&gt;Machtdemonstrationen &lt;/strong&gt;und &lt;strong&gt;Einsatz von Druckmitteln &lt;/strong&gt;zur &lt;strong&gt;Lösung&lt;/strong&gt; &lt;strong&gt;diverser Konflikte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aufgrund des &lt;strong&gt;immanenten Konfliktpotentials &lt;/strong&gt;entstand die Bezeichnung "&lt;strong&gt;Monarchie&lt;/strong&gt; auf &lt;strong&gt;Widerruf&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die utraquistischen Schulen&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestimmte Unterrichtsgegenständen mussten in einer, und andere Gegenstände in der anderen Sprache unterrichtet werden&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist der Trialismus?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Schlagwort &lt;/strong&gt;in der &lt;strong&gt;Nationalitätenfrage &lt;/strong&gt;in der &lt;strong&gt;Doppelmonarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beide&lt;/strong&gt; &lt;strong&gt;Seiten &lt;/strong&gt;wollten jeweils eine &lt;strong&gt;andere Gruppe &lt;/strong&gt;als &lt;strong&gt;dritte Kraft im Staat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-indent-1"&gt;&lt;strong&gt;Im Kern&lt;/strong&gt;: &lt;strong&gt;Erweiterung &lt;/strong&gt;der Doppelmonarchie um einen &lt;strong&gt;dritten Reichsteil&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Nennen Sie markante Entwicklungsschritte für den Reichsrat und die Reichsratswahlen.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1867&lt;/strong&gt;: Änderung des GG über die Reichsvertretung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1873&lt;/strong&gt;: Wahlrechtsreform und die Beendigung der Beschickung durch die Landtage&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1882&lt;/strong&gt;: Taaffesche Wahlrechtsreform und die Senkung des Zensus&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1896&lt;/strong&gt;: Badenische Wahlrechtsreform und die Erweiterung um eine 5. Kurie&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1907&lt;/strong&gt;: Beck’sche Wahlrechtsreform und das allgemeine Männerwahlrecht&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche Verfassung wird durch die Dezemberverfassung von 1867 außer Kraft gesetzt? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Verfassung &lt;/strong&gt;von &lt;strong&gt;1861&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;ausdrückliche&lt;/strong&gt;, sondern nur &lt;strong&gt;materielle&lt;/strong&gt; &lt;strong&gt;Derogation&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;alte &lt;/strong&gt;Vorschriften &lt;strong&gt;nicht explizit&lt;/strong&gt; &lt;strong&gt;gestrichen &lt;/strong&gt;werden, sondern werden &lt;strong&gt;durch &lt;/strong&gt;die &lt;strong&gt;neuen unanwendbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welchen Geltungsbereich hatte die Verfassung von 1861 und welche die von 1867?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;1861: Gesamtstaat&lt;/li&gt;&lt;li&gt;1867: Cisleithanien&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Aus welchen Gesetzen besteht die Dezemberverfassung von 1867?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gesetz über die Ministerverantwortlichkeit&lt;/li&gt;&lt;li&gt;Grundgesetz über die Reichsvertretung&lt;/li&gt;&lt;li&gt;StGG über die Staatsbürgerrechte&lt;/li&gt;&lt;li&gt;StGG über das Reichsgericht&lt;/li&gt;&lt;li&gt;StGG über die richterliche Gewalt&lt;/li&gt;&lt;li&gt;StGG über Regierungs- und Vollzugsgewalt&lt;/li&gt;&lt;li&gt;Delegationsgesetz&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wurde die Sozialdemokratische Partei Österreichs gegründet?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;SD Arbeitervereine &lt;/strong&gt;und &lt;strong&gt;Bewegungen &lt;/strong&gt;waren &lt;strong&gt;staatlichen Repressionen &lt;/strong&gt;ausgesetzt und führten &lt;strong&gt;interne Kämpfe &lt;/strong&gt;über &lt;strong&gt;Ausrichtung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Konflikte&lt;/strong&gt; im &lt;strong&gt;Einigungskongress 1847 nicht ausgeräumt&lt;/strong&gt;, &lt;strong&gt;aber&lt;/strong&gt;: &lt;strong&gt;Gründung&lt;/strong&gt; der &lt;strong&gt;sozialdemokratischen Arbeiterpartei&lt;/strong&gt; &lt;strong&gt;Ö&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1880er &lt;/strong&gt;vermehrt &lt;strong&gt;Spannungen &lt;/strong&gt;und &lt;strong&gt;Konflikte &lt;/strong&gt;über &lt;strong&gt;Ausrichtung &lt;/strong&gt;zwischen &lt;strong&gt;gemäßigten &lt;/strong&gt;und &lt;strong&gt;radikalen Kräften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1888/89 &lt;/strong&gt;Einigung am &lt;strong&gt;Hainfelder Parteitag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"eigentliche &lt;strong&gt;Geburtsstunde&lt;/strong&gt;" der Partei&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Kriegsabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;von &lt;strong&gt;Grundrechten&lt;/strong&gt; &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zensur&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unterstellung von &lt;strong&gt;Zivilpersonen &lt;/strong&gt;und &lt;strong&gt;Behörden &lt;/strong&gt;unter &lt;strong&gt;Armeekommando &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aussetzung &lt;/strong&gt;der &lt;strong&gt;1917 &lt;/strong&gt;anstehenden &lt;strong&gt;Neuwahlen&lt;/strong&gt;&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist das Notverordnungsrecht und was das Kriegswirtschaftliche Ermächtigungsgesetz von 1917?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Kaiserliche Verordnung 1914&lt;/em&gt; gab &lt;em&gt;Regierung&lt;/em&gt; &lt;em&gt;Notverordnungsrecht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Wirtschaftsleben &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;fördern, &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Versorgung &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;sichern, &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Schäden&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;abwenden &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;können&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Führte zu &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Kriegsabsolutismus &lt;/strong&gt;&lt;em style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;1914-1917&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Reichstag &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;bis 1917 &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;vertagt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Wiedereinberufung &lt;/strong&gt;des &lt;strong&gt;Reichsrates 1917&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bestätigung &lt;/strong&gt;des &lt;strong&gt;Notverordnungsrechts &lt;/strong&gt;mittels &lt;strong&gt;Gesetzesbeschluss &lt;/strong&gt;als &lt;strong&gt;KWEG&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiserliche Notverordnung &lt;/strong&gt;von 1914 &lt;strong&gt;außer Kraft&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Begleitet von &lt;strong&gt;heftiger&lt;/strong&gt; &lt;strong&gt;Kritik &lt;/strong&gt;wegen vorhergehender &lt;strong&gt;Aussetzung &lt;/strong&gt;des &lt;strong&gt;Reichsrates &lt;/strong&gt;und &lt;strong&gt;exzessiver Notrecht &lt;/strong&gt;Nutzung.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aber: &lt;strong&gt;Genehmigung einzelner Regierungsverordnungen &lt;/strong&gt;wäre &lt;strong&gt;nicht zeitlich &lt;/strong&gt;und &lt;strong&gt;rechtssicher Umsetzbar &lt;/strong&gt;gewesen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Daher trotz erkennbarer Ablehnung &lt;em&gt;zur Zustimmung genötigt&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was versuchte Karl I 1918? &lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wann?&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;17. Oktober 1918&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Manifest "&lt;em&gt;An meine getreuen österreichischen Völker&lt;/em&gt;"&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Umbau &lt;/strong&gt;der K u K &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bundesstaat&lt;/strong&gt; unter Berücksichtigung &lt;strong&gt;nationaler Siedlungsgebiete&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;mit &lt;em&gt;autonomer Selbstbestimmung &lt;/em&gt;(&lt;strong&gt;Föderalismus&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;2-Faches Problem:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zu spät: &lt;em&gt;Monarchie &lt;/em&gt;in &lt;em&gt;Auflösung &lt;/em&gt;begriffen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Völker &lt;/strong&gt;versuchten bereits &lt;strong&gt;staatliche Selbstbestimmung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhaltlich nicht &lt;em&gt;tiefgreifend genug&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarn nicht &lt;/strong&gt;einbezogen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarn&lt;/strong&gt; sah in Bildung von &lt;strong&gt;Bundesstaaten &lt;/strong&gt;einen &lt;strong&gt;Bruch &lt;/strong&gt;des Ö-U &lt;strong&gt;Ausgleichs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Von wann bis wann bestand die Republik Deutschösterreich?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1918-1920&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Warum gründete sich Deutschösterreich? &lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ende &lt;/strong&gt;des 1. &lt;strong&gt;WK &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Ende&lt;/strong&gt; der &lt;strong&gt;Doppelmonarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vorrevolutionäre &lt;/strong&gt;Situation durch &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zerfall &lt;/strong&gt;der &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Auflösung&lt;/strong&gt; der K u. K &lt;strong&gt;Armee&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unzufriedenheit &lt;/strong&gt;der Massen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;schwierige&lt;strong&gt; Versorgungslage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Lösung: &lt;strong&gt;Kompromiss, &lt;/strong&gt;Einigung auf&lt;strong&gt;:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;republikanische &lt;/strong&gt;Staatsform&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Demokratisierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abschaffung &lt;/strong&gt;des &lt;strong&gt;Adels&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Fortschrittliche Arbeits&lt;/strong&gt;- und &lt;strong&gt;Sozialgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Handelt es sich bei der Gründung Deutschösterreichs um eine Revolution?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trotz &lt;/strong&gt;unüblichem &lt;strong&gt;unblutigem Verlauf&lt;/strong&gt;, kann von einer &lt;strong&gt;bürgerlichen demokratischen Revolution &lt;/strong&gt;gesprochen werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Masse &lt;/strong&gt;der Bevölkerung &lt;strong&gt;getragen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bediente sich &lt;strong&gt;proletarischer Mittel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Vor allem in Hinblick auf &lt;strong&gt;Beseitigung privilegierter&lt;/strong&gt; &lt;strong&gt;Zugänge &lt;/strong&gt;und &lt;strong&gt;Machtpositionen &lt;/strong&gt;eindeutig &lt;strong&gt;Revolutionscharakter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;rechtlich&lt;/strong&gt;: &lt;strong&gt;Diskontinuität &lt;/strong&gt;der Verfassung&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was unterscheidet frühkonstitutionelle Element von (hoch)konstitutionellen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Frühkonstitutionell: Position des Monarchen stärker durchgesetzt&lt;/li&gt;&lt;li&gt;Konstitutionell: Position des Volkes stärker durchgesetzt &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie und durch wen wurde Deutschösterreich gegründet?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Oktober 1918&lt;/strong&gt;: &lt;strong&gt;Gründung&lt;/strong&gt; der provisorischen Nationalversammlung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Oktoberverfassung 1918&lt;/strong&gt;: &lt;strong&gt;provisorische Nationalversammlung &lt;/strong&gt;gibt sich selbst &lt;strong&gt;oberste Staatsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionärer &lt;/strong&gt;Akt&lt;strong&gt;: keine&lt;/strong&gt; &lt;strong&gt;rechtliche Legitimierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;3 großen Parteien&lt;/strong&gt; (&lt;em&gt;Christlichsozial&lt;/em&gt;, &lt;em&gt;Sozialdemokratisch&lt;/em&gt;, &lt;em&gt;Deutsch-National&lt;/em&gt;) stellten je einen &lt;strong&gt;Präsidenten &lt;/strong&gt;der &lt;strong&gt;provisorischen Nationalversammlung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Versammlung bestand aus den &lt;strong&gt;1911 gewählten Mitgliedern &lt;/strong&gt;des &lt;strong&gt;Abgeordnetenhauses &lt;/strong&gt;aus &lt;strong&gt;deutschsprachigen &lt;/strong&gt;Gebieten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wichtigste &lt;strong&gt;Aufgabe&lt;/strong&gt;: &lt;strong&gt;Verfassung &lt;/strong&gt;erarbeiten, und &lt;strong&gt;Wahl &lt;/strong&gt;einer &lt;strong&gt;konstituierenden Nationalversammlung vorbereiten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kaiser Karl verzichtet&lt;/strong&gt; in Erklärung am &lt;strong&gt;11. November 1918 &lt;/strong&gt;auf &lt;strong&gt;Anteil&lt;/strong&gt; an &lt;strong&gt;Staatsgeschäften &lt;/strong&gt;und &lt;strong&gt;erkannte Entscheidung Deutschösterreichs&lt;/strong&gt; über seine &lt;strong&gt;Staatsform&lt;/strong&gt; &lt;strong&gt;an&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesetz&lt;/strong&gt; vom &lt;strong&gt;12. November über die Staats- und Regierungsform von Deutschösterreich&lt;/strong&gt; erschuf den neuen &lt;strong&gt;Staat &lt;/strong&gt;als &lt;strong&gt;demokratische Republik&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Konzentrationsregierung &lt;/strong&gt;der&lt;strong&gt; 3 großen Lager&lt;/strong&gt; wurde&lt;strong&gt; &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;nach&lt;/strong&gt;&lt;strong&gt; den &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;ersten Monaten&lt;/strong&gt; der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;konstituierenden &lt;/strong&gt;&lt;strong&gt;NV &lt;/strong&gt;von &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Koalition &lt;/strong&gt;zwischen &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Sozialdemokraten&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Christlichsozialen&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;abgelöst&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Koalition &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;zerbrach&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;an &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Polarisierung &lt;/strong&gt;durch &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;interne Umwälzungen &lt;/strong&gt;der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Christlichsozialen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Mit welchem Gesetz wurde Frauen das Wahlrecht eingeräumt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Gesetz vom &lt;strong&gt;18.12.1918&lt;/strong&gt; über die&lt;strong&gt; Wahlordnung für die konstituierende Nationalversammlung&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was bedeutet materielle Kontinuität bei formeller Diskontinuität?&amp;nbsp;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Republik &lt;strong&gt;Deutschösterreich &lt;/strong&gt;führte &lt;strong&gt;neue Ordnung&lt;/strong&gt; auf &lt;strong&gt;Verfassungsebene &lt;/strong&gt;ein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Übernahm &lt;/strong&gt;aber die &lt;strong&gt;Rechtsordnung darunter &lt;/strong&gt;von &lt;strong&gt;Österreich/Cisleithanien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht wurde &lt;strong&gt;von &lt;/strong&gt;der &lt;strong&gt;neuen DÖ Autorität verbindlich &lt;/strong&gt;gemacht, blieb aber &lt;strong&gt;inhaltlich &lt;/strong&gt;weitgehend &lt;strong&gt;unverändert&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Im &lt;strong&gt;Vertrag von St. Germain&lt;/strong&gt; musste Deutschösterreich die &lt;strong&gt;Kontinuität anerkennen&lt;/strong&gt;.&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist dismembratio?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Zerfall eines Staats in mehrere Staaten&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was regelte die Dezember-Novelle von 1918?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Das &lt;strong&gt;Verhältnis zwischen den drei Präsidenten&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie &lt;strong&gt;zwischen&lt;/strong&gt; &lt;strong&gt;Staatsrat &lt;/strong&gt;und &lt;strong&gt;Provisorischer Nationalversammlung&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Staatsrat &lt;/strong&gt;erhielt ein &lt;strong&gt;suspensives &lt;/strong&gt;Veto bezüglich der &lt;strong&gt;Gesetzesbeschlüsse &lt;/strong&gt;der &lt;strong&gt;provisorischen NV&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber: &lt;strong&gt;Beharrungsbeschluss&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was umfasst die Märzverfassung von 1919?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;März 1919 &lt;/strong&gt;von der &lt;strong&gt;konstituierenden&lt;/strong&gt; &lt;strong&gt;Nationalversammlung erlassen&lt;/strong&gt;, bestehend aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz über die &lt;strong&gt;Volksvertretung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz über die &lt;strong&gt;Staatsregierung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Noch einmal ausdrücklich: &lt;strong&gt;Deutschösterreich &lt;/strong&gt;als &lt;strong&gt;demokratische Republik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch: &lt;strong&gt;Bestandteil &lt;/strong&gt;des &lt;strong&gt;Deutschen Reichs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Willensbildung &lt;/strong&gt;im &lt;strong&gt;Parlament&lt;/strong&gt; -&amp;gt; &lt;strong&gt;parlamentarische&lt;/strong&gt; &lt;strong&gt;Republik&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzgebungshoheit &lt;/strong&gt;der &lt;strong&gt;Länder &lt;/strong&gt;anerkannt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Staatsregierung &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;unter &lt;/em&gt;&lt;strong&gt;&lt;em&gt;politischer Verantwortlichkeit &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;der &lt;/em&gt;&lt;strong&gt;&lt;em&gt;NV &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;(&lt;/em&gt;&lt;strong&gt;&lt;em&gt;Misstrauensvotum&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Vertrag von St Germain?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Staatsvertrag von &lt;strong&gt;St Germain en Laye&lt;/strong&gt; &lt;strong&gt;1919&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Friedensvertrag &lt;/strong&gt;geschlossen von &lt;strong&gt;Teilnehmern &lt;/strong&gt;am&lt;strong&gt; 1. WK&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zur &lt;strong&gt;Friedenssicherung Völkerbund &lt;/strong&gt;geschaffen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Deutschösterreich &lt;/strong&gt;als &lt;strong&gt;Staatsvertrag &lt;/strong&gt;gesehen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Deutschösterreich &lt;strong&gt;Rechtsnachfolger &lt;/strong&gt;von &lt;strong&gt;Österreich &lt;/strong&gt;und der &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;DÖ &lt;/strong&gt;muss &lt;strong&gt;Schuld am Krieg &lt;/strong&gt;bestätigen und sich zur &lt;strong&gt;Wiedergutmachung &lt;/strong&gt;verpflichten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Festlegung &lt;/strong&gt;des &lt;strong&gt;Staatsgebiets &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Gebietsabtretungen &lt;/strong&gt;an Nachbarländer&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anschlussverbot &lt;/strong&gt;von DÖ an das Deutsche Reicch&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Name&lt;/strong&gt; muss zu &lt;strong&gt;Österreich &lt;/strong&gt;geändert werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Distanz &lt;/strong&gt;zum &lt;strong&gt;Deutschen Reich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bekräftigung&lt;/strong&gt; der &lt;strong&gt;Kontinuität &lt;/strong&gt;zu &lt;strong&gt;Österreich &lt;/strong&gt;unter &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;DÖ zur &lt;strong&gt;Unabhängigkeit &lt;/strong&gt;verpflichtet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbot &lt;/strong&gt;der allg. &lt;strong&gt;Wehrpflicht &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Freiwilligenheer &lt;/strong&gt;max &lt;strong&gt;30.000 &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Weiteres:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;von &lt;strong&gt;konstituierender NV &lt;/strong&gt;nur &lt;strong&gt;unter Protest &lt;/strong&gt;anerkannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Diktatfriede&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Höhe &lt;/strong&gt;der &lt;strong&gt;Reparationszahlung&lt;/strong&gt; &lt;strong&gt;nie festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Alliierte &lt;/strong&gt;aufgrund &lt;strong&gt;schlechter Wirtschaftslage in Ö&lt;/strong&gt; &lt;strong&gt;verzichtet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das &lt;span style="background-color: yellow;"&gt;Berchtesgadener Abkommen?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1938 &lt;/strong&gt;gewann &lt;strong&gt;in Ö&lt;/strong&gt; die noch &lt;strong&gt;illegale NSDAP &lt;/strong&gt;an &lt;strong&gt;Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Februar 1938&lt;/strong&gt;: &lt;strong&gt;Hitler &lt;/strong&gt;trifft &lt;strong&gt;Schuschnigg &lt;/strong&gt;in &lt;strong&gt;Berchtesgaden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Hitler &lt;/strong&gt;stellt &lt;strong&gt;3 Tage Ultimatum &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö muss &lt;strong&gt;Außen&lt;/strong&gt;, &lt;strong&gt;Militär&lt;/strong&gt;, &lt;strong&gt;Wirtschaft &lt;/strong&gt;und &lt;strong&gt;Pressepolitik &lt;/strong&gt;an &lt;strong&gt;Deutsche anpassen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Betätigungsfreiheit &lt;/strong&gt;und &lt;strong&gt;Amnestie &lt;/strong&gt;für &lt;strong&gt;NSDAP &lt;/strong&gt;in &lt;strong&gt;Ö&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ernennung von &lt;strong&gt;Seyß-Inquart&lt;/strong&gt; zum &lt;strong&gt;Innenminister&lt;/strong&gt; mit &lt;strong&gt;Polizeigewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; Bei &lt;strong&gt;Ablehnung&lt;/strong&gt;: &lt;strong&gt;Einmarsch &lt;/strong&gt;der &lt;strong&gt;Wehrmacht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuschnigg beugt sich &lt;/strong&gt;Ultimatum im Glauben die &lt;strong&gt;Unabhängigkeit Ös zu sichern&lt;/strong&gt; und Seyß Inquart wird Innenminister&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Mai-Verfassung 1934&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Bestand aus &lt;em&gt;Mai-Verfassung 1934&lt;/em&gt; und &lt;em&gt;Verfassungs-Übergangsgesetz 1934&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;2x Erlassen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;auf Basis des &lt;strong&gt;KWEG&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;beide male &lt;strong&gt;rechtswidrig&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;5 Prinzipien&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;autoritär&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;bundesstaatlich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;christlich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;deutsch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;ständisch&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Gesetzgebung&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;4 beratende &lt;/strong&gt;Organe (Staatsrat, Bundeskulturrat, Bundeswirtschaftsrat, Länderrrat)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1 beschließendes Organ&lt;/strong&gt;: &lt;em&gt;Bundestag&lt;/em&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Verfahren:&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Initiative bei &lt;strong&gt;BReg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bei &lt;strong&gt;Ablehnung &lt;/strong&gt;durch &lt;strong&gt;Bundestag &lt;/strong&gt;-&amp;gt; &lt;strong&gt;BPräs &lt;/strong&gt;kann das &lt;strong&gt;Gesetz als VO &lt;/strong&gt;erlassen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;weiterer Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Berufung auf &lt;strong&gt;Gott&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufhebung der Gewaltentrennung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BReg&lt;/strong&gt;: &lt;strong&gt;Machtzentrum &lt;/strong&gt;der &lt;strong&gt;Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;BK Führer der BReg&lt;/em&gt; -&amp;gt; nur von BPräs abhängig&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Bundesgerichtshof &lt;/strong&gt;statt VfGH und VwGH&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Austrofaschismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Faschismus&lt;/strong&gt;: von &lt;strong&gt;Mussolini &lt;/strong&gt;gegründete &lt;strong&gt;Bewegung &lt;/strong&gt;und &lt;strong&gt;Ideologie &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bezeichnung &lt;/strong&gt;für &lt;strong&gt;ideologisch verwandte totalitäre&lt;/strong&gt; &lt;strong&gt;Systeme &lt;/strong&gt;in &lt;strong&gt;Europa&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Staat unter &lt;strong&gt;Führer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einzelperson&lt;/strong&gt; umfassend &lt;strong&gt;kontrollieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ideologische Gegner&lt;/strong&gt; &lt;strong&gt;vernichten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Austrofaschismus: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;1933-1938&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ständestaatlich &lt;/strong&gt;und &lt;strong&gt;faschistisch &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angelehnt an &lt;strong&gt;Mussolini &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Selbstbezeichnung &lt;strong&gt;Ständestaat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nationalistische&lt;/strong&gt; &lt;strong&gt;kontrarevolutionäre Wehreinheiten aus Heimwehren &lt;/strong&gt;entstanden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Antidemokratisch&lt;/strong&gt;,&lt;strong&gt; Antimarxistisch &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Staatsstreich auf Raten?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Begriff für die &lt;strong&gt;Selbstausschaltung &lt;/strong&gt;des &lt;strong&gt;Parlaments &lt;/strong&gt;und folgende &lt;strong&gt;Ausschaltung &lt;/strong&gt;des &lt;strong&gt;VfGH&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aber &lt;em&gt;verfehlt&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Parlament &lt;/strong&gt;kann sich in Demokratie als &lt;strong&gt;Repräsentant&lt;/strong&gt; des &lt;strong&gt;Volkswillen nicht &lt;/strong&gt;selbst &lt;strong&gt;ausschalten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Krise &lt;/strong&gt;war &lt;strong&gt;nur &lt;/strong&gt;im &lt;strong&gt;Plenum &lt;/strong&gt;(nicht im ganzen Parlament)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hauptausschuss &lt;/strong&gt;des NR &lt;strong&gt;tagte weiterhin&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Regierung &lt;/strong&gt;setzte &lt;strong&gt;Reaktivierung &lt;/strong&gt;des NR als &lt;strong&gt;Druckmittel &lt;/strong&gt;ein, um &lt;strong&gt;Verfassungsänderungen&lt;/strong&gt; &lt;strong&gt;erzwingen &lt;/strong&gt;zu können&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Selbstausschaltung des Parlaments?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nationalratssitzung März 1933&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Streit &lt;/strong&gt;über &lt;strong&gt;Gültigkeit &lt;/strong&gt;eines &lt;strong&gt;Stimmzettels &lt;/strong&gt;während Antrag&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Renner&lt;/strong&gt;, NR Präsident der &lt;strong&gt;SD &lt;/strong&gt;legt &lt;strong&gt;Amt nieder&lt;/strong&gt; um &lt;strong&gt;selbst wählen &lt;/strong&gt;zu können&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dann &lt;strong&gt;Ramek&lt;/strong&gt; der &lt;strong&gt;CS &lt;/strong&gt;und &lt;strong&gt;Staffner &lt;/strong&gt;der &lt;strong&gt;GD&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Nationalratspräsidenten &lt;/strong&gt;mehr &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geschäftsordnung&lt;/strong&gt; hatte &lt;strong&gt;keine Lösung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Letzter zurückgetretener Präsident &lt;/strong&gt;versucht &lt;strong&gt;neue&lt;/strong&gt; &lt;strong&gt;Sitzung &lt;/strong&gt;einzuberufen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung Dollfuß &lt;/strong&gt;spricht von &lt;strong&gt;Selbstausschaltung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erklärt &lt;strong&gt;neue Sitzung&lt;/strong&gt; für &lt;strong&gt;rechtswidrig &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Besetzung &lt;/strong&gt;des &lt;strong&gt;Parlamentsgebäudes &lt;/strong&gt;durch &lt;strong&gt;Polizei &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;Was war die VfGH Ausschaltung?&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;ul&gt;&lt;li&gt;nach "&lt;strong&gt;Ausschaltung &lt;/strong&gt;des &lt;strong&gt;Nationalrats&lt;/strong&gt;" nahm &lt;strong&gt;Regierung Gesetzgebung &lt;/strong&gt;für sich in Anspruch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Regierung &lt;strong&gt;wusste&lt;/strong&gt;, das &lt;strong&gt;VO Prüfung &lt;/strong&gt;durch &lt;strong&gt;VfGH nicht standhalten &lt;/strong&gt;würden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;daher: &lt;strong&gt;VfGH Ausschalten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;VO &lt;/strong&gt;das &lt;strong&gt;Mitglieder&lt;/strong&gt;/&lt;strong&gt;Ersatzmitglieder &lt;/strong&gt;des &lt;strong&gt;VfGH &lt;/strong&gt;die auf &lt;strong&gt;Vorschlag &lt;/strong&gt;von &lt;strong&gt;NR u. BR ernann&lt;/strong&gt;t wurden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nur an Sitzung teilnehmen&lt;/strong&gt; dürfen, wenn &lt;strong&gt;alle&lt;/strong&gt; der per Vorschlag von &lt;strong&gt;NR u. BR ernannten&lt;/strong&gt; Mitglieder daran &lt;strong&gt;teilnehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierungsnahe &lt;/strong&gt;Mitglieder legten &lt;strong&gt;VfGH Amt nieder&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Prüfung &lt;/strong&gt;der Verfassungsmäßigkeit damit &lt;strong&gt;verhindert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Weiters:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Republikanischer Schutzbund&lt;/strong&gt;, &lt;strong&gt;Kommunistische Partei&lt;/strong&gt; und &lt;strong&gt;NSDAP verboten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sozialdemokraten &lt;/strong&gt;mit &lt;strong&gt;Einschränkungen &lt;/strong&gt;belegt&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
+    <t>&lt;p&gt;Was war der Ständestaat?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;Berufsgruppen&lt;/strong&gt; &lt;strong&gt;organisierter &lt;/strong&gt;Staat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne polit&lt;/strong&gt;. &lt;strong&gt;Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne demokratisch &lt;/strong&gt;gewähltes &lt;strong&gt;Parlament&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dollfuß &lt;/strong&gt;verkündete &lt;strong&gt;September&lt;/strong&gt; &lt;strong&gt;1933&lt;/strong&gt;, dass &lt;strong&gt;ständische Gliederung &lt;/strong&gt;der Gesellschaft &lt;strong&gt;empfehlenswert &lt;/strong&gt;sei&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Arbeitgeber &lt;/strong&gt;und &lt;strong&gt;Arbeitnehmer &lt;/strong&gt;damit &lt;strong&gt;theoretisch gleich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Regierung &lt;strong&gt;scheiterte &lt;/strong&gt;an &lt;strong&gt;Durchsetzung&lt;/strong&gt;, &lt;strong&gt;nur 2 Stände &lt;/strong&gt;realisiert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;öffentlicher Dienst&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Land/Forstwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Vergleich des Ö. Ermächtigungsgesetz von 1934 zum D von 1933?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gemeinsamkeit&lt;/strong&gt;: &lt;strong&gt;Regierungsgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Besonderes Ö&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verfassungsbrüche &lt;/strong&gt;in der ersten Publikation &lt;strong&gt;reparieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eindruck der &lt;strong&gt;Verfassungskontinuität erwecken&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Weiters in Ö&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BReg &lt;/strong&gt;erhält &lt;em&gt;ohne Vorbehalte &lt;/em&gt;und &lt;em&gt;Beschränkungen &lt;/em&gt;&lt;strong&gt;einfache&lt;/strong&gt;- und &lt;strong&gt;Verfassungsgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Österreichische Bürgerkrieg (Februaraufstand 1934)?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Februar 1934 &lt;/strong&gt;4-Tägiger Bürgerkrieg&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schlecht verschlüsseltes&lt;/strong&gt; &lt;strong&gt;Telefonat&lt;/strong&gt; zwischen &lt;strong&gt;Sozialdemokrat &lt;/strong&gt;Otto &lt;strong&gt;Bauer &lt;/strong&gt;und &lt;strong&gt;Schutzbundführer &lt;/strong&gt;Richard &lt;strong&gt;Bernascheck &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schutzbund war &lt;strong&gt;bereits verboten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Folge: &lt;strong&gt;Hausdurchsuchungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Gesamte &lt;strong&gt;Leitung &lt;/strong&gt;des &lt;strong&gt;Linzer&lt;/strong&gt; &lt;strong&gt;Schutzbundes&lt;/strong&gt; wird &lt;strong&gt;entdeckt &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Widerstände - 4 Tage kämpfe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Regierung siegte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber&lt;strong&gt;: &lt;/strong&gt;Erster &lt;strong&gt;&lt;em&gt;Versuch&lt;/em&gt; &lt;em&gt;aufstieg Faschismus &lt;/em&gt;&lt;/strong&gt;zu &lt;em&gt;verhindern&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Verfassungsübergangsgesetz von 1934?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Regelt &lt;strong&gt;Übergang&lt;/strong&gt; zur &lt;strong&gt;ständischen Verfassung&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verlust &lt;/strong&gt;der &lt;strong&gt;Rechtsstaatlichkeit &lt;/strong&gt;durch &lt;strong&gt;Aufhebung &lt;/strong&gt;von &lt;strong&gt;Unabhängigkeit &lt;/strong&gt;und &lt;strong&gt;Unversetzbarkeit &lt;/strong&gt;der &lt;strong&gt;Richter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Untersagt Bundesgerichtshof &lt;/strong&gt;&lt;em&gt;Gesetze &lt;/em&gt;&lt;strong&gt;vor Juli 1934&lt;/strong&gt; auf &lt;strong&gt;Verfassungswidrigkeit &lt;/strong&gt;zu &lt;strong&gt;prüfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Einheitliche Führung &lt;/strong&gt;der &lt;strong&gt;Wirtschaft &lt;/strong&gt;an &lt;strong&gt;Regierung &lt;/strong&gt;übertragen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Weitergeltung &lt;/strong&gt;des &lt;strong&gt;ErmächtigungsG&lt;/strong&gt; &lt;strong&gt;1934 &lt;/strong&gt;angeordnet&lt;/li&gt;&lt;li&gt;Mitglieder des &lt;strong&gt;Bundeskultur&lt;/strong&gt;- und &lt;strong&gt;Bundeswirtschaftsrat &lt;/strong&gt;werden auf &lt;strong&gt;Vorschlag&lt;/strong&gt; der &lt;strong&gt;BR &lt;/strong&gt;vom &lt;strong&gt;BP berufen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;föderalistisches&lt;/strong&gt; Prinzip &lt;strong&gt;eingeschränkt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BK &lt;/strong&gt;kann &lt;strong&gt;LH&lt;/strong&gt;, &lt;strong&gt;Landesregierung&lt;/strong&gt; und &lt;strong&gt;Bürgermeister absetzen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die römischen Protokolle?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dollfuß &lt;/strong&gt;suchte &lt;strong&gt;Annäherung &lt;/strong&gt;an &lt;strong&gt;faschistisches Italien&lt;/strong&gt; zum &lt;strong&gt;Schutz vor &lt;/strong&gt;"&lt;strong&gt;Hitler&lt;/strong&gt;-Deutschland"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;17.3.1934 &lt;/strong&gt;wurden die röm. Protokolle von &lt;strong&gt;Italien&lt;/strong&gt;, &lt;strong&gt;Ungarn &lt;/strong&gt;und &lt;strong&gt;Österreich unterzeichnet&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;wirtschaftliche &lt;/strong&gt;und &lt;strong&gt;politische Zusammenarbeit&lt;/strong&gt; der 3 Staaten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unabhängigkeit Österreichs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Konkordat von 1934?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unterzeichnet &lt;/strong&gt;bereits &lt;strong&gt;1933&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Veröffentlicht &lt;/strong&gt;erst mit der &lt;strong&gt;2. Kundmachung&lt;/strong&gt; der &lt;strong&gt;Verfassung &lt;/strong&gt;von 1934 im &lt;strong&gt;Mai 1934&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;32 Artikel &lt;/strong&gt;im &lt;strong&gt;Verfassungsrang&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückgängigmachung &lt;/strong&gt;der &lt;strong&gt;Trennung&lt;/strong&gt; von &lt;strong&gt;Staat &lt;/strong&gt;und &lt;strong&gt;Kirche &lt;/strong&gt;von &lt;strong&gt;1868&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rekatholisierung &lt;/strong&gt;des Landes&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Annexionstheorie vs Okkupationstheorie&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Völkerrechtliche Stellung &lt;/strong&gt;Ös &lt;strong&gt;nach &lt;/strong&gt;dem &lt;strong&gt;Anschluss &lt;/strong&gt;lange &lt;strong&gt;umstritten &lt;/strong&gt;- auch die &lt;em&gt;Kriegsschuldfrage&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Annexionstheorie&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ö &lt;strong&gt;ging &lt;/strong&gt;mit Anschluss &lt;strong&gt;staats- und völkerrechtlich unter.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Okkupationstheorie&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ö &lt;strong&gt;völkerrechtlich &lt;/strong&gt;Handlungs&lt;strong&gt;unfähig &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Staat &lt;/strong&gt;hat &lt;strong&gt;aber &lt;/strong&gt;das NS-Regime&lt;strong&gt; in Art "Scheintod" überstanden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ö als &lt;em&gt;erstes Opfer &lt;/em&gt;Hitlers&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ab &lt;strong&gt;Moskauer Deklaration &lt;/strong&gt;30.&lt;strong&gt;10.1943&lt;/strong&gt; wurde &lt;strong&gt;Okkupationstheorie &lt;/strong&gt;bejaht&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Verfassungsnovelle 1925?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Ziele&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;B-VG 1920 vollenden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Doppelgleisigkeit &lt;/strong&gt;in der &lt;strong&gt;Verwaltung beenden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kompetenzbestimmungen &lt;/strong&gt;in Kraft bringen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Inhalt&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzbestimmungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verwaltung neu organisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Behörden staatlicher Verwaltung &lt;/strong&gt;nun &lt;strong&gt;organisatorisch Landesbehörden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;VfGH &lt;/strong&gt;wurde zuständig bei&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Komptenzkonflikten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Entscheidungsbefugnis &lt;/strong&gt;über &lt;strong&gt;Zuständigkeit &lt;/strong&gt;von &lt;strong&gt;Bund&lt;/strong&gt;/&lt;strong&gt;Land&lt;/strong&gt; bei &lt;strong&gt;Gesetzgebungs&lt;/strong&gt;- und &lt;strong&gt;Vollziehungsakten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was passierte 1804?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;August 1804&lt;/strong&gt;:&lt;strong&gt; Franz II&lt;/strong&gt; verlieh sich Titel des &lt;strong&gt;erblichen Kaisers von Ö&lt;/strong&gt; zusätzlich zu seinem &lt;strong&gt;bestehenden Titel als röm. deutscher Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine verfassungsrechtliche Bedeutung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Anlass:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausrufung &lt;/strong&gt;des &lt;strong&gt;erblichen Kaiserreichs &lt;/strong&gt;in Frankreich durch &lt;strong&gt;Napoleon &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Befürchtung&lt;/strong&gt;, dass der &lt;strong&gt;protestantische preußische König &lt;/strong&gt;bei der &lt;strong&gt;nächsten Kaiserwahl über &lt;/strong&gt;den &lt;strong&gt;kath&lt;/strong&gt;. &lt;strong&gt;Habsburger bevorzugt &lt;/strong&gt;wird.&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was passierte 1806?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Juni 1806&lt;/strong&gt;: 16 deutsche Fürsten unter Protektorat Napoleons: &lt;strong&gt;Rheinbund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;August 1806&lt;/strong&gt;: &lt;strong&gt;Niederlegung &lt;/strong&gt;der &lt;strong&gt;röm. deutschen&lt;/strong&gt; &lt;strong&gt;Kaiserkrone &lt;/strong&gt;durch &lt;strong&gt;Franz II&lt;/strong&gt; auf Forderung Napoleons &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Schlacht am weißen Berg? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1618&lt;/strong&gt; Ausbruch des&lt;strong&gt; 30-jährigen Kriegs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;politische&lt;/strong&gt; &lt;strong&gt;Ursachen &lt;/strong&gt;(&lt;em&gt;Prager Fenstersturz&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;religiöses Konfliktpotenzial&lt;/strong&gt; durch &lt;strong&gt;Komplikationen&lt;/strong&gt; aus &lt;strong&gt;Augsburger Religionsfrieden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sommer 1619 &lt;/strong&gt;schlossen sich &lt;strong&gt;böhmische Landstände &lt;/strong&gt;zur &lt;strong&gt;böhmischen&lt;/strong&gt; &lt;strong&gt;Konföderation &lt;/strong&gt;zusammen und &lt;strong&gt;verweigerten Untertanschaft &lt;/strong&gt;gegenüber &lt;strong&gt;Kaiser Ferdinand II&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Landstände &lt;strong&gt;protestantisch &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1620: Schlacht am Weißen Berg bei Prag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Heer der &lt;strong&gt;Landstände &lt;/strong&gt;von &lt;strong&gt;übermächtigen Gegnern vernichtend geschlagen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Gegner:&lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; Kaiser Ferdinand II&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Spanien&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Papst &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;und &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Herzog &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;von &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Bayern&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rekatholisierung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;politische Ziele &lt;/strong&gt;für die &lt;strong&gt;einzelnen Länder&lt;/strong&gt; nun vom &lt;strong&gt;Landesfürst alleine vorgegeben &lt;/strong&gt;(&lt;strong&gt;&lt;em&gt;politischer&lt;/em&gt;&lt;/strong&gt; &lt;strong&gt;&lt;em&gt;Absolutismus&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landstände &lt;/strong&gt;und &lt;strong&gt;ihre Institutionen&lt;/strong&gt; bleiben &lt;strong&gt;bestehen &lt;/strong&gt;(&lt;em&gt;institutioneller Dualismus&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;aber &lt;/strong&gt;dem Landesfürsten/Monarchen &lt;strong&gt;Untergeordnet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Nürnberger Rassegesetze?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Am &lt;strong&gt;15.9.1935&lt;/strong&gt; in &lt;strong&gt;Nürnberg &lt;/strong&gt;am &lt;strong&gt;Reichsparteitag der Freiheit &lt;/strong&gt;beschlossen&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Reichsflaggengesetz&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Austausch &lt;/strong&gt;der Farben&lt;strong&gt; Rot&lt;/strong&gt; &lt;strong&gt;Weiß Gold&lt;/strong&gt; der &lt;strong&gt;Weimarer&lt;/strong&gt; &lt;strong&gt;Republik&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gegen Weiß Rot Schwarz&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wenn möglich &lt;strong&gt;zusammen mit&lt;/strong&gt; &lt;strong&gt;Hakenkreuz &lt;/strong&gt;verwendet.&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-align-justify"&gt;&lt;br&gt;&lt;/p&gt;&lt;p class="ql-align-justify"&gt;&lt;strong&gt;Reichsbürgergesetz&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bevorzugung &lt;/strong&gt;Bürger von &lt;strong&gt;deutschem &lt;/strong&gt;und "&lt;strong&gt;artverwandtem&lt;/strong&gt;" &lt;strong&gt;Blutes &lt;/strong&gt;gegenüber &lt;strong&gt;Juden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aberkennung politischer &lt;/strong&gt;Rechte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;keine &lt;/strong&gt;Ausübung öffentlicher &lt;strong&gt;Ämter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Die&lt;strong&gt; erste VO&lt;/strong&gt; zum Gesetz legte fest wer &lt;strong&gt;Jude&lt;/strong&gt;, &lt;strong&gt;jüdischer&lt;/strong&gt; &lt;strong&gt;Mischling&lt;/strong&gt;, &lt;strong&gt;Geltungsjude &lt;/strong&gt;oder &lt;strong&gt;Deutschblütiger &lt;/strong&gt;ist&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-align-justify"&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Gesetz zum Schutz des deutschen Blutes und der deutschen Ehre&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;auch Blutschutzgesetz genannt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbietet Eheschließungen &lt;/strong&gt;zwischen &lt;strong&gt;Juden &lt;/strong&gt;und &lt;strong&gt;Staatsangehörigen &lt;/strong&gt;von &lt;strong&gt;deutschem&lt;/strong&gt; oder "&lt;strong&gt;artverwandtem&lt;/strong&gt;" &lt;strong&gt;Blut&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Schattendorfer Prozess?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Januar&lt;/strong&gt; &lt;strong&gt;1927 Kampf &lt;/strong&gt;zwischen &lt;strong&gt;Frontkämpfervereinigung &lt;/strong&gt;und &lt;strong&gt;Republikanischem&lt;/strong&gt; &lt;strong&gt;Schutzbund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frontkämpfer töteten &lt;/strong&gt;ein &lt;strong&gt;Kind &lt;/strong&gt;und einen &lt;strong&gt;Invaliden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Angeklagt, &lt;/strong&gt;jedoch von&lt;strong&gt; Geschworenen freigesprochen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Empörung &lt;/strong&gt;über &lt;strong&gt;Fehlurteil &lt;/strong&gt;unter der &lt;strong&gt;arbeitenden&lt;/strong&gt;, &lt;strong&gt;sozialdemokratischen &lt;/strong&gt;Bevölkerung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Massenprotest Juli 1927&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Justizpalast &lt;/strong&gt;in &lt;strong&gt;Brand &lt;/strong&gt;gesteckt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Regierung ging mit &lt;strong&gt;Polizei gegen Demonstrierende &lt;/strong&gt;vor&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Legitimität &lt;/strong&gt;der Regierung wurde &lt;strong&gt;in Frage &lt;/strong&gt;gestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rücktrittsforderungen&lt;/strong&gt; (durch SD) &lt;strong&gt;abgelehnt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Rechtsquellen der NSDAP?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Ohne feste Rangfolge:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Führerwille&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;nationalsozialistische Weltanschauung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;gesundes&lt;/strong&gt; &lt;strong&gt;Volksempfinden&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;NSDAP Parteiprogramm&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Lehenswesen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Verbindung &lt;/strong&gt;von &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vasallität &lt;/strong&gt;(&lt;strong&gt;persönliches&lt;/strong&gt; Element)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abhängigkeit &lt;/strong&gt;zwischen &lt;strong&gt;Vasall &lt;/strong&gt;und &lt;strong&gt;Herr&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vasall &lt;/strong&gt;leistet &lt;strong&gt;lebenslangen Dienst&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herr &lt;/strong&gt;gewährt &lt;strong&gt;Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Benefizium &lt;/strong&gt;(&lt;strong&gt;dingliches &lt;/strong&gt;Element) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herr &lt;/strong&gt;stattet Vasallen mit &lt;strong&gt;Grund &lt;/strong&gt;und &lt;strong&gt;Boden &lt;/strong&gt;aus &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schon&lt;/strong&gt; 718 &lt;strong&gt;Karl Martell&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;im &lt;strong&gt;Frühmittelalter entstanden&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Volksgerichtshof?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anlass&lt;/strong&gt;: &lt;strong&gt;unbefriedigender &lt;/strong&gt;Ausgang des &lt;strong&gt;Reichstagsbrandprozesses&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Hitler: dauerte &lt;strong&gt;zu lange&lt;/strong&gt;, &lt;strong&gt;lächerliches Ergebnis &lt;/strong&gt;(&lt;em&gt;Freispruch&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;Eingerichtet &lt;strong&gt;1934&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;IN&lt;strong&gt; Ö&lt;/strong&gt; ab &lt;strong&gt;1938&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste &lt;/strong&gt;und &lt;strong&gt;letzte Instanz &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem gegen den &lt;strong&gt;Tatbestand Verrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erlaubte &lt;strong&gt;Gegner &lt;/strong&gt;in "&lt;strong&gt;völlig legaler Weise&lt;/strong&gt;" zu &lt;strong&gt;verfolgen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Senate &lt;/strong&gt;bestehend aus&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zwei Berufsrichter&lt;/strong&gt;, von &lt;strong&gt;Hitler &lt;/strong&gt;auf &lt;strong&gt;Vorschlag &lt;/strong&gt;des &lt;strong&gt;Justizministers &lt;/strong&gt;ernannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Drei Laien&lt;/strong&gt;, üblicherweise hohe &lt;strong&gt;Funktionäre&lt;/strong&gt; der &lt;strong&gt;NSDAP&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Entwicklung der Rechtswissenschaften im 12./13 JH?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;MA zwei Rechtswelten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;heimisch&lt;/strong&gt;/&lt;strong&gt;partikuläres &lt;/strong&gt;Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aus &lt;strong&gt;Gewohnheitsrecht&lt;/strong&gt;/&lt;strong&gt;Fallrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sehr &lt;strong&gt;zersplittert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;zuerst &lt;strong&gt;Personalitätsprinzip &lt;/strong&gt;(Recht d. &lt;strong&gt;Geburtsort&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;danach &lt;strong&gt;Territorialitätsprinzip &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gelehrtes &lt;/strong&gt;Recht (&lt;strong&gt;ius commune&lt;/strong&gt;): röm + kanonisches (Kirchen-) Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab &lt;strong&gt;Ende 11 JH &lt;/strong&gt;basierend auf &lt;strong&gt;Wiederentdeckung &lt;/strong&gt;der &lt;strong&gt;Digesten&lt;/strong&gt; (&lt;strong&gt;&lt;em&gt;altröm&lt;/em&gt;&lt;/strong&gt;. &lt;strong&gt;&lt;em&gt;Rechtsliteratur&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entstehung der &lt;strong&gt;Rechtswissenschaften &lt;/strong&gt;an den &lt;strong&gt;Unis&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Scholastik&lt;/strong&gt; durch die &lt;strong&gt;Kanonisten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Digesten &lt;/strong&gt;umfangreich &lt;strong&gt;bearbeitet -&amp;gt; &lt;/strong&gt;&lt;em&gt;Methodik der Exegese&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Wort &lt;/strong&gt;+ &lt;strong&gt;Sacherklärungen &lt;/strong&gt;versehen -&amp;gt;&lt;em&gt; Glossen &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;(Übernahme) ab &lt;strong&gt;12 JH, 13 JH&lt;/strong&gt; ins &lt;strong&gt;gesamte Reich&lt;/strong&gt; verbreitet, durch &lt;strong&gt;Kirche&lt;/strong&gt; + &lt;strong&gt;Kaisertum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Kameralismus / Merkantilismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kameralismus &lt;/strong&gt;ist &lt;strong&gt;deutsche&lt;/strong&gt; &lt;strong&gt;Form &lt;/strong&gt;des &lt;strong&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Fokus&lt;/strong&gt; aber auf &lt;strong&gt;Landwirtschaft &lt;/strong&gt;und &lt;strong&gt;Bevölkerungswachstum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;vorherrschende Wirtschaftspolitik &lt;/strong&gt;in der &lt;strong&gt;Frühen&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eingriff des &lt;strong&gt;Staates &lt;/strong&gt;in die &lt;strong&gt;Wirtschaftsprozesse&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Förderung &lt;/strong&gt;des &lt;strong&gt;Handels&lt;/strong&gt;, vor allem des &lt;strong&gt;Außenhandels&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vernachlässigung&lt;/strong&gt; der &lt;strong&gt;Landwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landflucht &lt;/strong&gt;&amp;amp; &lt;strong&gt;Nahrungsknappheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; Einseitig&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Physiokratismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Landwirtschaft &lt;/strong&gt;als einzig &lt;strong&gt;produktive Kraft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bauer &lt;/strong&gt;ist &lt;strong&gt;Quelle&lt;/strong&gt; des &lt;strong&gt;Wohlstandes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landwirtschaft &lt;/strong&gt;in &lt;strong&gt;gebildeten Schichten&lt;/strong&gt; &lt;strong&gt;thematisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;eigener &lt;strong&gt;Lehrstuhl&lt;/strong&gt; der &lt;strong&gt;Nationalökonomie &lt;/strong&gt;an der &lt;strong&gt;Uni&lt;/strong&gt; &lt;strong&gt;Wien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der reichsständische Dualismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Machtausübung geteilt &lt;/strong&gt;zwischen &lt;strong&gt;König &lt;/strong&gt;und &lt;strong&gt;Reichsständen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3 Kurien&lt;/strong&gt; der Reichsstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kurfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsstädte &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reichsstände &lt;/strong&gt;bildeten den &lt;strong&gt;Reichstag&lt;/strong&gt;, dieser beschloss über&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;steuern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;außenpolitik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;gesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Reichstag &lt;strong&gt;vertrat nicht &lt;/strong&gt;Volk&lt;strong&gt;, &lt;/strong&gt;sondern &lt;strong&gt;Individualinteressen &lt;/strong&gt;der Reichsstände&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der landständische Dualismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Landesherr &lt;/strong&gt;war &lt;strong&gt;formell&lt;/strong&gt; Inhaber der &lt;strong&gt;Landesherrschaft&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;war ein &lt;strong&gt;reichsunmittelbarer Fürst&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Übte &lt;strong&gt;Reichsamt &lt;/strong&gt;das ihm &lt;strong&gt;königliche&lt;/strong&gt; &lt;strong&gt;Rechte&lt;/strong&gt; und &lt;strong&gt;Pflichten &lt;/strong&gt;ermöglichte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gerichts&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wehr&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Befestigungs&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verwaltungs&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kirchen&lt;/strong&gt;hoheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Landstände &lt;/strong&gt;entstanden aus &lt;strong&gt;Zusammenschlüssen landsässiger Herren &lt;/strong&gt;und &lt;strong&gt;Ritter&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bevorrechtete Personen&lt;/strong&gt; oder &lt;strong&gt;Gruppen &lt;/strong&gt;die einen Sitz und eine &lt;strong&gt;Stimme &lt;/strong&gt;im &lt;strong&gt;Landtag &lt;/strong&gt;hatten&lt;/li&gt;&lt;li&gt;Meist &lt;strong&gt;landsässiger Adel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Herrschaftsgewalt&lt;/strong&gt; &lt;strong&gt;geteilt &lt;/strong&gt;zwischen &lt;strong&gt;Landesherrn &lt;/strong&gt;und &lt;strong&gt;Landständen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ständig-landesfürstlicher Dualismus &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;verhinderte&lt;/strong&gt; Idee &lt;strong&gt;einheitlicher&lt;/strong&gt; &lt;strong&gt;Staaten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind Beispiele von frühkonstitutionellen und hochkonstitutionellen Verfassungen und Elementen?&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Frühkonstitutionell&lt;/em&gt;: &lt;strong&gt;Pillersdorfer &lt;/strong&gt;Verfassung, &lt;strong&gt;oktroyierte Märzverfassung&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;vom &lt;strong&gt;Monarchen einseitig erlassen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kein Selbstversammlungsrecht &lt;/strong&gt;des Parlaments&lt;/li&gt;&lt;li&gt;Kaiser &lt;strong&gt;absolutes&lt;/strong&gt; &lt;strong&gt;Veto&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundrechteschutz &lt;/strong&gt;mit Klage beim &lt;strong&gt;Reichsgericht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Hochkonstitutionell&lt;/em&gt;: &lt;strong&gt;Kremsierer &lt;/strong&gt;Entwurf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;volle Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzeskontrolle&lt;/strong&gt; durch &lt;strong&gt;freie Gerichte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;2-Kammern&lt;/strong&gt;system mit &lt;strong&gt;Selbstversammlungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;bloß &lt;strong&gt;suspensives&lt;/strong&gt; &lt;strong&gt;Veto &lt;/strong&gt;des Kaisers&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundrechteschutz&lt;/strong&gt; mittels &lt;strong&gt;Amtshaftung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was sind die 6 Reformen Maria Theresias?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Steuerreformen&lt;/li&gt;&lt;li&gt;Wirtschaftsreform&lt;/li&gt;&lt;li&gt;Agrarreform&lt;/li&gt;&lt;li&gt;Staatsreform (Behördenreform)&lt;/li&gt;&lt;li&gt;Religionsreform&lt;/li&gt;&lt;li&gt;Bildungsreform&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Steuerreformen Maria Theresias?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Ziel: &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;stehendes&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Heer&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;von &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;100.000&lt;/strong&gt; Mann&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;direkte &lt;/strong&gt;Steuern (vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Landesfürst gefordert&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;indirekte &lt;/strong&gt;Steuern (vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Landesfürsten genehmigt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;10-jährige Steuergarantie&lt;/strong&gt; der Landtage (&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dezennalrezesse&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegenleistung: &lt;strong&gt;Truppen&lt;/strong&gt; &lt;strong&gt;nicht&lt;/strong&gt; mehr &lt;strong&gt;verköstigen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Grundsteuerregulierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sämtl. &lt;strong&gt;Grundbesitz verzeichnet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Rustikalland&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(Bauern) &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;höher&lt;/strong&gt; als &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dominikalland &lt;/strong&gt;(Grundherren)&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Einkommens&lt;/strong&gt;- und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Besoldungssteuer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Wirtschaftsreformen Maria Theresias? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;basierend auf &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(56, 190, 155);"&gt;Gewerbe&lt;/em&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(56, 190, 155);"&gt;: &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Produktionssteigerung&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;durch &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufweichung&lt;/strong&gt;/&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufheben&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zunftvorschriften &lt;/strong&gt;für &lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Handel&lt;/em&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;: &lt;/span&gt;Ausbau der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verkehrswege&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zollpolitik&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Außenhandel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Neue &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wirtschaftsstandorte &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Förderung&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;von &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Fabriken &lt;/strong&gt;in wirtschaftl. unterentwickelten Regionen&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Zollwesen&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Abschaffung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Binnenzölle&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zollunion &lt;/strong&gt;der &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ö. Länder&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Agrarreform Maria Theresias?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verbesserung &lt;/strong&gt;der &lt;strong&gt;Verhältnisse &lt;/strong&gt;der Bauern durch &lt;strong&gt;Maria Theresia &lt;/strong&gt;(&lt;em&gt;freie Eheschließung&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Leistungspflichten gesenkt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Robotpatente&lt;/strong&gt;: &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Dauer &lt;/strong&gt;der &lt;strong&gt;Verpflichtungen&lt;/strong&gt; der &lt;strong&gt;Bauern&lt;/strong&gt; gegenüber Grundherr genau &lt;strong&gt;festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Joseph II:&lt;/em&gt; &lt;/strong&gt;Endgültige &lt;strong&gt;Abschaffung &lt;/strong&gt;grundherrschaftlicher &lt;strong&gt;Abhängigkeiten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Staatsreform (Behördenreform) Maria Theresias?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Ausschaltung&lt;/strong&gt; der &lt;strong&gt;ständischen Behörden&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Entmachtung&lt;/strong&gt; der &lt;strong&gt;Landstände&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Weiteres Ziel: &lt;em&gt;mehr gebildete Beamte&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Erste Reform: &lt;/em&gt;&lt;strong&gt;Haugwitzsche &lt;/strong&gt;Staatsreform&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Hofkanzlei &lt;/strong&gt;und &lt;strong&gt;Hofkriegsrat &lt;/strong&gt;wurden in &lt;strong&gt;Staatskanzlei &lt;/strong&gt;zusammengelegt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Trennung&lt;/strong&gt; von &lt;strong&gt;politischer Verwaltung &lt;/strong&gt;und &lt;strong&gt;Justiz&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Zweite Reform: &lt;/em&gt;benannt nach Staatskanzler&lt;strong&gt; Kaunitz-Rietberg&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Einsetzung des &lt;strong&gt;Staatsrat &lt;/strong&gt;- &lt;strong&gt;Beratung &lt;/strong&gt;des &lt;strong&gt;Herrschers &lt;/strong&gt;in allen &lt;strong&gt;Regierungsfragen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Religionsreform von Maria Theresia?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Maria Theresia &lt;/strong&gt;streng &lt;strong&gt;katholisch&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Herrschaft "&lt;strong&gt;gottgewollt&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Protestantenvertreibungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;auswandern&lt;/strong&gt; nach &lt;strong&gt;Ungarn &lt;/strong&gt;oder &lt;strong&gt;Siebenbürgen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vorurteile&lt;/strong&gt; gegenüber &lt;strong&gt;Juden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Bildungsreform von Maria Theresia?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;allgemeine Schulpflicht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gebildete &lt;/strong&gt;Bevölkerung &lt;strong&gt;mehr Nutzen &lt;/strong&gt;für Staat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;staatl&lt;/strong&gt;. &lt;strong&gt;Kontrolle &lt;/strong&gt;der &lt;strong&gt;Lehrinhalte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3&lt;/strong&gt; verschiedene &lt;strong&gt;Schultypen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;1-jährig &lt;strong&gt;Trivialschule &lt;/strong&gt;(obligat.)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hauptschulen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Normalschulen&lt;span class="ql-cursor"&gt;﻿&lt;/span&gt;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Von wann bis wann dauerte die frühe Neuzeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1500-1740&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der aufgeklärte Absolutismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Reformzeit: 1740-1792&lt;/p&gt;&lt;p&gt;Vormärz: 1792-1848&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der Frühkonstitutionalismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1848-1851&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der Neoabsolutismus?&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;1851-1867&lt;/p&gt;</t>
+  </si>
+  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der Konstitutionalismus?&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;1867-1918&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der Neoabsolutismus?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;1851-1867&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der Frühkonstitutionalismus?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;1848-1851&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann dauerte der aufgeklärte Absolutismus?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Reformzeit: 1740-1792&lt;/p&gt;&lt;p&gt;Vormärz: 1792-1848&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Von wann bis wann dauerte die frühe Neuzeit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;1500-1740&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Bildungsreform von Maria Theresia?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;allgemeine Schulpflicht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gebildete &lt;/strong&gt;Bevölkerung &lt;strong&gt;mehr Nutzen &lt;/strong&gt;für Staat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;staatl&lt;/strong&gt;. &lt;strong&gt;Kontrolle &lt;/strong&gt;der &lt;strong&gt;Lehrinhalte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3&lt;/strong&gt; verschiedene &lt;strong&gt;Schultypen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;1-jährig &lt;strong&gt;Trivialschule &lt;/strong&gt;(obligat.)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hauptschulen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Normalschulen&lt;span class="ql-cursor"&gt;﻿&lt;/span&gt;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Religionsreform von Maria Theresia?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Maria Theresia &lt;/strong&gt;streng &lt;strong&gt;katholisch&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Herrschaft "&lt;strong&gt;gottgewollt&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Protestantenvertreibungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;auswandern&lt;/strong&gt; nach &lt;strong&gt;Ungarn &lt;/strong&gt;oder &lt;strong&gt;Siebenbürgen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vorurteile&lt;/strong&gt; gegenüber &lt;strong&gt;Juden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Staatsreform (Behördenreform) Maria Theresias?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Ausschaltung&lt;/strong&gt; der &lt;strong&gt;ständischen Behörden&lt;/strong&gt; &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Entmachtung&lt;/strong&gt; der &lt;strong&gt;Landstände&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;Haugwitzsche Staatsreform&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Errichtung von &lt;strong&gt;Hofkanzlei&lt;/strong&gt; und &lt;strong&gt;Hofkriegsrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Trennung&lt;/strong&gt; von &lt;strong&gt;politischer Verwaltung &lt;/strong&gt;und &lt;strong&gt;Justiz&lt;/strong&gt; durch Schaffung &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;oberster Justizstelle &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kammer&lt;/strong&gt; als &lt;strong&gt;Verwaltungsbehörde&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Agrarreform Maria Theresias?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verbesserung &lt;/strong&gt;der &lt;strong&gt;Verhältnisse &lt;/strong&gt;der Bauern durch &lt;strong&gt;Maria Theresia &lt;/strong&gt;(&lt;em&gt;freie Eheschließung&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Leistungspflichten gesenkt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Robotpatente&lt;/strong&gt;: &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Dauer &lt;/strong&gt;der &lt;strong&gt;Verpflichtungen&lt;/strong&gt; der &lt;strong&gt;Bauern&lt;/strong&gt; gegenüber Grundherr genau &lt;strong&gt;festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Joseph II:&lt;/em&gt; &lt;/strong&gt;Endgültige &lt;strong&gt;Abschaffung &lt;/strong&gt;grundherrschaftlicher &lt;strong&gt;Abhängigkeiten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Wirtschaftsreformen Maria Theresias? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;basierend auf &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(56, 190, 155);"&gt;Gewerbe&lt;/em&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(56, 190, 155);"&gt;: &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Produktionssteigerung&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;durch &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufweichung&lt;/strong&gt;/&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Aufheben&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zunftvorschriften &lt;/strong&gt;für &lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Handel&lt;/em&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;: &lt;/span&gt;Ausbau der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verkehrswege&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zollpolitik&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Außenhandel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Neue &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wirtschaftsstandorte &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Förderung&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;von &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Fabriken &lt;/strong&gt;in wirtschaftl. unterentwickelten Regionen&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Zollwesen&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Abschaffung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Binnenzölle&lt;/strong&gt;, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Zollunion &lt;/strong&gt;der &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ö. Länder&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 6 Reformen Maria Theresias?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Steuerreformen&lt;/li&gt;&lt;li&gt;Wirtschaftsreform&lt;/li&gt;&lt;li&gt;Agrarreform&lt;/li&gt;&lt;li&gt;Staatsreform (Behördenreform)&lt;/li&gt;&lt;li&gt;Religionsreform&lt;/li&gt;&lt;li&gt;Bildungsreform&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Steuerreformen Maria Theresias?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ziel: &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;stehendes&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Heer&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;von &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;100.000&lt;/strong&gt; Mann&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;direkte &lt;/strong&gt;Steuern (vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Landesfürst gefordert&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;indirekte &lt;/strong&gt;Steuern (vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Landesfürsten genehmigt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;10-jährige Steuergarantie&lt;/strong&gt; der Landtage (&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dezennalrezesse&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gegenleistung: &lt;strong&gt;Truppen&lt;/strong&gt; &lt;strong&gt;nicht&lt;/strong&gt; mehr &lt;strong&gt;verköstigen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Grundsteuerregulierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sämtl. &lt;strong&gt;Grundbesitz verzeichnet&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Rustikalland&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(Bauern) &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;höher&lt;/strong&gt; als &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Dominikalland &lt;/strong&gt;(Grundherren)&lt;/li&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Einkommens&lt;/strong&gt;- und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Besoldungssteuer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Beispiele von frühkonstitutionellen und hochkonstitutionellen Verfassungen und Elementen?&lt;/p&gt;&lt;p&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;em&gt;Frühkonstitutionell&lt;/em&gt;: &lt;strong&gt;Pillersdorfer &lt;/strong&gt;Verfassung, &lt;strong&gt;oktroyierte Märzverfassung&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;vom &lt;strong&gt;Monarchen einseitig erlassen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;kein Selbstversammlungsrecht &lt;/strong&gt;des Parlaments&lt;/li&gt;&lt;li&gt;Kaiser &lt;strong&gt;absolutes&lt;/strong&gt; &lt;strong&gt;Veto&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundrechteschutz &lt;/strong&gt;mit Klage beim &lt;strong&gt;Reichsgericht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Hochkonstitutionell&lt;/em&gt;: &lt;strong&gt;Kremsierer &lt;/strong&gt;Entwurf&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;volle Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzeskontrolle&lt;/strong&gt; durch &lt;strong&gt;freie Gerichte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;2-Kammern&lt;/strong&gt;system mit &lt;strong&gt;Selbstversammlungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;bloß &lt;strong&gt;suspensives&lt;/strong&gt; &lt;strong&gt;Veto &lt;/strong&gt;des Kaisers&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundrechteschutz&lt;/strong&gt; mittels &lt;strong&gt;Amtshaftung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der landständische Dualismus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Landesherr &lt;/strong&gt;war &lt;strong&gt;formell&lt;/strong&gt; Inhaber der &lt;strong&gt;Landesherrschaft&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;war ein &lt;strong&gt;reichsunmittelbarer Fürst&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Übte &lt;strong&gt;Reichsamt &lt;/strong&gt;das ihm &lt;strong&gt;königliche&lt;/strong&gt; &lt;strong&gt;Rechte&lt;/strong&gt; und &lt;strong&gt;Pflichten &lt;/strong&gt;ermöglichte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gerichts&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wehr&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Befestigungs&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verwaltungs&lt;/strong&gt;hoheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kirchen&lt;/strong&gt;hoheit&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Landstände &lt;/strong&gt;entstanden aus &lt;strong&gt;Zusammenschlüssen landsässiger Herren &lt;/strong&gt;und &lt;strong&gt;Ritter&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bevorrechtete Personen&lt;/strong&gt; oder &lt;strong&gt;Gruppen &lt;/strong&gt;die einen Sitz und eine &lt;strong&gt;Stimme &lt;/strong&gt;im &lt;strong&gt;Landtag &lt;/strong&gt;hatten&lt;/li&gt;&lt;li&gt;Meist &lt;strong&gt;landsässiger Adel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Herrschaftsgewalt&lt;/strong&gt; &lt;strong&gt;geteilt &lt;/strong&gt;zwischen &lt;strong&gt;Landesherrn &lt;/strong&gt;und &lt;strong&gt;Landständen&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ständig-landesfürstlicher Dualismus &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;verhinderte&lt;/strong&gt; Idee &lt;strong&gt;einheitlicher&lt;/strong&gt; &lt;strong&gt;Staaten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der reichsständische Dualismus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Machtausübung geteilt &lt;/strong&gt;zwischen &lt;strong&gt;König &lt;/strong&gt;und &lt;strong&gt;Reichsständen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;3 Kurien&lt;/strong&gt; der Reichsstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kurfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsstädte &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reichsstände &lt;/strong&gt;bildeten den &lt;strong&gt;Reichstag&lt;/strong&gt;, dieser beschloss über&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;steuern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;außenpolitik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;strong&gt;gesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Reichstag &lt;strong&gt;vertrat nicht &lt;/strong&gt;Volk&lt;strong&gt;, &lt;/strong&gt;sondern &lt;strong&gt;Individualinteressen &lt;/strong&gt;der Reichsstände&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Physiokratismus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Landwirtschaft &lt;/strong&gt;als einzig &lt;strong&gt;produktive Kraft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bauer &lt;/strong&gt;ist &lt;strong&gt;Quelle&lt;/strong&gt; des &lt;strong&gt;Wohlstandes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landwirtschaft &lt;/strong&gt;in &lt;strong&gt;gebildeten Schichten&lt;/strong&gt; &lt;strong&gt;thematisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;eigener &lt;strong&gt;Lehrstuhl&lt;/strong&gt; der &lt;strong&gt;Nationalökonomie &lt;/strong&gt;an der &lt;strong&gt;Uni&lt;/strong&gt; &lt;strong&gt;Wien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Kameralismus / Merkantilismus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kameralismus &lt;/strong&gt;ist &lt;strong&gt;deutsche&lt;/strong&gt; &lt;strong&gt;Form &lt;/strong&gt;des &lt;strong&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Fokus&lt;/strong&gt; aber auf &lt;strong&gt;Landwirtschaft &lt;/strong&gt;und &lt;strong&gt;Bevölkerungswachstum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Merkantilismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;vorherrschende Wirtschaftspolitik &lt;/strong&gt;in der &lt;strong&gt;Frühen&lt;/strong&gt; &lt;strong&gt;Neuzeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eingriff des &lt;strong&gt;Staates &lt;/strong&gt;in die &lt;strong&gt;Wirtschaftsprozesse&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Förderung &lt;/strong&gt;des &lt;strong&gt;Handels&lt;/strong&gt;, vor allem des &lt;strong&gt;Außenhandels&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vernachlässigung&lt;/strong&gt; der &lt;strong&gt;Landwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landflucht &lt;/strong&gt;&amp;amp; &lt;strong&gt;Nahrungsknappheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; Einseitig&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Entwicklung der Rechtswissenschaften im 12./13 JH?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;MA zwei Rechtswelten:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;heimisch&lt;/strong&gt;/&lt;strong&gt;partikuläres &lt;/strong&gt;Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aus &lt;strong&gt;Gewohnheitsrecht&lt;/strong&gt;/&lt;strong&gt;Fallrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sehr &lt;strong&gt;zersplittert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;zuerst &lt;strong&gt;Personalitätsprinzip &lt;/strong&gt;(Recht d. &lt;strong&gt;Geburtsort&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;danach &lt;strong&gt;Territorialitätsprinzip &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gelehrtes &lt;/strong&gt;Recht (&lt;strong&gt;ius commune&lt;/strong&gt;): röm + kanonisches (Kirchen-) Recht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ab &lt;strong&gt;Ende 11 JH &lt;/strong&gt;basierend auf &lt;strong&gt;Wiederentdeckung &lt;/strong&gt;der &lt;strong&gt;Digesten&lt;/strong&gt; (&lt;strong&gt;&lt;em&gt;altröm&lt;/em&gt;&lt;/strong&gt;. &lt;strong&gt;&lt;em&gt;Rechtsliteratur&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Entstehung der &lt;strong&gt;Rechtswissenschaften &lt;/strong&gt;an den &lt;strong&gt;Unis&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Scholastik&lt;/strong&gt; durch die &lt;strong&gt;Kanonisten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Digesten &lt;/strong&gt;umfangreich &lt;strong&gt;bearbeitet, kommentiert &lt;/strong&gt;und Methoden zur &lt;strong&gt;Klärung von Widersprüchen &lt;/strong&gt;entwickelt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rezeption &lt;/strong&gt;(Übernahme) ab &lt;strong&gt;12 JH, 13 JH&lt;/strong&gt; ins &lt;strong&gt;gesamte Reich&lt;/strong&gt; verbreitet, durch &lt;strong&gt;Kirche&lt;/strong&gt; + &lt;strong&gt;Kaisertum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Volksgerichtshof?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Anlass&lt;/strong&gt;: &lt;strong&gt;unbefriedigender &lt;/strong&gt;Ausgang des &lt;strong&gt;Reichstagsbrandprozesses&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Hitler: dauerte &lt;strong&gt;zu lange&lt;/strong&gt;, &lt;strong&gt;lächerliches Ergebnis &lt;/strong&gt;(&lt;em&gt;Freispruch&lt;/em&gt;)&lt;/li&gt;&lt;li&gt;Eingerichtet &lt;strong&gt;1934&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;IN&lt;strong&gt; Ö&lt;/strong&gt; ab &lt;strong&gt;1938&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste &lt;/strong&gt;und &lt;strong&gt;letzte Instanz &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem gegen den &lt;strong&gt;Tatbestand Verrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erlaubte &lt;strong&gt;Gegner &lt;/strong&gt;in "&lt;strong&gt;völlig legaler Weise&lt;/strong&gt;" zu &lt;strong&gt;verfolgen&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Senate &lt;/strong&gt;bestehend aus&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zwei Berufsrichter&lt;/strong&gt;, von &lt;strong&gt;Hitler &lt;/strong&gt;auf &lt;strong&gt;Vorschlag &lt;/strong&gt;des &lt;strong&gt;Justizministers &lt;/strong&gt;ernannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Drei Laien&lt;/strong&gt;, üblicherweise hohe &lt;strong&gt;Funktionäre&lt;/strong&gt; der &lt;strong&gt;NSDAP&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Korneuburger Eid?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1928&lt;/strong&gt; begannen die &lt;strong&gt;Heimwehren &lt;/strong&gt;mit &lt;strong&gt;Vorbereitungen&lt;/strong&gt; für &lt;strong&gt;bewaffneten Putsch&lt;/strong&gt;, unterstützt von &lt;strong&gt;Christlichsozialen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Im &lt;strong&gt;Mai 1930 Korneuburger Eid&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bekenntnis&lt;/strong&gt; der &lt;strong&gt;Heimwehren &lt;/strong&gt;zum &lt;strong&gt;Faschismus &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gegen demokratisches&lt;/strong&gt; &lt;strong&gt;Parlament&lt;/strong&gt; und &lt;strong&gt;Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1931 Pfrimer Putsch&lt;/strong&gt; in der Steiermark &lt;/li&gt;&lt;li class="ql-indent-1"&gt;geprägt von &lt;strong&gt;Weltwirtschaftskrise&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schwächte &lt;/strong&gt;den &lt;strong&gt;Staat &lt;/strong&gt;weiter&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1932 zerbrach Koalition &lt;/strong&gt;der &lt;strong&gt;Christlichsozialen&lt;/strong&gt; und &lt;strong&gt;Großdeutschen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;nächste Koalition aus &lt;strong&gt;Christlichsozialen&lt;/strong&gt;, &lt;strong&gt;Heimwehren &lt;/strong&gt;und &lt;strong&gt;Landbund&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Lehenswesen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Verbindung &lt;/strong&gt;von &lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Vasallität &lt;/strong&gt;(&lt;strong&gt;persönliches&lt;/strong&gt; Element)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abhängigkeit &lt;/strong&gt;zwischen &lt;strong&gt;Vasall &lt;/strong&gt;und &lt;strong&gt;Herr&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vasall &lt;/strong&gt;leistet &lt;strong&gt;lebenslangen Dienst&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herr &lt;/strong&gt;gewährt &lt;strong&gt;Unterhalt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Benefizium &lt;/strong&gt;(&lt;strong&gt;dingliches &lt;/strong&gt;Element) &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herr &lt;/strong&gt;stattet Vasallen mit &lt;strong&gt;Grund &lt;/strong&gt;und &lt;strong&gt;Boden &lt;/strong&gt;aus &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schon&lt;/strong&gt; 718 &lt;strong&gt;Karl Martell&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;im &lt;strong&gt;Frühmittelalter entstanden&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Rechtsquellen der NSDAP?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Ohne feste Rangfolge:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Führerwille&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;nationalsozialistische Weltanschauung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;gesundes&lt;/strong&gt; &lt;strong&gt;Volksempfinden&lt;/strong&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;NSDAP Parteiprogramm&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Schattendorfer Prozess?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Januar&lt;/strong&gt; &lt;strong&gt;1927 Kampf &lt;/strong&gt;zwischen &lt;strong&gt;Frontkämpfervereinigung &lt;/strong&gt;und &lt;strong&gt;Republikanischem&lt;/strong&gt; &lt;strong&gt;Schutzbund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Frontkämpfer töteten &lt;/strong&gt;ein &lt;strong&gt;Kind &lt;/strong&gt;und einen &lt;strong&gt;Invaliden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Angeklagt, &lt;/strong&gt;jedoch von&lt;strong&gt; Geschworenen freigesprochen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Empörung &lt;/strong&gt;über &lt;strong&gt;Fehlurteil &lt;/strong&gt;unter der &lt;strong&gt;arbeitenden&lt;/strong&gt;, &lt;strong&gt;sozialdemokratischen &lt;/strong&gt;Bevölkerung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Massenprotest Juli 1927&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Justizpalast &lt;/strong&gt;in &lt;strong&gt;Brand &lt;/strong&gt;gesteckt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;SD fordern Rücktritt &lt;/strong&gt;der &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Christlichsozialer Bundeskanzler &lt;/strong&gt;erfuhr &lt;strong&gt;Stärkung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Nürnberger Rassegesetze?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Am &lt;strong&gt;15.9.1935&lt;/strong&gt; in &lt;strong&gt;Nürnberg &lt;/strong&gt;am &lt;strong&gt;Reichsparteitag der Freiheit &lt;/strong&gt;beschlossen&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Reichsflaggengesetz&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Austausch &lt;/strong&gt;der Farben&lt;strong&gt; Rot&lt;/strong&gt; &lt;strong&gt;Weiß Gold&lt;/strong&gt; der &lt;strong&gt;Weimarer&lt;/strong&gt; &lt;strong&gt;Republik&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;gegen Weiß Rot Schwarz&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wenn möglich &lt;strong&gt;zusammen mit&lt;/strong&gt; &lt;strong&gt;Hakenkreuz &lt;/strong&gt;verwendet.&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-align-justify"&gt;&lt;br&gt;&lt;/p&gt;&lt;p class="ql-align-justify"&gt;&lt;strong&gt;Reichsbürgergesetz&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bevorzugung &lt;/strong&gt;Bürger von &lt;strong&gt;deutschem &lt;/strong&gt;und "&lt;strong&gt;artverwandtem&lt;/strong&gt;" &lt;strong&gt;Blutes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Juden bleiben Träger von Rechten und Pflichten als Staatsangehörige&lt;/li&gt;&lt;li&gt;Die&lt;strong&gt; erste VO&lt;/strong&gt; legte fest wer &lt;strong&gt;Jude&lt;/strong&gt;, &lt;strong&gt;jüdischer&lt;/strong&gt; &lt;strong&gt;Mischling&lt;/strong&gt;, &lt;strong&gt;Geltungsjude &lt;/strong&gt;oder &lt;strong&gt;Deutschblütiger &lt;/strong&gt;ist&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-align-justify"&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Gesetz zum Schutz des deutschen Blutes und der deutschen Ehre&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;auch Blutschutzgesetz genannt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbietet Eheschließungen &lt;/strong&gt;zwischen &lt;strong&gt;Juden &lt;/strong&gt;und &lt;strong&gt;Staatsangehörigen &lt;/strong&gt;von &lt;strong&gt;deutschem&lt;/strong&gt; oder "&lt;strong&gt;artverwandtem&lt;/strong&gt;" &lt;strong&gt;Blut&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Schlacht am weißen Berg? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1618&lt;/strong&gt; Ausbruch des&lt;strong&gt; 30-jährigen Kriegs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;politische&lt;/strong&gt; &lt;strong&gt;Ursachen &lt;/strong&gt;(&lt;em&gt;Prager Fenstersturz&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;religiöses Konfliktpotenzial&lt;/strong&gt; durch &lt;strong&gt;Komplikationen&lt;/strong&gt; aus &lt;strong&gt;Augsburger Religionsfrieden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sommer 1619 &lt;/strong&gt;schlossen sich &lt;strong&gt;böhmische Landstände &lt;/strong&gt;zur &lt;strong&gt;böhmischen&lt;/strong&gt; &lt;strong&gt;Konföderation &lt;/strong&gt;zusammen und &lt;strong&gt;verweigerten Untertanschaft &lt;/strong&gt;gegenüber &lt;strong&gt;Kaiser Ferdinand II&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1620: Schlacht am Weißen Berg bei Prag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Heer der &lt;strong&gt;Landstände &lt;/strong&gt;von &lt;strong&gt;übermächtigen Gegnern vernichtend  geschlagen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Gegner:&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; Kaiser Ferdinand II&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Spanien&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Papst &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Herzog &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;von &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bayern&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;politische Ziele &lt;/strong&gt;für die &lt;strong&gt;einzelnen Länder&lt;/strong&gt; nun vom &lt;strong&gt;Landesfürst alleine vorgegeben &lt;/strong&gt;(&lt;strong&gt;&lt;em&gt;politischer&lt;/em&gt;&lt;/strong&gt; &lt;strong&gt;&lt;em&gt;Absolutismus&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landstände &lt;/strong&gt;und &lt;strong&gt;ihre Institutionen&lt;/strong&gt; bleiben &lt;strong&gt;bestehen &lt;/strong&gt;(&lt;em&gt;institutioneller Dualismus&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;aber &lt;/strong&gt;dem Landesfürsten/Monarchen &lt;strong&gt;Untergeordnet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was passierte 1806?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Juni 1806&lt;/strong&gt;: 16 deutsche Fürsten unter Protektorat Napoleons: &lt;strong&gt;Rheinbund&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;August 1806&lt;/strong&gt;: &lt;strong&gt;Niederlegung &lt;/strong&gt;der &lt;strong&gt;röm. deutschen&lt;/strong&gt; &lt;strong&gt;Kaiserkrone &lt;/strong&gt;durch &lt;strong&gt;Franz II&lt;/strong&gt; auf Forderung Napoleons &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was passierte 1804?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;August 1804&lt;/strong&gt;:&lt;strong&gt; Franz II&lt;/strong&gt; verlieh sich Titel des &lt;strong&gt;erblichen Kaisers von Ö&lt;/strong&gt; zusätzlich zu seinem &lt;strong&gt;bestehenden Titel als röm. deutscher Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine verfassungsrechtliche Bedeutung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Anlass:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausrufung &lt;/strong&gt;des &lt;strong&gt;erblichen Kaiserreichs &lt;/strong&gt;in Frankreich durch &lt;strong&gt;Napoleon &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Befürchtung&lt;/strong&gt;, dass der &lt;strong&gt;protestantische preußische König &lt;/strong&gt;bei der &lt;strong&gt;nächsten Kaiserwahl über &lt;/strong&gt;den &lt;strong&gt;kath&lt;/strong&gt;. &lt;strong&gt;Habsburger bevorzugt &lt;/strong&gt;wird.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Verfassungsnovelle 1925?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Ziele&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;B-VG 1920 vollenden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Doppelgleisigkeit &lt;/strong&gt;in der &lt;strong&gt;Verwaltung beenden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kompetenzbestimmungen &lt;/strong&gt;in Kraft bringen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Inhalt&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kompetenzbestimmungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verwaltung neu organisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Behörden staatlicher Verwaltung &lt;/strong&gt;nun &lt;strong&gt;organisatorisch Landesbehörden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;VfGH &lt;/strong&gt;wurde zuständig bei&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Komptenzkonflikten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Entscheidungsbefugnis &lt;/strong&gt;über &lt;strong&gt;Zuständigkeit &lt;/strong&gt;von &lt;strong&gt;Bund&lt;/strong&gt;/&lt;strong&gt;Land&lt;/strong&gt; bei &lt;strong&gt;Gesetzgebungs&lt;/strong&gt;- und &lt;strong&gt;Vollziehungsakten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Annexionstheorie vs Okkupationstheorie&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Völkerrechtliche Stellung &lt;/strong&gt;Ös &lt;strong&gt;nach &lt;/strong&gt;dem &lt;strong&gt;Anschluss &lt;/strong&gt;lange &lt;strong&gt;umstritten&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Annexionstheorie&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ö &lt;strong&gt;ging &lt;/strong&gt;mit Anschluss &lt;strong&gt;staats- und völkerrechtlich unter.&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Okkupationstheorie&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ö &lt;strong&gt;völkerrechtlich &lt;/strong&gt;Handlungs&lt;strong&gt;unfähig &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Staat &lt;/strong&gt;hat &lt;strong&gt;aber &lt;/strong&gt;das NS-Regime&lt;strong&gt; in Art "Scheintod" überstanden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Ab &lt;strong&gt;Moskauer Deklaration &lt;/strong&gt;30.&lt;strong&gt;10.1943&lt;/strong&gt;  wurde &lt;strong&gt;Okkupationstheorie &lt;/strong&gt;bejaht&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Konkordat von 1934?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Unterzeichnet &lt;/strong&gt;bereits &lt;strong&gt;1933&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Veröffentlicht &lt;/strong&gt;erst mit der &lt;strong&gt;2. Kundmachung&lt;/strong&gt; der &lt;strong&gt;Verfassung &lt;/strong&gt;von 1934 im &lt;strong&gt;Mai 1934&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;32 Artikel &lt;/strong&gt;im &lt;strong&gt;Verfassungsrang&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückgängigmachung &lt;/strong&gt;der &lt;strong&gt;Trennung&lt;/strong&gt; von &lt;strong&gt;Staat &lt;/strong&gt;und &lt;strong&gt;Kirche &lt;/strong&gt;von &lt;strong&gt;1868&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rekatholisierung &lt;/strong&gt;des Landes&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die römischen Protokolle?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Dollfuß &lt;/strong&gt;suchte &lt;strong&gt;Annäherung &lt;/strong&gt;an &lt;strong&gt;faschistisches Italien&lt;/strong&gt; zum &lt;strong&gt;Schutz vor &lt;/strong&gt;"&lt;strong&gt;Hitler&lt;/strong&gt;-Deutschland"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;17.3.1934 &lt;/strong&gt;wurden die röm. Protokolle von &lt;strong&gt;Italien&lt;/strong&gt;, &lt;strong&gt;Ungarn &lt;/strong&gt;und &lt;strong&gt;Österreich unterzeichnet&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhalt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;wirtschaftliche &lt;/strong&gt;und &lt;strong&gt;politische Zusammenarbeit&lt;/strong&gt; der 3 Staaten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unabhängigkeit Österreichs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Verfassungsübergangsgesetz von 1934?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Regelt &lt;strong&gt;Übergang&lt;/strong&gt; zur &lt;strong&gt;ständischen Verfassung&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verlust &lt;/strong&gt;der &lt;strong&gt;Rechtsstaatlichkeit &lt;/strong&gt;durch &lt;strong&gt;Aufhebung &lt;/strong&gt;von &lt;strong&gt;Unabhängigkeit &lt;/strong&gt;und &lt;strong&gt;Unversetzbarkeit &lt;/strong&gt;der &lt;strong&gt;Richter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Untersagt Bundesgerichtshof &lt;/strong&gt;&lt;em&gt;Gesetze &lt;/em&gt;&lt;strong&gt;vor Juli 1934&lt;/strong&gt; auf &lt;strong&gt;Verfassungswidrigkeit &lt;/strong&gt;zu &lt;strong&gt;prüfen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Einheitliche Führung &lt;/strong&gt;der &lt;strong&gt;Wirtschaft &lt;/strong&gt;an &lt;strong&gt;Regierung &lt;/strong&gt;übertragen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Weitergeltung &lt;/strong&gt;des &lt;strong&gt;ErmächtigungsG&lt;/strong&gt; &lt;strong&gt;1934 &lt;/strong&gt;angeordnet&lt;/li&gt;&lt;li&gt;Mitglieder des &lt;strong&gt;Bundeskultur&lt;/strong&gt;- und &lt;strong&gt;Bundeswirtschaftsrat &lt;/strong&gt;werden auf &lt;strong&gt;Vorschlag&lt;/strong&gt; der &lt;strong&gt;BR &lt;/strong&gt;vom &lt;strong&gt;BP berufen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;föderalistisches&lt;/strong&gt; Prinzip &lt;strong&gt;eingeschränkt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;BK &lt;/strong&gt;kann &lt;strong&gt;LH&lt;/strong&gt;, &lt;strong&gt;Landesregierung&lt;/strong&gt; und &lt;strong&gt;Bürgermeister absetzen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Österreichische Bürgerkrieg (Februaraufstand 1934)?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Februar 1934 &lt;/strong&gt;4-Tägiger Bürgerkrieg&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schlecht verschlüsseltes&lt;/strong&gt; &lt;strong&gt;Telefonat&lt;/strong&gt; zwischen &lt;strong&gt;Sozialdemokrat &lt;/strong&gt;Otto &lt;strong&gt;Bauer &lt;/strong&gt;und &lt;strong&gt;Schutzbundführer &lt;/strong&gt;Richard &lt;strong&gt;Bernascheck &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schutzbund war &lt;strong&gt;bereits verboten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Folge: &lt;strong&gt;Hausdurchsuchungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Gesamte &lt;strong&gt;Leitung &lt;/strong&gt;des &lt;strong&gt;Linzer&lt;/strong&gt; &lt;strong&gt;Schutzbundes&lt;/strong&gt; wird &lt;strong&gt;entdeckt &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Widerstände - 4 Tage kämpfe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Regierung siegte&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Unterschiede des Ö. Ermächtigungsgesetz von 1934 zum D von 1933?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erste Veröffentlichung &lt;/strong&gt;der &lt;strong&gt;Verfassung &lt;/strong&gt;von &lt;strong&gt;1934&lt;/strong&gt; sollte &lt;strong&gt;repariert &lt;/strong&gt;werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anschein &lt;/strong&gt;der &lt;strong&gt;Verfassungskontinuität &lt;/strong&gt;herstellen&lt;/li&gt;&lt;li&gt; &lt;strong&gt;Ö&lt;/strong&gt;: &lt;strong&gt;Verfassungsgesetzgebung &lt;/strong&gt;an &lt;strong&gt;Bundesregierung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeinsamkeit&lt;/strong&gt;: &lt;strong&gt;Gesetzgebung &lt;/strong&gt;durch &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Ständestaat?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;Berufsgruppen&lt;/strong&gt; &lt;strong&gt;organisierter &lt;/strong&gt;Staat&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne polit&lt;/strong&gt;. &lt;strong&gt;Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ohne demokratisch &lt;/strong&gt;gewähltes &lt;strong&gt;Parlament&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dollfuß &lt;/strong&gt;verkündete &lt;strong&gt;September&lt;/strong&gt; &lt;strong&gt;1933&lt;/strong&gt;, dass &lt;strong&gt;ständische Gliederung &lt;/strong&gt;der Gesellschaft &lt;strong&gt;empfehlenswert &lt;/strong&gt;sei&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Arbeitgeber &lt;/strong&gt;und &lt;strong&gt;Arbeitnehmer &lt;/strong&gt;damit &lt;strong&gt;theoretisch gleich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Regierung &lt;strong&gt;scheiterte &lt;/strong&gt;an &lt;strong&gt;Durchsetzung&lt;/strong&gt;, &lt;strong&gt;nur 2 Stände &lt;/strong&gt;realisiert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;öffentlicher Dienst&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Land/Forstwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
     <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann existierte die Demokratische Republik Österreich?&lt;/span&gt;&lt;/p&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;1920-1933&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;p&gt;Was war die Selbstausschaltung des Parlaments?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nationalratssitzung März 1933&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Streit &lt;/strong&gt;über &lt;strong&gt;Gültigkeit &lt;/strong&gt;eines &lt;strong&gt;Stimmzettels &lt;/strong&gt;während Antrag&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Renner&lt;/strong&gt;, NR Präsident der &lt;strong&gt;SD &lt;/strong&gt;legt &lt;strong&gt;Amt nieder&lt;/strong&gt; um &lt;strong&gt;selbst wählen &lt;/strong&gt;zu können&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dann &lt;strong&gt;Ramek&lt;/strong&gt; der &lt;strong&gt;CS &lt;/strong&gt;und &lt;strong&gt;Staffner &lt;/strong&gt;der &lt;strong&gt;GD&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Nationalratspräsidenten &lt;/strong&gt;mehr &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geschäftsordnung&lt;/strong&gt; hatte &lt;strong&gt;keine Lösung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Letzter zurückgetretener Präsident &lt;/strong&gt;versucht &lt;strong&gt;neue&lt;/strong&gt; &lt;strong&gt;Sitzung &lt;/strong&gt;einzuberufen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung Dollfuß &lt;/strong&gt;spricht von &lt;strong&gt;Selbstausschaltung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erklärt &lt;strong&gt;neue Sitzung&lt;/strong&gt; für &lt;strong&gt;rechtswidrig &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Besetzung &lt;/strong&gt;des &lt;strong&gt;Parlamentsgebäudes &lt;/strong&gt;durch &lt;strong&gt;Polizei &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Staatsstreich auf Raten?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kombination aus &lt;/p&gt;&lt;ul&gt;&lt;li&gt;Selbstausschaltung des Parlaments&lt;/li&gt;&lt;li&gt;VfGH Ausschaltung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Austrofaschismus?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Faschismus&lt;/strong&gt;: von &lt;strong&gt;Mussolini &lt;/strong&gt;gegründete &lt;strong&gt;Bewegung &lt;/strong&gt;und &lt;strong&gt;Ideologie &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bezeichnung &lt;/strong&gt;für &lt;strong&gt;ideologisch verwandte totalitäre&lt;/strong&gt; &lt;strong&gt;Systeme &lt;/strong&gt;in &lt;strong&gt;Europa&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Staat unter &lt;strong&gt;Führer&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einzelperson&lt;/strong&gt; umfassend &lt;strong&gt;kontrollieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ideologische Gegner&lt;/strong&gt; &lt;strong&gt;vernichten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Austrofaschismus: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;1933-1938&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ständestaatlich &lt;/strong&gt;und &lt;strong&gt;faschistisch &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Angelehnt an &lt;strong&gt;Mussolini &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Selbstbezeichnung &lt;strong&gt;Ständestaat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nationalistische&lt;/strong&gt; &lt;strong&gt;kontrarevolutionäre Wehreinheiten aus Heimwehren &lt;/strong&gt;entstanden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Antidemokratisch&lt;/strong&gt;,&lt;strong&gt; Antimarxistisch &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Mai-Verfassung 1934&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Im Kontext des &lt;strong&gt;Ermächtigungsgesetz &lt;/strong&gt;von&lt;strong&gt; 1934 2x&lt;/strong&gt; auf basis des KWEG&lt;strong&gt; erlassen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beide male &lt;strong&gt;verfassungswidrig&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Christlicher, autoritärer Ständestaat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gott &lt;/strong&gt;als&lt;strong&gt; Rechtserzeuger&lt;/strong&gt;, &lt;strong&gt;keine Volkssouveränität&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;3 (statt 4) Kompetenztypen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Finanzverfassungsgesetz &lt;/strong&gt;über Abgaben&lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine Gewaltentrennung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bundesgesetzgebung &lt;/strong&gt;durch bestimmte Organe von &lt;strong&gt;Organisationen&lt;/strong&gt;/&lt;strong&gt;Vereinen&lt;/strong&gt; sowie vom &lt;strong&gt;Bundeskanzler&lt;/strong&gt;- und &lt;strong&gt;Präsident bestimmte Personen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beschließendes &lt;/strong&gt;Organ: &lt;strong&gt;Bundestag&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Initiative &lt;/strong&gt;bei &lt;strong&gt;Bundesregierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;auch &lt;strong&gt;gesetzesändernde VO&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;BP &lt;/strong&gt;Notrecht &lt;strong&gt;Verfassungsgesetze &lt;/strong&gt;zu &lt;strong&gt;ändern&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Alle &lt;strong&gt;Akte &lt;/strong&gt;benötigten &lt;strong&gt;Gegenzeichnung &lt;/strong&gt;durch &lt;strong&gt;BK&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bundesgerichtshof &lt;/strong&gt;statt VfGH und VwGH&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das &lt;span style="background-color: yellow;"&gt;Berchtesgadener Abkommen?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1938 &lt;/strong&gt;gewann &lt;strong&gt;in Ö&lt;/strong&gt; die noch &lt;strong&gt;illegale NSDAP &lt;/strong&gt;an &lt;strong&gt;Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Februar 1938&lt;/strong&gt;: &lt;strong&gt;Hitler &lt;/strong&gt;trifft &lt;strong&gt;Schuschnigg &lt;/strong&gt;in &lt;strong&gt;Berchtesgaden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Hitler &lt;/strong&gt;stellt &lt;strong&gt;3 Tage Ultimatum &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö muss &lt;strong&gt;Außen&lt;/strong&gt;, &lt;strong&gt;Militär&lt;/strong&gt;, &lt;strong&gt;Wirtschaft &lt;/strong&gt;und &lt;strong&gt;Pressepolitik &lt;/strong&gt;an &lt;strong&gt;Deutsche anpassen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Betätigungsfreiheit &lt;/strong&gt;und &lt;strong&gt;Amnestie &lt;/strong&gt;für &lt;strong&gt;NSDAP &lt;/strong&gt;in &lt;strong&gt;Ö&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ernennung von &lt;strong&gt;Seyß-Inquart&lt;/strong&gt; zum &lt;strong&gt;Innenminister&lt;/strong&gt; mit &lt;strong&gt;Polizeigewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; Bei &lt;strong&gt;Ablehnung&lt;/strong&gt;: &lt;strong&gt;Einmarsch &lt;/strong&gt;der &lt;strong&gt;Wehrmacht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuschnigg beugt sich &lt;/strong&gt;Ultimatum im Glauben die &lt;strong&gt;Unabhängigkeit Ös zu sichern&lt;/strong&gt; und Seyß Inquart wird Innenminister&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Im März 1938: Machtzunahme&lt;/strong&gt; der Nationalsozialisten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schuschnigg &lt;/strong&gt;kündigt als letztes Mittel &lt;strong&gt;Volksabstimmung&lt;/strong&gt; über Unabhängigkeit&lt;strong&gt; &lt;/strong&gt;an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unternehmen Otto: &lt;/strong&gt;Einmarsch der deutschen Truppen &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erneutes &lt;strong&gt;Ultimatum &lt;/strong&gt;an Schuschnigg für &lt;strong&gt;Rücktritt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schuschnigg &lt;strong&gt;gibt nach&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Seyß-Inquart &lt;/strong&gt;wurde &lt;strong&gt;Bundeskanzler&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einmarsch &lt;/strong&gt;der Truppen begann&lt;strong&gt; am selben Tag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Seyß-Inquart unterzeichnet &lt;strong&gt;„Gesetz über Wiedervereinigung Österreichs mit dem Deutschen Reich“&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war der Augsburger Religionsfriede?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1517 Martin Luthers 95 Thesen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reform &lt;/strong&gt;der &lt;strong&gt;Kirche -&amp;gt; &lt;/strong&gt;v.a. gegen &lt;strong&gt;Ablasshandel&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;u.a. &lt;strong&gt;Kirchliche Regierungsgewalt &lt;/strong&gt;für &lt;strong&gt;Landesherren&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Karl V&lt;/strong&gt; verhängt &lt;strong&gt;Reichsacht &lt;/strong&gt;über Luther&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Protestanten &lt;/strong&gt;(evangelische Reichsstände) formen &lt;strong&gt;Schmalkaldischen Bund -&amp;gt; Krieg &lt;/strong&gt;mit Kaiser und Katholiken&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kaiser &lt;/strong&gt;erkennt, dass &lt;strong&gt;Protestantismus nicht militärisch &lt;/strong&gt;besiegt werden kann&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1552 &lt;/strong&gt;vorläufiger Frieden mit &lt;strong&gt;Passauer Vertrag &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1555 Augsburger Reichstag&lt;/strong&gt;: &lt;strong&gt;Langfristiger Friede &lt;/strong&gt;nach langen Verhandlungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Freie Religionsausübung &lt;/strong&gt;für jeden &lt;strong&gt;Fürsten &lt;/strong&gt;in &lt;strong&gt;seinem Land &lt;/strong&gt;(&lt;em&gt;Cuius regio, eius religio&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Untertanen&lt;/strong&gt; dürfen &lt;strong&gt;auswandern&lt;/strong&gt;, wenn sie mit &lt;strong&gt;Bekenntnis &lt;/strong&gt;des Fürsten&lt;strong&gt; &lt;/strong&gt;nicht einverstanden sind&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Hielt &lt;strong&gt;bis 1618 &lt;/strong&gt;→ 30-Jähriger Krieg&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Vertrag von St Germain?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Staatsvertrag von &lt;strong&gt;St Germain en Laye&lt;/strong&gt; &lt;strong&gt;1919&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Friedensvertrag &lt;/strong&gt;geschlossen von &lt;strong&gt;Teilnehmern &lt;/strong&gt;am&lt;strong&gt; 1. WK&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zur &lt;strong&gt;Friedenssicherung Völkerbund &lt;/strong&gt;geschaffen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Deutschösterreich &lt;/strong&gt;als &lt;strong&gt;Staatsvertrag &lt;/strong&gt;gesehen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Deutschösterreich &lt;strong&gt;Rechtsnachfolger &lt;/strong&gt;von &lt;strong&gt;Österreich &lt;/strong&gt;und der &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;DÖ &lt;/strong&gt;muss &lt;strong&gt;Schuld am Krieg &lt;/strong&gt;bestätigen und sich zur &lt;strong&gt;Wiedergutmachung &lt;/strong&gt;verpflichten&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Festlegung &lt;/strong&gt;des &lt;strong&gt;Staatsgebiets &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Gebietsabtretungen &lt;/strong&gt;an Nachbarländer&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Anschlussverbot &lt;/strong&gt;von DÖ an das Deutsche Reicch&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Name&lt;/strong&gt; muss zu &lt;strong&gt;Österreich &lt;/strong&gt;geändert werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Distanz &lt;/strong&gt;zum &lt;strong&gt;Deutschen Reich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bekräftigung&lt;/strong&gt; der &lt;strong&gt;Kontinuität &lt;/strong&gt;zu &lt;strong&gt;Österreich &lt;/strong&gt;unter &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;DÖ zur &lt;strong&gt;Unabhängigkeit &lt;/strong&gt;verpflichtet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verbot &lt;/strong&gt;der allg. &lt;strong&gt;Wehrpflicht &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Freiwilligenheer &lt;/strong&gt;max &lt;strong&gt;30.000 &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Weiteres:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;von &lt;strong&gt;konstituierender NV &lt;/strong&gt;nur &lt;strong&gt;unter Protest &lt;/strong&gt;anerkannt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Diktatfriede&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Höhe &lt;/strong&gt;der &lt;strong&gt;Reparationszahlung&lt;/strong&gt; &lt;strong&gt;nie festgelegt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Alliierte &lt;/strong&gt;aufgrund &lt;strong&gt;schlechter Wirtschaftslage in Ö&lt;/strong&gt; &lt;strong&gt;verzichtet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das &lt;strong&gt;Rumpfparlament &lt;/strong&gt;in Österreich 1934?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Stark verkleinertes Parlament da:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Sozialdemokraten&lt;/strong&gt; aufgrund von &lt;strong&gt;Parteiverbot &lt;/strong&gt;nicht teilnehmen konnten &lt;/li&gt;&lt;li&gt;&lt;strong&gt;großdeutsche &lt;/strong&gt;(Nationaler Wirtschaftsblock) größtenteils aus Protest &lt;strong&gt;boykottierten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das Wormser Konkordat? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;1122&lt;/em&gt;: &lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Wormser Konkordat &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zwischen &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Heinrich V&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und Papst &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Calixt II&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unterscheidung von &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Temporalien &lt;/strong&gt;(weltliche/materielle Güter) und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Spiritualien &lt;/strong&gt;(geistliches Amt)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Heinrich verzichtet&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;auf&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Investitur mit Ring und Stab&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;(Ehe mit Kirche + priesterliches Hirtentum) -&amp;gt; &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;keine Laieninvestitur &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;in geistliche Ämter &lt;/span&gt;mehr.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Papst&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gestand&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;zu&lt;/strong&gt;: Wahl von Bischöfen&lt;strong&gt; &lt;/strong&gt;und Äbten &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;des &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;deutschen Reiches in Gegenwart des Kaisers &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Konsequenzen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kaiser verliert &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Personalhoheit &lt;/strong&gt;über Reichskirche&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Bischöfe &lt;/strong&gt;und&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Äbte&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unabhängig &lt;/strong&gt;von Kaiser, &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Territorien&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;bleiben &lt;/strong&gt;in Kaisers Hand&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Reichskirche &lt;/strong&gt;wird &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;feudalisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Geistliche &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Reichsfürsten &lt;/strong&gt;(in der Lehenspyramide über weltlichen) nutzen Doppelstellung als geistliche+weltliche Herrscher um &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;kirchliche Landherrschaft&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;auszubauen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Königtum &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;büßt religiöses Prestige&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;(sakraler Nimbus) &lt;strong&gt;ein&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Investiturstreit?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1076 &lt;/strong&gt;bis &lt;strong&gt;1122 &lt;/strong&gt;(Wormser Konkordat)&lt;/li&gt;&lt;li&gt;Die Durchsetzung des &lt;strong&gt;libertas ecclasiae&lt;/strong&gt; (Kirchenfreiheit) durch &lt;strong&gt;Papst Gregor VII&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konflikt zwischen geistlicher und weltlicher Macht bzgl. &lt;strong&gt;Amtseinsetzungen von Geistlichen durch die weltliche Macht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kirche gegen Laieninvestitur&lt;/strong&gt;, Heinrich IV für.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eskalation: Heinrich IV lässt &lt;strong&gt;Papst&lt;/strong&gt; &lt;strong&gt;durch Bischofsversammlung in Worms absetzen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;1076&lt;/em&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;: &lt;/span&gt;&lt;strong&gt;Papst &lt;/strong&gt;Gregor VII &lt;strong&gt;exkommuniziert Heinrich IV&lt;/strong&gt;, u&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ntersagt Regierung und löst Treueeide -&amp;gt;&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; schränkt politische Handlungsfähigkeit stark ein&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Canossagang&lt;/strong&gt;: Heinrich IV geht zu Papst und bittet um &lt;strong&gt;Aufhebung der Exkommunizierung &lt;/strong&gt;-&amp;gt; &lt;strong&gt;erfolgreich&lt;/strong&gt;, beendet Streit aber nicht.&lt;strong&gt; &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1084&lt;/em&gt;: Erhebung des &lt;strong&gt;Gegenpapstes Klemens III &lt;/strong&gt;-&amp;gt; krönt Heinrich zu &lt;strong&gt;Kaiser&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vertrag von Sutri (strikte Trennung von REich und Kirche) gescheitert&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;Beendet &lt;/span&gt;&lt;em style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;1122 &lt;/em&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgb(40, 45, 88);"&gt;mit &lt;/span&gt;&lt;strong&gt;Wormser Konkordat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist eine&lt;strong&gt; Real&lt;/strong&gt;union?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Völkerrechtliche Verbindung selbständiger Staaten durch ein &lt;strong&gt;gemeinsames Staatsoberhaupt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Mit &lt;strong&gt;weiteren gemeinsamen&lt;/strong&gt; &lt;strong&gt;Institutionen&lt;/strong&gt;, also Staatsorganen und Verwaltungseinrichtungen&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Reichstag, was der Reichsrat in Österreich-Ungarn?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Reichstag: Parlament in Ungarn&lt;/p&gt;&lt;p&gt;Reichsrat: Parlament in Österreich (Eselsbrücke: Öste&lt;strong&gt;rr&lt;/strong&gt;eichs&lt;strong&gt;r&lt;/strong&gt;at)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der österreichisch-ungarische Ausgleich? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Verfassungsrechtliche Vereinbarung, durch die das Kaisertum Österreich zur &lt;strong&gt;österreichisch-ungarischen Monarchie&lt;/strong&gt; wurde.&lt;/li&gt;&lt;li&gt;Rechtliche Grundlagen bildeten die &lt;strong&gt;Pragmatische Sanktion &lt;/strong&gt;sowie der &lt;strong&gt;Gesetzesartikel XII von 1867 für Ungarn&lt;/strong&gt; und das &lt;strong&gt;Delegationsgesetz 1867&lt;/strong&gt; für Österreich. Ungarn ging dabei von einer abänderbaren Verpflichtung aus, Österreich von einem Vertrag. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die Rechtsnatur  „&lt;strong&gt;Realunion besonderer Art zweier ansonsten selbstständiger Staaten&lt;/strong&gt;“ . &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Teilung der Monarchie in 2 Staaten, in denen die &lt;strong&gt;pragmatischen Angelegenheiten gemeinsam&lt;/strong&gt; und andere (&lt;strong&gt;dualistische&lt;/strong&gt;) nach &lt;strong&gt;regelmäßig&lt;/strong&gt; zu &lt;strong&gt;vereinbarenden Grundätzen &lt;/strong&gt;zu behandeln waren. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichshälften: Cisleithanien (Österreich), Transleithanien (Ungarn)&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;pragmatischen Angelegenheiten &lt;/strong&gt;(&lt;strong&gt;Äußeres, Kriegswesen, Finanzen&lt;/strong&gt;) wurden durch &lt;strong&gt;zwei Delegationen &lt;/strong&gt;besorgt, die von den Parlamenten mit je 60 Mitgliedern beschickt wurden. Zum &lt;strong&gt;Inkrafttreten&lt;/strong&gt; &lt;strong&gt;der Beschlüsse&lt;/strong&gt;, die durch die Minister vorgelegt wurden, bedurfte es &lt;strong&gt;zweier übereinstimmender Beschlüsse der Delegationen&lt;/strong&gt; und keinem Veto. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;militärische Oberbefehl lag beim Kaiser&lt;/strong&gt;, hier war &lt;strong&gt;keine Gegenzeichnung &lt;/strong&gt;der Minister notwendig.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;Finanzierung &lt;/strong&gt;sollte sich nach einer vom &lt;strong&gt;Reichsrat &lt;/strong&gt;(Ö) und vom &lt;strong&gt;Reichstag&lt;/strong&gt; (U) zu &lt;strong&gt;sanktionierenden Aufteilung zwischen &lt;/strong&gt;den &lt;strong&gt;beiden Staaten &lt;/strong&gt;richten.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Dualistischen Angelegenheiten &lt;/strong&gt;(&lt;strong style="font-family: &amp;quot;Open Sans&amp;quot;;"&gt;Wirtschaftsfragen&lt;/strong&gt;): &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Getrennte, &lt;/strong&gt;aber &lt;strong&gt;übereinstimmende &lt;/strong&gt;Gesetze in Ö und U &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht durch die gemeinsamen Delegationen &lt;/strong&gt;beschlossen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Ö und U Behörden getrennt ausgeführt&lt;/strong&gt;, nicht von gemeinsamen Ministerien&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der Westfälische Friede?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der Westfälische Friede &lt;strong&gt;beendete &lt;/strong&gt;&lt;em&gt;1648 &lt;/em&gt;&lt;strong&gt;den 30-jährigen Krieg &lt;/strong&gt;formal, der &lt;strong&gt;eigentlich eine Reihe gesamteuropäischer Auseinandersetzungen&lt;/strong&gt; zusammenfasst, in denen es um die Vorherrschaft in Europa ging.&lt;/p&gt;&lt;ul&gt;&lt;li&gt;In &lt;strong&gt;Münster&lt;/strong&gt; fanden die Verhandlungen zwischen Kaiser, den Reichsständen&lt;strong&gt; &lt;/strong&gt;und &lt;strong&gt;Frankreich &lt;/strong&gt;statt.&lt;/li&gt;&lt;li&gt;In &lt;strong&gt;Osnabrück &lt;/strong&gt;fanden die Verhandlungen zwischen Kaiser, den Reichsständen&lt;strong&gt; &lt;/strong&gt;und &lt;strong&gt;Schweden &lt;/strong&gt;statt.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Die &lt;strong&gt;Ergebnisse &lt;/strong&gt;der Friedensverhandlungen wurden in einem eigentümlich verschränkten System völkerrechtlicher und rechtsstaatlicher Vereinbarungen in &lt;strong&gt;zwei getrennten, juristisch aber als Einheit betrachteten Urkunden, festgelegt.&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Konfessionelle Bestimmungen:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das &lt;strong&gt;reformierte Bekenntnis &lt;/strong&gt;(&lt;strong&gt;Calvin&lt;/strong&gt;) wurde dem &lt;strong&gt;augsburgischen &lt;/strong&gt;(&lt;strong&gt;Luther&lt;/strong&gt;) &lt;strong&gt;gleichgestellt&lt;/strong&gt;, beide Konfessionen &lt;strong&gt;den Katholiken gegenüber als Einheit behandelt.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Augsburger Religionsfriede&lt;/strong&gt; (cuius regio, eius religio) und durch eine&lt;strong&gt; Normaltags- und Normaljahrsregelung ergänzt&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wiederherstellung &lt;/strong&gt;des &lt;strong&gt;Besitzstandes &lt;/strong&gt;von Protestanten und Katholiken von&lt;strong&gt; 1. Januar 1624 &lt;/strong&gt;-&amp;gt; Vor allem Rückgängigmachung des &lt;strong&gt;Restitutionsedikts &lt;/strong&gt;von 1629, bei dem Kaiser Protestanten enteignete.&lt;/li&gt;&lt;li&gt;Der&lt;strong&gt; geistliche Vorbehalt&lt;/strong&gt; wurde auch &lt;strong&gt;auf protestantische Bistumsadministratoren ausgedehnt&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;In &lt;strong&gt;Religionsfragen &lt;/strong&gt;hatte der &lt;strong&gt;Reichstag &lt;/strong&gt;nicht in der &lt;strong&gt;Kuriengliederung&lt;/strong&gt;, &lt;strong&gt;sondern &lt;/strong&gt;getrennt nach &lt;strong&gt;Religionsgruppen &lt;/strong&gt;zu beraten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;freundschaftlicher Ausgleich statt&lt;/strong&gt; &lt;strong&gt;Mehrheitsprinzip&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Allgemeine Verfassungsfragen:&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die&lt;strong&gt; Territorialherrschaft der Reichsstände &lt;/strong&gt;wurde anerkannt. Dazu gehörte auch das &lt;strong&gt;ius foederis.&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;Struktur an der Reichsspitze&lt;/strong&gt; wurde durch die &lt;strong&gt;Anerkennung&lt;/strong&gt; &lt;strong&gt;der bayrischen&lt;/strong&gt; &lt;strong&gt;Kurwürde &lt;/strong&gt;verändert&lt;/li&gt;&lt;li&gt;Das &lt;strong&gt;beratende Stimmrecht &lt;/strong&gt;der &lt;strong&gt;Reichsstände &lt;/strong&gt;wurde in ein &lt;strong&gt;volles&lt;/strong&gt; &lt;strong&gt;Stimmrecht umgewandelt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Die &lt;strong&gt;obersten&lt;/strong&gt; &lt;strong&gt;Reichsgerichte&lt;/strong&gt;, besonders das &lt;strong&gt;Reichskammergericht&lt;/strong&gt;, sowie die &lt;strong&gt;Reichsdeputationen &lt;/strong&gt;sollten &lt;strong&gt;paritätisch &lt;/strong&gt;(Konfessionen zahlenmäßig gleich vertreten) &lt;strong&gt;besetzt &lt;/strong&gt;werden.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext der Dezemberverfassung 1867?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die Dezemberverfassung von 1867 ist &lt;strong&gt;keine umfassende Verfassungsurkunde&lt;/strong&gt;, sondern besteht aus mehren Gesetzen.&lt;/li&gt;&lt;li&gt;Die vom Reichsrat ausgearbeiteten Gesetze stellten einen &lt;strong&gt;Kompromiss &lt;/strong&gt;zwischen den &lt;strong&gt;monarchischen Ansprüchen&lt;/strong&gt; des &lt;strong&gt;Kaisers&lt;/strong&gt; und den &lt;strong&gt;liberalen-konstitutionellen Ideen &lt;/strong&gt;der &lt;strong&gt;Abgeordneten&lt;/strong&gt; dar.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Gesetz über die Verantwortlichkeit der Minister&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierungsakte&lt;/strong&gt; &lt;strong&gt;des Kaisers &lt;/strong&gt;waren von dem &lt;strong&gt;verantwortlichen&lt;/strong&gt; &lt;strong&gt;Minister&lt;/strong&gt; &lt;strong&gt;gegenzuzeichnen&lt;/strong&gt;. Dieser konnte durch vorsätzliche oder grob fahrlässige Verletzung der Verfassung sowie sonstiger Gesetze vom &lt;strong&gt;Reichsrat &lt;/strong&gt;zur &lt;strong&gt;Verantwortung gezogen &lt;/strong&gt;werden (&lt;strong&gt;Ministerialklage&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&amp;nbsp;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Grundgesetz über die Reichsvertretung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Das Grundgesetz über die Reichsvertretung&lt;strong&gt; änderte die Form von 1861 ab&lt;/strong&gt;, wodurch der Ausgleich praktisch vorweggenommen wurde:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Reichsrat bestand wie bisher aus &lt;strong&gt;Herren- und Abgeordnetenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Reichsrat sollte j&lt;strong&gt;ährlich vom Kaiser einberufen&lt;/strong&gt; werden&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gesetzgebungskompetenzen&lt;/strong&gt; wurden taxativ &lt;strong&gt;aufgezählt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gesetzesbeschluss bedurfte Zustimmung beider Häuser&lt;/strong&gt; und der &lt;strong&gt;Sanktion durch den Kaiser (=absolutes Veto)&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die allgemeinen Rechte der Staatsbürger&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechtskatalog der Dezemberverfassung, wobei eine Reihe von &lt;strong&gt;liberalen Freiheitsrechten&lt;/strong&gt; normiert wurden, jedoch&lt;strong&gt; keine sozialen oder politischen &lt;/strong&gt;Grundrechte. Die &lt;strong&gt;Möglichkeit der Aussetzung der Grundrechte&lt;/strong&gt; stellte eine gravierende Schwäche dar.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über Einsetzung eines Reichsgerichtes&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schuf erstmals die Möglichkeit &lt;strong&gt;Kompetenzkonflikte &lt;/strong&gt;zwischen &lt;strong&gt;Gerichten&lt;/strong&gt; &lt;strong&gt;und Verwaltungsbehörden &lt;/strong&gt;bzw &lt;strong&gt;Ländervertretern und Regierung &lt;/strong&gt;durch verbindlichen &lt;strong&gt;Beschluss des Reichsrates &lt;/strong&gt;zu &lt;strong&gt;lösen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Durch die &lt;strong&gt;Judikatur des Reichsgerichts &lt;/strong&gt;kam es zu einer Präzisierung der Grundrechte. Allerdings besaßen diese Erkenntnisse nur deklaratorischen Charakter, eine &lt;strong&gt;Aufhebung des verfassungswidrigen Aktes konnte nicht angeordnet werden&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die richterliche Gewalt &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stellte die Grundsätze der Gerichtsbarkeit dar (&lt;strong&gt;garantierte richterliche Unabhängigkeit&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;kündigte&lt;strong&gt; Regelungen zur Amtshaftung&lt;/strong&gt; an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;legte &lt;strong&gt;Öffentlichkeit der Verfahren &lt;/strong&gt;fest&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;und &lt;strong&gt;Verwaltung &lt;/strong&gt;bestätigt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;StGG über die Ausübung der Regierungs- und Vollzugsgewalt&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/em&gt;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Beschäftigte sich mit der&lt;strong&gt; Person des Kaisers (geheiligt, unverletzlich, unverantwortlich)&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Delegationsgesetz &lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ist die &lt;strong&gt;Vollzugsnorm des Ausgleichs&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompetenzverteilung zwischen &lt;/strong&gt;den &lt;strong&gt;Reichshälften &lt;/strong&gt;und deren Finanzierung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gemeinsame Organe &lt;/strong&gt;und deren &lt;strong&gt;Handlungsbefugnisse&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was unterscheidet den &lt;strong&gt;Augsburger Religionsfrieden &lt;/strong&gt;vom &lt;strong&gt;Westfälischen Frieden&lt;/strong&gt;? &lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Augsburger Religionsfrieden &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;bezog sich lediglich auf die &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Augsburger&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Konfession&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Luther&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;). &lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;westfälische Friede &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;bezog sich nun auch auf das &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;reformierte Bekenntnis&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; (&lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Calvin&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wurde der BP vor der Verfassungsnovelle 1929 gewählt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Durch die Bundesversammlung&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Skizzieren Sie die Entwicklung des Wahlrechts&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;Februarpatent 1861&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einrichtung von Reichsrat, eine Art Parlament aus &lt;strong&gt;Abgeordneten&lt;/strong&gt; und &lt;strong&gt;Herrenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herrenhaus von Kaiser &lt;/strong&gt;bestellt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abgeordnetenhaus von Landtagen &lt;/strong&gt;bestellt, dies gewählt.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landtagswahlrecht&lt;/strong&gt;: &lt;strong&gt;Kurienwahlrecht &lt;/strong&gt;(4: Großgrundbesitzer, Städte + Märkte + Industriestandorte, Handels + Gewerbekammern, Landgemeinden) + &lt;strong&gt;Zensuswahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Kurienwahlrecht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Zusammenfassung der&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; Wähler in Wählerklassen&lt;/span&gt;, denen unterschiedliche Mandate zukommen.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;&lt;em&gt;Zensuswahlrecht&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Wahlrecht von der &lt;strong&gt;Steuerleistung abhängig&lt;/strong&gt;, da politische Mitwirkungsrechte wirtschaftliche Unabhängigkeit voraussetzten. Dahinter stand die politische Zielsetzung, die &lt;strong&gt;feudale &lt;/strong&gt;und &lt;strong&gt;bürgerliche&lt;/strong&gt; &lt;strong&gt;Oberschicht &lt;/strong&gt;zu &lt;strong&gt;privilegieren&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Frauen nicht ausgeschlossen,&lt;/strong&gt; wenn Steuerleistung erfüllt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1873 &lt;/em&gt;&lt;strong&gt;&lt;em&gt;direkte Wahl der Abgeordneten&lt;/em&gt;&lt;/strong&gt; (ohne Umweg via Landtag), Wahlrecht nur mehr für Männer, außer Großgrundbesitzer&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1882: Taaffe'sche Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zensus &lt;/strong&gt;auf 5 Gulden &lt;strong&gt;gesenkt &lt;/strong&gt;-&amp;gt; mehr Wahlberechtigte &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verschiebung von Wahlbezirken &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1896: Badenische Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;5. Kurie: Allgemeine Wählerklasse&lt;/strong&gt; -&amp;gt; nur Männer&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Erfordert 1 Jahr Sesshaftigkeit &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Senkung von Steuerzensus&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pluralwahlrecht&lt;/strong&gt;: Mitglieder anderer Kurien konnten auch hier wählen. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Wenig Einfluss:&lt;/strong&gt; 5. Kurie wählte nur 72/425 Abgeordnete&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1907: Beck’sche Wahlrechtsreform&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abschaffung von Kurien+Zensuswahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Allgemeines, gleiches, direktes und geheimes Wahlrecht &lt;strong&gt;für Männer &lt;/strong&gt;→ jetzt gar keine Frauen mehr wählen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Erfordert 1 Jahr Sesshaftigkeit &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aufstockung der Mandate&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;1918: Allgemeines Wahlrecht auch für Frauen &lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;em&gt;Von 1933 (Ständestaat) über 1938 (Anschluss) bis 1945 (Republik Österreich) kein Wahlrecht, erst danach wieder. &lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was kennzeichnet die Verfassungsnovelle von 1929?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das &lt;strong&gt;B-VG 1920&lt;/strong&gt; stellte einen &lt;strong&gt;parteipolitischen Kompromiss&lt;/strong&gt; dar, den &lt;strong&gt;sozialdemokratische &lt;/strong&gt;und die &lt;strong&gt;Christlichsoziale &lt;/strong&gt;Partei aufgrund des herrschenden Kräfteverhältnisses im Nationalrat eingegangen waren. Es zeigte sich jedoch vor allem, dass das &lt;strong&gt;bürgerliche Lager &lt;/strong&gt;mit der &lt;strong&gt;bestehenden Verfassungslage&lt;/strong&gt; &lt;strong&gt;unzufrieden &lt;/strong&gt;war&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wesentliches Merkmal der &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verfassungsnovelle &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;war eine &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Neuordnung &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;des &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Verhältnisses&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; zwischen den &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;obersten&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundesorganen&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;. &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;NR &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;BP&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt; waren &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;gleichgeordnet&lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Bundesregierung &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;war sowohl vom &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;NR &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;als auch vom &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;BP abhängig.&amp;nbsp;&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Die &lt;strong&gt;Novelle &lt;/strong&gt;brachte eine &lt;strong&gt;Verschiebung der Kompetenzen zugunsten des Bundes&lt;/strong&gt; mit sich:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aufrechterhaltung der &lt;strong&gt;öffentlichen Ruhe, Ordnung und Sicherheit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Organisation und Führung der &lt;strong&gt;Bundespolizei &lt;/strong&gt;werden in &lt;strong&gt;Gesetzgebung und Vollziehung &lt;/strong&gt;dem &lt;strong&gt;Bund &lt;/strong&gt;übertragen.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Das Recht auf &lt;strong&gt;Einberufung des NR&lt;/strong&gt; kam nunmehr dem &lt;strong&gt;BP &lt;/strong&gt;zu. Die Bundesregierung hatte im Falle der Auflösung des NR Neuwahlen anzuordnen. Die &lt;strong&gt;Wahl der Bundesregierung&lt;/strong&gt; erfolgte &lt;strong&gt;nicht &lt;/strong&gt;mehr länger &lt;strong&gt;durch &lt;/strong&gt;den &lt;strong&gt;Nationalrat&lt;/strong&gt;, dessen Tätigkeit auf zwei ordentliche Tagungen pro Jahr konzentriert wurde.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der &lt;strong&gt;BP&lt;/strong&gt; wurde durch&lt;strong&gt; &lt;/strong&gt;das &lt;strong&gt;Bundesvolk gewählt&lt;/strong&gt;, eine &lt;strong&gt;Absetzung &lt;/strong&gt;des BP vor Ablauf seiner sechsjährigen Funktionsperiode war durch &lt;strong&gt;Volksabstimmung &lt;/strong&gt;möglich. Die &lt;strong&gt;Initiative &lt;/strong&gt;zu einer solchen Volksabstimmung stand der &lt;strong&gt;Bundesversammlung&lt;/strong&gt; zu. Der &lt;strong&gt;BP ernannte &lt;/strong&gt;und &lt;strong&gt;entließ &lt;/strong&gt;die &lt;strong&gt;Bundesregierung&lt;/strong&gt;.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Das &lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des Bundespräsidenten war an mehrere &lt;strong&gt;Voraussetzungen &lt;/strong&gt;geknüpft: Abwehr eines offenkundigen, nicht wiedergutzumachenden &lt;strong&gt;Schadens für die Allgemeinheit&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Der&lt;strong&gt; Bundesrat wurde durch einen Länder- und Ständerat ersetzt&lt;/strong&gt;, dessen Zusammensetzung durch ein eigenes Bundesverfassungsgesetz geregelt werden sollte, das &lt;strong&gt;jedoch nie erlassen&lt;/strong&gt; wurde. Es blieb daher defacto bei der alten Rechtslage.&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Die &lt;strong&gt;Gerichtshöfe&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;öffentlichen &lt;/strong&gt;Rechts sollten entpolitisiert werden, weshalb das &lt;strong&gt;Ernennungsrecht des&lt;/strong&gt; &lt;strong&gt;Nationalrates&lt;/strong&gt; &lt;strong&gt;in &lt;/strong&gt;ein &lt;strong&gt;bloßes Vorschlagsrecht umgewandelt &lt;/strong&gt;wurde. Der &lt;strong&gt;NR und der Länder- und Ständerat&lt;/strong&gt; erhielten das Vorschlagsrecht für &lt;strong&gt;drei Verfassungsrichter&lt;/strong&gt;, die &lt;strong&gt;Bundesregierung &lt;/strong&gt;war berechtigt, &lt;strong&gt;sechs Verfassungsrichter &lt;/strong&gt;vorzuschlagen. &lt;strong&gt;Ernannt&lt;/strong&gt; wurden sie &lt;strong&gt;vom BP&lt;/strong&gt;. Die neue Regelung hatte &lt;strong&gt;weniger &lt;/strong&gt;eine &lt;strong&gt;Entpolitisierung als &lt;/strong&gt;eine &lt;strong&gt;Umpolitisierung &lt;/strong&gt;zur Folge. Sämtliche Mitglieder der Verwaltungsgerichte wurden von der Bundesregierung vorgeschlagen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die &lt;strong&gt;konstitutionellen &lt;/strong&gt;Elemente der Dezemberverfassung von 1867?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;In Anknüpfung an die Verfassung von 1849 wies die Dezemberverfassung einige konstitutionelle Elemente auf:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ministerverantwortlichkeit &lt;/strong&gt;(politische und rechtliche Kontrolle)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gewaltentrennung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Verbindung der &lt;strong&gt;Volkssouveränität &lt;/strong&gt;mit der &lt;strong&gt;monarchischen&lt;/strong&gt; &lt;strong&gt;Legitimität&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Notverordnungen &lt;/strong&gt;mussten &lt;strong&gt;genehmigt &lt;/strong&gt;werden&amp;nbsp;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des Kaisers &lt;strong&gt;materiellen Schranken &lt;/strong&gt;unterworfen&lt;/li&gt;&lt;li&gt;Auch wenn nur &lt;strong&gt;deklaratorischer &lt;/strong&gt;Charakter, &lt;strong&gt;Überprüfung der Gesetze&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie wurde das Notverordnungsrecht in der Dezemberverfassung von 1867 geregelt? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&amp;nbsp;Noch im Juli 1867 wurde das Notverordnungsrecht des Grundgesetzes über die Reichsvertretung präzisiert und die &lt;strong&gt;Geltung der Notverordnungen &lt;/strong&gt;auf den &lt;strong&gt;Zeitraum&lt;/strong&gt; &lt;strong&gt;bis &lt;/strong&gt;zum nächsten &lt;strong&gt;Zusammentritt&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;Reichsrates beschränkt&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;Wenn die &lt;strong&gt;Notverordnungen nicht&lt;/strong&gt; &lt;strong&gt;binnen&lt;/strong&gt; &lt;strong&gt;vier Wochen&lt;/strong&gt; &lt;strong&gt;vorgelegt &lt;/strong&gt;wurden, &lt;strong&gt;erlosch&lt;/strong&gt; die Rechtskraft. &lt;/li&gt;&lt;li&gt;Dem &lt;strong&gt;kaiserlichen&lt;/strong&gt; &lt;strong&gt;Notverordnungsrecht&lt;/strong&gt; wurden &lt;strong&gt;materielle Schranken &lt;/strong&gt;gesetzt. So durften keine Verordnungen erlassen werden, die &lt;strong&gt;Staatsgrundgesetze verändern&lt;/strong&gt;, den &lt;strong&gt;Staatsschatz&lt;/strong&gt; dauernd &lt;strong&gt;belasten &lt;/strong&gt;oder &lt;strong&gt;Staatsgut veräußern&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Das Notverordnungsrecht wurde in der Folge &lt;strong&gt;immer extensiver genutzt &lt;/strong&gt;und mündete zur Zeit des Austrofaschismus in einer Überspannung des Anwendungsrahmens. Allerdings &lt;strong&gt;diente &lt;/strong&gt;es in der Zeit &lt;strong&gt;nach &lt;/strong&gt;der &lt;strong&gt;Dezemberverfassung &lt;/strong&gt;dazu, &lt;strong&gt;unaufschiebbare Materien &lt;/strong&gt;möglichst &lt;strong&gt;zeitnah &lt;/strong&gt;zu &lt;strong&gt;regeln&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie zeigte sich die Ministerverantwortlichkeit in der Dezemberverfassung von 1867?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Jeder der &lt;strong&gt;Kammern &lt;/strong&gt;hatte die Möglichkeit, einen &lt;strong&gt;Minister &lt;/strong&gt;wegen &lt;strong&gt;behaupteter&lt;/strong&gt; &lt;strong&gt;Gesetzesverletzung vor &lt;/strong&gt;einem neu einzurichtenden &lt;strong&gt;Staatsgerichtshof anzuklagen&lt;/strong&gt;.&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext des Ermächtigungsgesetzes von 1934? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Verfassung von 1934 &lt;/strong&gt;wurde &lt;strong&gt;zwei Mal erlassen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Das erste Mal erließ die Bundesregierung aufgrund des &lt;strong&gt;KWEG  (Kriegswirtschaftlichen Ermächtigungsgesetz) &lt;/strong&gt;eine Verordnung, die die Verfassung 1934 zum Inhalt hatte. Damit versuchte sie eine Verfassung zu erzwingen bzw. aufzuzwingen und stütze dies zumindest vorgeblich auf eine Rechtsgrundlage.&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Trotz der Berufung auf das KWEG war die &lt;strong&gt;Erlassung verfassungswidrig&lt;/strong&gt;. Einerseits &lt;strong&gt;überschritt &lt;/strong&gt;die Regierung damit sowohl den &lt;strong&gt;formellen &lt;/strong&gt;als auch &lt;strong&gt;materiellen&lt;/strong&gt; &lt;strong&gt;Rahmen&lt;/strong&gt; &lt;strong&gt;des&lt;/strong&gt; &lt;strong&gt;KWEG&lt;/strong&gt;, da dieses keineswegs zur Erlassung einer neuen Verfassung ermächtigte. Andererseits &lt;strong&gt;fehlte &lt;/strong&gt;die zur &lt;strong&gt;Gesamtänderung &lt;/strong&gt;der Verfassung gem Art 44 Abs 2 erforderliche &lt;strong&gt;Volksabstimmung&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch der zweite Weg basierte auf dem KWEG. Eine Notverordnung verfügte die Ergänzung der Geschäftsordnung des Nationalrates und der 1933 zurückgetretene christlichsoziale Nationalratspräsident Ramek berief für den 30. April 1934 den NR ein. Das &lt;strong&gt;76-köpfige Rumpfparlament stimmte mit 74 Stimmen für ein Bundesverfassungsgesetz&lt;/strong&gt; über außerordentliche Maßnahmen im Bereich der Verfassung. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Dieses sogenannte Ermächtigungsgesetz bestimmte zunächst die &lt;strong&gt;Aufhebung des Artikel 44 Abs 2&lt;/strong&gt;, der bei jeder &lt;strong&gt;Gesamtänderung eine Volksabstimmung vorsieht&lt;/strong&gt;. Zudem erklärte das Ermächtigungsgesetz die bereits am 24. April 1934 auf dem Verordnungsweg erlassene Verfassung zum „Bundesverfassungsgesetz auch im Sinne der gegenwärtig geltenden Verfassung“.&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&amp;nbsp;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;Funktionen des NR und des BR&lt;/strong&gt; galten als &lt;strong&gt;erloschen&lt;/strong&gt;, alle ihre &lt;strong&gt;Befugnisse &lt;/strong&gt;wurden der &lt;strong&gt;Bundesregierung&lt;/strong&gt; &lt;strong&gt;übertragen&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Das Ermächtigungsgesetz räumte der &lt;strong&gt;Bundesregierung &lt;/strong&gt;ferner die &lt;strong&gt;Befugnis &lt;/strong&gt;ein, den Übergang zur neuen Verfassung zu regeln und den Zeitpunkt des Beginns der Wirksamkeit der Verfassung 1934 festzusetzen. Diese Vorgehensweise sollte primär dazu dienen, das &lt;strong&gt;Ausland durch den Anschein von Rechtskontinuität zu beruhigen&lt;/strong&gt;, war aber dadurch aber nicht weniger &lt;strong&gt;verfassungswidrig &lt;/strong&gt;als die erste Erlassung der Verfassung 1934. Trotz der erheblichen Mängel im Gesetzgebungsverfahren &lt;strong&gt;beurkundete Bundespräsident &lt;/strong&gt;Miklas das &lt;strong&gt;verfassungsgemäße Zustandekommen des Ermächtigungsgesetzes&lt;/strong&gt;. Die &lt;strong&gt;Verfassung &lt;/strong&gt;sollte allerdings erst &lt;strong&gt;schrittweise wieder in Kraft&lt;/strong&gt; gesetzt werden, sodass &lt;strong&gt;zum Teil bis 1938&lt;/strong&gt; bezüglich zentraler Materien die Bestimmungen des Verfassungs-Übergangsgesetzes galten.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist Inhalt und Kontext des Ermächtigungsgesetzes von 1933? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Grundsätze der Weimarer Reichsverfassung &lt;/strong&gt;mussten zur Verwirklichung des nationalsozialistischen Führerstaates &lt;strong&gt;beseitigt &lt;/strong&gt;werden.&lt;/li&gt;&lt;li&gt;Am 27. Februar &lt;strong&gt;1933 brannte &lt;/strong&gt;der &lt;strong&gt;Reichstag &lt;/strong&gt;und Marinus van der Lubbe wurde als vermeintlicher Täter verhaftet.&lt;/li&gt;&lt;li&gt;Die Nationalsozialisten nahmen dies zum Anlass, um das &lt;strong&gt;Schreckensbild einer kommunistischen Revolution &lt;/strong&gt;heraufzubeschwören.&lt;/li&gt;&lt;li&gt;Deshalb wurde auf Art. 48 Abs 2 der Weimarer Reichsverfassung gestützt am &lt;strong&gt;28. Februar 1933&lt;/strong&gt; die &lt;strong&gt;Verordnung des Reichspräsidenten zum Schutz von Volk und Staat&lt;/strong&gt; erlassen, die die demokratiepolitisch &lt;strong&gt;wichtigen Grundrechte &lt;/strong&gt;nachhaltig &lt;strong&gt;beseitigte&lt;/strong&gt;. Durch die Beseitigung der nachstehenden Grundrechte war die Grundlage der Schreckensherrschaft von SS und Gestapo geschaffen:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht auf persönliche Freiheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Meinungsfreiheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Pressefreiheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vereinsfreiheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Versammlungsfreiheit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schutz des Briefgeheimnisses&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Unverletzlichkeit des Eigentums und der Wohnung&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zuvor hatte Hitler mit der&lt;strong&gt; Verordnung des Reichspräsidenten zum Schutze des deutschen Volkes (Schubladenverordnung)&lt;/strong&gt; bereits am 04. Februar 1933 die &lt;strong&gt;Versammlungs- und Pressefreiheit weitgehend beseitigt &lt;/strong&gt;und Minister Frick weitreichende Befugnisse zugesprochen.&lt;/li&gt;&lt;li&gt;Mit dem &lt;strong&gt;Ermächtigungsgesetz vom 24. März 1933 &lt;/strong&gt;bzw. dem Gesetz zur Behebung der Not von Volk und Reich ging die &lt;strong&gt;gesetzgebende Gewalt praktisch auf Adolf Hitler &lt;/strong&gt;über. Es war die Grundlage zur Aufhebung der Gewaltenteilung und ermöglichte alle folgenden Maßnahmen zur Festigung der nationalsozialistischen Diktatur. Am gravierendsten war, dass so&lt;strong&gt; verabschiedete Gesetze von der Verfassung abweichen durften&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Unter welchem &lt;/span&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Rechtsmakel &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;ist das Ermächtigungsgesetz von 1933 zustande gekommen? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gem. &lt;strong&gt;Artikel 76 der Weimarer Reichsverfassung&lt;/strong&gt; mussten mindestens &lt;strong&gt;2/3&lt;/strong&gt; der Abgeordneten für eine &lt;strong&gt;Verfassungsänderung &lt;/strong&gt;stimmen. &lt;/li&gt;&lt;li&gt;Dieses erhöhte Konsensquorum wurde auch bei der Abstimmung erzielt, allerdings verhinderte die &lt;strong&gt;vorangegangene Verhaftungswelle der gewählten KPD-Mitglieder&lt;/strong&gt; ein rechtskonformes Zustandekommen dieses Gesetzes.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;&amp;nbsp;Wie war das Wahlrecht vor der Goldenen Bulle? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das Wahlrecht bewegte sich im Spannungsfeld zwischen dem &lt;strong&gt;Wahlrecht des hohen Adels, Geblütsrecht einer bestimmten Dynastie und kirchlichen Ansprüchen&lt;/strong&gt;. Vor der Goldenen Bulle wurde der Kaiser vom Papst in Rom gekrönt, dem deutschen König kam eine Anwartschaft auf diese Kaiserkrönung zu. Daraus leitete das Papsttum eine Reihe umstrittener Rechte ab&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Approbation der deutschen Kaiserwahl&lt;/li&gt;&lt;li&gt;Reichsvikariat solange der Thron unbesetzt war&lt;/li&gt;&lt;li&gt;Depositionsrecht bzgl. des Königs/Kaisers&lt;/li&gt;&lt;li&gt;Recht, das Imperium auf ein anderes Reich zu übertragen&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das &lt;strong&gt;ius foederis&lt;/strong&gt;?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Das Recht der Fürsten, Bündnisse zu schließen, sofern sie sich nicht gegen den Kaiser richten&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der geistliche Vorbehalt im Zusammenhang mit dem Augsburger Religionsfrieden? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der &lt;strong&gt;reservatum ecclesiasticium &lt;/strong&gt;verhängte über die den Katholizismus aufgebenden geistlichen Territorialherren (Erzbischöfe, Bischöfe, Äbte, Prälaten) den ipso facto (durch diese Tatsache) eintretenden Verlust ihrer Territorien und Kirchenämter.&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was umfasst die Märzverfassung von 1919?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;März 1919 &lt;/strong&gt;von der &lt;strong&gt;konstituierenden&lt;/strong&gt; &lt;strong&gt;Nationalversammlung erlassen&lt;/strong&gt;, bestehend aus:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz über die &lt;strong&gt;Volksvertretung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gesetz über die &lt;strong&gt;Staatsregierung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Noch einmal ausdrücklich: &lt;strong&gt;Deutschösterreich &lt;/strong&gt;als &lt;strong&gt;demokratische Republik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Auch: &lt;strong&gt;Bestandteil &lt;/strong&gt;des &lt;strong&gt;Deutschen Reichs&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Willensbildung &lt;/strong&gt;im &lt;strong&gt;Parlament&lt;/strong&gt; -&amp;gt; &lt;strong&gt;parlamentarische&lt;/strong&gt; &lt;strong&gt;Republik&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzgebungshoheit &lt;/strong&gt;der &lt;strong&gt;Länder &lt;/strong&gt;anerkannt&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Staatsregierung &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;unter &lt;/em&gt;&lt;strong&gt;&lt;em&gt;politischer Verantwortlichkeit &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;der &lt;/em&gt;&lt;strong&gt;&lt;em&gt;NV &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;(&lt;/em&gt;&lt;strong&gt;&lt;em&gt;Misstrauensvotum&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was regelte die Dezember-Novelle von 1918?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Das &lt;strong&gt;Verhältnis zwischen den drei Präsidenten&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie &lt;strong&gt;zwischen&lt;/strong&gt; &lt;strong&gt;Staatsrat &lt;/strong&gt;und &lt;strong&gt;Provisorischer Nationalversammlung&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;Staatsrat &lt;/strong&gt;erhielt ein &lt;strong&gt;suspensives &lt;/strong&gt;Veto bezüglich der &lt;strong&gt;Gesetzesbeschlüsse &lt;/strong&gt;der &lt;strong&gt;provisorischen NV&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber: &lt;strong&gt;Beharrungsbeschluss&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist dismembratio?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Zerfall eines Staats in mehrere Staaten&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was bedeutet materielle Kontinuität bei formeller Diskontinuität?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Republik &lt;strong&gt;Deutschösterreich &lt;/strong&gt;führte &lt;strong&gt;neue Ordnung&lt;/strong&gt; auf &lt;strong&gt;Verfassungsebene &lt;/strong&gt;ein&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Übernahm &lt;/strong&gt;aber die &lt;strong&gt;Rechtsordnung darunter &lt;/strong&gt;von &lt;strong&gt;Österreich/Cisleithanien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Recht wurde &lt;strong&gt;von &lt;/strong&gt;der &lt;strong&gt;neuen DÖ Autorität verbindlich &lt;/strong&gt;gemacht, blieb aber &lt;strong&gt;inhaltlich &lt;/strong&gt;weitgehend &lt;strong&gt;unverändert&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Staatsrechtslehrer in Ö:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Merkl: &lt;strong&gt;Formelle Diskontinuität &lt;/strong&gt;wegen &lt;strong&gt;Revolution&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Kelsen: &lt;strong&gt;formelle Diskontinuität&lt;/strong&gt;, weil es sind &lt;strong&gt;zwei selbständige Staaten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Im &lt;strong&gt;Vertrag von St. Germain&lt;/strong&gt; musste Deutschösterreich die &lt;strong&gt;Kontinuität anerkennen&lt;/strong&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die Jakobinerprozesse?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Trotz &lt;strong&gt;Bemühungen&lt;/strong&gt; &lt;strong&gt;um Geheimhaltung &lt;/strong&gt;der österr. und ungar. &lt;strong&gt;Jakobiner &lt;/strong&gt;konnten die &lt;strong&gt;Polizei Spitzel &lt;/strong&gt;einschleusen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verhaftungswelle &lt;/strong&gt;im Juli &lt;strong&gt;1794 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Führende Köpfe wie &lt;strong&gt;Martinovics &lt;/strong&gt;und &lt;strong&gt;Riedel&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Exempel statuieren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anzeige wegen &lt;strong&gt;Majestätsbeleidigung &lt;/strong&gt;oder &lt;strong&gt;Landesverrat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Todesstrafe &lt;/strong&gt;für &lt;strong&gt;ungarische Bürger &lt;/strong&gt;und &lt;strong&gt;Militärpersonen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Für &lt;strong&gt;österreichische Zivilisten &lt;/strong&gt;war &lt;strong&gt;keine Todesstrafe &lt;/strong&gt;möglich&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Sondergericht &lt;/strong&gt;um &lt;strong&gt;Todesstrafe &lt;/strong&gt;zu &lt;strong&gt;ermöglichen von  &lt;/strong&gt;&lt;em&gt;Jurist &lt;/em&gt;&lt;strong&gt;Karl Anton von Martini&lt;/strong&gt; &lt;strong&gt;&lt;em&gt;verhindert &lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stattdessen: schwerer Festungsarrest&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt; Was ist die oktroyierte Märzverfassung von &lt;strong&gt;1849&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;Auflösung des&lt;/strong&gt; &lt;strong&gt;Reichstages&lt;/strong&gt; in &lt;strong&gt;Kremsier verabschiedete &lt;/strong&gt;der &lt;strong&gt;Kaiser &lt;/strong&gt;eine &lt;strong&gt;oktroyierte &lt;/strong&gt;(&lt;em&gt;aufgezwungene&lt;/em&gt;) &lt;strong&gt;Verfassung&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Inhaltlich &lt;/strong&gt;geprägt von &lt;strong&gt;Innenminister Graf &lt;/strong&gt;Franz &lt;strong&gt;Stadion&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Revolution niedergeschlagen&lt;/strong&gt;, aber: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ideen&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;konnten &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;nicht&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;mehr &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;unterdrückt &lt;/strong&gt;werde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle Elemente sind dem &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Konstitutionalismus &lt;/strong&gt;verpflichtet (&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gesetzgebung&lt;/em&gt;, &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichtsbarkeit&lt;/em&gt;, &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundrechtspatent&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gewaltenteilendes &lt;/strong&gt;Prinzip&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Föderalismus &lt;/strong&gt;(-&amp;gt; Nationale Forderungen)&lt;/li&gt;&lt;li&gt;Aber: &lt;strong&gt;frühkonstitutionelle &lt;/strong&gt;Elemente&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;absolutes&lt;/strong&gt; &lt;strong&gt;Veto &lt;/strong&gt;des Kaisers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein Selbstversammlungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nie umgesetzt Kaiser &lt;/strong&gt;regierte &lt;strong&gt;absolut&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war das Oktoberdiplom von 1860? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Verwaltungsreform &lt;/strong&gt;ohne &lt;strong&gt;tatsächlich &lt;/strong&gt;was &lt;strong&gt;zu ändern&lt;/strong&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Verweis auf die &lt;strong&gt;Erbfolgeordnung &lt;/strong&gt;der &lt;strong&gt;pragmatischen Sanktion&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unteilbarkeit &lt;/strong&gt;der habsburgischen Länder&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beteiligung &lt;/strong&gt;der &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Völker&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;in &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Gesetzgebung &lt;/strong&gt;und &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zusammenwachsen &lt;/strong&gt;der &lt;strong&gt;Völker &lt;/strong&gt;durch&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Staatsbürgerliche &lt;strong&gt;Gleichheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gleiche Wehr&lt;/strong&gt;- und &lt;strong&gt;Steuerpflicht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Religionsfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Gleicher &lt;strong&gt;Ämterzugang&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Kontext:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Versuch &lt;/strong&gt;durch &lt;strong&gt;Verweis auf &lt;/strong&gt;die &lt;strong&gt;Landtage&lt;/strong&gt;, die &lt;strong&gt;ungarischen &lt;/strong&gt;Länder zu &lt;strong&gt;beruhigen&lt;/strong&gt; und die &lt;strong&gt;Einheit &lt;/strong&gt;der Monarchie zu &lt;strong&gt;festigen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;"&lt;strong&gt;Differenzierter&lt;/strong&gt;" &lt;strong&gt;Föderalismus &lt;/strong&gt;in der Monarchie: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarische Angelegenheiten &lt;/strong&gt;mit &lt;strong&gt;Landtag &lt;/strong&gt;behandelt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Nicht&lt;/strong&gt;-&lt;strong&gt;Ungarische &lt;/strong&gt;Länder beziehen zusätzlich &lt;strong&gt;weiterhin Reichstag&lt;/strong&gt; ein&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aufstockung &lt;/strong&gt;der von den &lt;strong&gt;Landtagen &lt;/strong&gt;zu entsendenden &lt;strong&gt;Reichsratsmitgliedern&lt;/strong&gt; auf &lt;strong&gt;100&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ankündigung &lt;/strong&gt;von &lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Justiz &lt;/strong&gt;und &lt;strong&gt;Verwaltung&lt;/strong&gt; und &lt;strong&gt;Stärkung &lt;/strong&gt;der &lt;strong&gt;Selbstverwaltung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Ungarn &lt;/strong&gt;erhielt zurück:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Historische &lt;strong&gt;Verfassung &lt;/strong&gt;(Vor 1848)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Hofkanzlei&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;oberster&lt;/strong&gt; &lt;strong&gt;Gerichtshof&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Sollte&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;ungarischen Adel &lt;/strong&gt;auf &lt;strong&gt;Seite&lt;/strong&gt; des &lt;strong&gt;Kaisers &lt;/strong&gt;bringen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zentralismus durch &lt;/strong&gt;neue Form des &lt;strong&gt;Föderalismus kaschieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Änderungen&lt;/strong&gt; wurden in &lt;strong&gt;Ungarn&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vom &lt;strong&gt;Feudaladel&lt;/strong&gt; &lt;strong&gt;begrüßt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Von der &lt;strong&gt;Mehrheit&lt;/strong&gt; der &lt;strong&gt;Bevölkerung&lt;/strong&gt; &lt;strong&gt;abgelehnt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Für die &lt;strong&gt;westlichen Länder&lt;/strong&gt; ergab es &lt;strong&gt;keine richtigen Änderungen&lt;/strong&gt;.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Mit welchem Gesetz wurde Frauen das Wahlrecht eingeräumt?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Gesetz vom &lt;strong&gt;18.12.1918&lt;/strong&gt; über die&lt;strong&gt; Wahlordnung für die konstituierende Nationalversammlung&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie und durch wen wurde Deutschösterreich gegründet?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Oktober 1918&lt;/strong&gt;: &lt;strong&gt;Gründung&lt;/strong&gt; der provisorischen Nationalversammlung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Oktoberverfassung 1918&lt;/strong&gt;: &lt;strong&gt;provisorische Nationalversammlung &lt;/strong&gt;gibt sich selbst &lt;strong&gt;oberste Staatsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionärer &lt;/strong&gt;Akt&lt;strong&gt;: keine&lt;/strong&gt; &lt;strong&gt;rechtliche Legitimierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;3 großen Parteien&lt;/strong&gt; (&lt;em&gt;Christlichsozial&lt;/em&gt;, &lt;em&gt;Sozialdemokratisch&lt;/em&gt;, &lt;em&gt;Deutsch-National&lt;/em&gt;) stellten je einen &lt;strong&gt;Präsidenten &lt;/strong&gt;der &lt;strong&gt;provisorischen Nationalversammlung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Versammlung bestand aus den &lt;strong&gt;1911 gewählten Mitgliedern &lt;/strong&gt;des &lt;strong&gt;Abgeordnetenhauses &lt;/strong&gt;aus &lt;strong&gt;deutschsprachigen &lt;/strong&gt;Gebieten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Wichtigste &lt;strong&gt;Aufgabe&lt;/strong&gt;: &lt;strong&gt;Verfassung &lt;/strong&gt;erarbeiten, und &lt;strong&gt;Wahl &lt;/strong&gt;einer &lt;strong&gt;konstituierenden Nationalversammlung vorbereiten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kaiser Karl verzichtet&lt;/strong&gt; in Erklärung am &lt;strong&gt;11. November 1918 &lt;/strong&gt;auf &lt;strong&gt;Anteil&lt;/strong&gt; an &lt;strong&gt;Staatsgeschäften &lt;/strong&gt;und &lt;strong&gt;erkannte Entscheidung Deutschösterreichs&lt;/strong&gt; über seine &lt;strong&gt;Staatsform&lt;/strong&gt; &lt;strong&gt;an&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesetz&lt;/strong&gt; vom &lt;strong&gt;12. November über die Staats- und Regierungsform von Deutschösterreich&lt;/strong&gt; erschuf den neuen &lt;strong&gt;Staat &lt;/strong&gt;als &lt;strong&gt;demokratische Republik&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Konzentrationsregierung &lt;/strong&gt;der&lt;strong&gt; 3 großen Lager&lt;/strong&gt; wurde&lt;strong&gt; &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;nach&lt;/strong&gt;&lt;strong&gt; den &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;ersten Monaten&lt;/strong&gt; der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;konstituierenden &lt;/strong&gt;&lt;strong&gt;NV &lt;/strong&gt;von &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Koalition &lt;/strong&gt;zwischen &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Sozialdemokraten&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Christlichsozialen&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;abgelöst&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Koalition &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;zerbrach&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;an &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Polarisierung &lt;/strong&gt;durch &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;interne Umwälzungen &lt;/strong&gt;der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Christlichsozialen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was unterscheidet frühkonstitutionelle Element von (hoch)konstitutionellen?&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Frühkonstitutionell: Position des Monarchen stärker durchgesetzt&lt;/li&gt;&lt;li&gt;Konstitutionell: Position des Volkes stärker durchgesetzt &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Handelt es sich bei der Gründung Deutschösterreichs um eine Revolution?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trotz &lt;/strong&gt;unüblichem &lt;strong&gt;unblutigem Verlauf&lt;/strong&gt;, kann von einer &lt;strong&gt;bürgerlichen demokratischen Revolution &lt;/strong&gt;gesprochen werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von &lt;strong&gt;Masse &lt;/strong&gt;der Bevölkerung &lt;strong&gt;getragen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bediente sich &lt;strong&gt;proletarischer Mittel&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Vor allem in Hinblick auf &lt;strong&gt;Beseitigung privilegierter&lt;/strong&gt; &lt;strong&gt;Zugänge &lt;/strong&gt;und &lt;strong&gt;Machtpositionen &lt;/strong&gt;eindeutig &lt;strong&gt;Revolutionscharakter&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Auch &lt;strong&gt;rechtlich&lt;/strong&gt;: &lt;strong&gt;Diskontinuität &lt;/strong&gt;der Verfassung&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Warum gründete sich Deutschösterreich? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ende &lt;/strong&gt;des 1. &lt;strong&gt;WK &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Ende&lt;/strong&gt; der &lt;strong&gt;Doppelmonarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vorrevolutionäre &lt;/strong&gt;Situation durch &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zerfall &lt;/strong&gt;der &lt;strong&gt;Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Auflösung&lt;/strong&gt; der K u. K &lt;strong&gt;Armee&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unzufriedenheit &lt;/strong&gt;der Massen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;schwierige&lt;strong&gt; Versorgungslage&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Lösung: &lt;strong&gt;Kompromiss, &lt;/strong&gt;Einigung auf&lt;strong&gt;:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;republikanische &lt;/strong&gt;Staatsform&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Demokratisierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abschaffung &lt;/strong&gt;des &lt;strong&gt;Adels&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Fortschrittliche Arbeits&lt;/strong&gt;- und &lt;strong&gt;Sozialgesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Von wann bis wann bestand die Republik Deutschösterreich?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;1918-1920&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;&amp;nbsp;Was versuchte Karl I 1918? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Staats&lt;/strong&gt;- und &lt;strong&gt;Verfassungsrechtlichen&lt;/strong&gt; &lt;strong&gt;Umbau &lt;/strong&gt;durch &lt;strong&gt;Manifest &lt;/strong&gt;vorantreiben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schaffung &lt;/strong&gt;eines &lt;strong&gt;Bundesstaates &lt;/strong&gt;unter &lt;strong&gt;Berücksichtigung nationaler Siedlungsgebiete&lt;/strong&gt; und &lt;strong&gt;autonomer Selbstbestimmung &lt;/strong&gt;angekündigt&lt;/li&gt;&lt;li&gt;Doppelter &lt;strong&gt;Fehlschlag&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Inhaltlich &lt;/strong&gt;nicht den &lt;strong&gt;Gegebenheiten entsprach&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zu spät &lt;/strong&gt;erfolgte&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Notverordnungsrecht und was das Kriegswirtschaftliche Ermächtigungsgesetz von 1914?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des Monarchen + Möglichkeit der &lt;strong&gt;Suspendierung &lt;/strong&gt;einzelner &lt;strong&gt;Grundrechte &lt;/strong&gt;-&amp;gt; zeigt &lt;strong&gt;Beschränktheit &lt;/strong&gt;der &lt;strong&gt;konstitutionellen Garantien&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kaiser &lt;/strong&gt;konnte &lt;strong&gt;auch&lt;/strong&gt; &lt;strong&gt;regieren&lt;/strong&gt;, wenn &lt;strong&gt;Parlament&lt;/strong&gt;/&lt;strong&gt;Reichsrat&lt;/strong&gt; &lt;strong&gt;nicht Regierungsfähig &lt;/strong&gt;waren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;auch &lt;/strong&gt;bei &lt;strong&gt;Versammlung &lt;/strong&gt;des &lt;strong&gt;Reichsrates &lt;/strong&gt;kam es zu &lt;strong&gt;Notverordnungen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;In den &lt;strong&gt;Kriegsjahren&lt;/strong&gt;: &lt;strong&gt;Kriegsabsolutismus &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;von &lt;strong&gt;1914 &lt;/strong&gt;-&lt;strong&gt;1917 vertagt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;weiter &lt;strong&gt;ausgebaut &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Wiedereinberufung &lt;/strong&gt;des &lt;strong&gt;Reichsrates 1917&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bestätigung &lt;/strong&gt;des &lt;strong&gt;Notverordnungsrechts &lt;/strong&gt;mittels &lt;strong&gt;Gesetzesbeschluss &lt;/strong&gt;als &lt;strong&gt;KWEG&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiserliche Notverordnung &lt;/strong&gt;von 1914 &lt;strong&gt;außer Kraft&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Begleitet von &lt;strong&gt;heftiger&lt;/strong&gt; &lt;strong&gt;Kritik &lt;/strong&gt;wegen vorhergehender &lt;strong&gt;Aussetzung &lt;/strong&gt;des &lt;strong&gt;Reichsrates &lt;/strong&gt;und &lt;strong&gt;exzessiver Notrecht &lt;/strong&gt;Nutzung. &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Aber&lt;/strong&gt;: &lt;strong&gt;Genehmigung einzelner Regierungsverordnungen &lt;/strong&gt;wäre &lt;strong&gt;nicht zeitlich &lt;/strong&gt;und &lt;strong&gt;rechtssicher Umsetzbar &lt;/strong&gt;gewesen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Daher &lt;strong&gt;trotz&lt;/strong&gt; &lt;strong&gt;erkennbarer&lt;/strong&gt; &lt;strong&gt;Ablehnung&lt;/strong&gt; zur &lt;strong&gt;Zustimmung genötigt &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung &lt;/strong&gt;sollte via &lt;strong&gt;per Verordnungsrecht Wirtschaftsleben &lt;/strong&gt;fördern, &lt;strong&gt;Versorgung &lt;/strong&gt;sichern, &lt;strong&gt;Schäden abwenden &lt;/strong&gt;können&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Kriegsabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Einschränkung &lt;/strong&gt;von &lt;strong&gt;Grundrechten&lt;/strong&gt; &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zensur&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unterstellung von &lt;strong&gt;Zivilpersonen &lt;/strong&gt;und &lt;strong&gt;Behörden &lt;/strong&gt;unter &lt;strong&gt;Armeekommando &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Aussetzung &lt;/strong&gt;der &lt;strong&gt;1917 &lt;/strong&gt;anstehenden &lt;strong&gt;Neuwahlen&lt;/strong&gt;&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann wurde die Sozialdemokratische Partei Österreichs gegründet?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;SD Arbeitervereine &lt;/strong&gt;und &lt;strong&gt;Bewegungen &lt;/strong&gt;waren &lt;strong&gt;staatlichen Repressionen &lt;/strong&gt;ausgesetzt und führten &lt;strong&gt;interne Kämpfe &lt;/strong&gt;über &lt;strong&gt;Ausrichtung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Konflikte&lt;/strong&gt; im &lt;strong&gt;Einigungskongress 1847 nicht ausgeräumt&lt;/strong&gt;, &lt;strong&gt;aber&lt;/strong&gt;: &lt;strong&gt;Gründung&lt;/strong&gt; der &lt;strong&gt;sozialdemokratischen Arbeiterpartei&lt;/strong&gt; &lt;strong&gt;Ö&lt;/strong&gt;.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1880er &lt;/strong&gt;vermehrt &lt;strong&gt;Spannungen &lt;/strong&gt;und &lt;strong&gt;Konflikte &lt;/strong&gt;über &lt;strong&gt;Ausrichtung &lt;/strong&gt;zwischen &lt;strong&gt;gemäßigten &lt;/strong&gt;und &lt;strong&gt;radikalen Kräften&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1888/89 &lt;/strong&gt;Einigung am &lt;strong&gt;Hainfelder Parteitag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"eigentliche &lt;strong&gt;Geburtsstunde&lt;/strong&gt;" der Partei&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Aus welchen Gesetzen besteht die Dezemberverfassung von 1867?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gesetz über die Ministerverantwortlichkeit&lt;/li&gt;&lt;li&gt;Grundgesetz über die Reichsvertretung&lt;/li&gt;&lt;li&gt;StGG über die Staatsbürgerrechte&lt;/li&gt;&lt;li&gt;StGG über das Reichsgericht&lt;/li&gt;&lt;li&gt;StGG über die richterliche Gewalt&lt;/li&gt;&lt;li&gt;StGG über Regierungs- und Vollzugsgewalt&lt;/li&gt;&lt;li&gt;Delegationsgesetz&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welchen Geltungsbereich hatte die Verfassung von 1861 und welche die von 1867?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;1861: Gesamtstaat&lt;/li&gt;&lt;li&gt;1867: Cisleithanien&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Welche Verfassung wird durch die Dezemberverfassung von 1867 außer Kraft gesetzt? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Verfassung &lt;/strong&gt;von &lt;strong&gt;1861&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;ausdrückliche&lt;/strong&gt;, sondern nur &lt;strong&gt;materielle&lt;/strong&gt; &lt;strong&gt;Derogation&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;alte &lt;/strong&gt;Vorschriften &lt;strong&gt;nicht explizit&lt;/strong&gt; &lt;strong&gt;gestrichen &lt;/strong&gt;werden, sondern werden &lt;strong&gt;durch &lt;/strong&gt;die &lt;strong&gt;neuen unanwendbar&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nennen Sie markante Entwicklungsschritte für den Reichsrat und die Reichsratswahlen.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1867&lt;/strong&gt;: Änderung des GG über die Reichsvertretung&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1873&lt;/strong&gt;: Wahlrechtsreform und die Beendigung der Beschickung durch die Landtage&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1882&lt;/strong&gt;: Taaffesche Wahlrechtsreform und die Senkung des Zensus&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1896&lt;/strong&gt;: Badenische Wahlrechtsreform und die Erweiterung um eine 5. Kurie&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1907&lt;/strong&gt;: Beck’sche Wahlrechtsreform und das allgemeine Männerwahlrecht&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Trialismus?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Ein &lt;strong&gt;Schlagwort &lt;/strong&gt;in der &lt;strong&gt;Nationalitätenfrage &lt;/strong&gt;in der &lt;strong&gt;Doppelmonarchie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beide&lt;/strong&gt; &lt;strong&gt;Seiten &lt;/strong&gt;wollten jeweils eine &lt;strong&gt;andere Gruppe &lt;/strong&gt;als &lt;strong&gt;dritte Kraft im Staat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p class="ql-indent-1"&gt;&lt;strong&gt;Im Kern&lt;/strong&gt;: &lt;strong&gt;Erweiterung &lt;/strong&gt;der Doppelmonarchie um einen &lt;strong&gt;dritten Reichsteil&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die utraquistischen Schulen&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Bestimmte Unterrichtsgegenständen mussten in einer, und andere Gegenstände in der anderen Sprache unterrichtet werden&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die Monarchie auf Widerruf?&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Budget &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Wirtschaftspolitik&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;in &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;K. u. K Monarchie &lt;/strong&gt;benötigte &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;ständige&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Verhandlungen&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;zwischen&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Ö und U&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;und war vom &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Versuch &lt;/strong&gt;der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Aufrechterhaltung &lt;/strong&gt;einer &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;gemeinsamen&lt;/strong&gt; &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Wirtschaft &lt;/strong&gt;geprägt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Diese &lt;strong&gt;Verhandlungen &lt;/strong&gt;in &lt;strong&gt;Konferenzen &lt;/strong&gt;und &lt;strong&gt;Deputationen &lt;/strong&gt;waren oft Austragungsort von &lt;strong&gt;Machtdemonstrationen &lt;/strong&gt;und &lt;strong&gt;Einsatz von Druckmitteln &lt;/strong&gt;zur &lt;strong&gt;Lösung&lt;/strong&gt; &lt;strong&gt;diverser Konflikte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aufgrund des &lt;strong&gt;immanenten Konfliktpotentials &lt;/strong&gt;entstand die Bezeichnung "&lt;strong&gt;Monarchie&lt;/strong&gt; auf &lt;strong&gt;Widerruf&lt;/strong&gt;"&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind frühkonstitutionelle Elemente der Dezemberverfassung 1867?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Macht &lt;/strong&gt;beim &lt;strong&gt;Kaiser &lt;/strong&gt;konzentriert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;oberster Träger &lt;/strong&gt;von &lt;strong&gt;Regierungs &lt;/strong&gt;+ &lt;strong&gt;Vollzugsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;absolutes &lt;/strong&gt;Veto&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Herrenhaus &lt;/strong&gt;von &lt;strong&gt;Kaiser ernannt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Abgeordnetenhaus Ausschusslandtag &lt;/strong&gt;-&amp;gt; &lt;strong&gt;keine Volksvertretung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist der Panslawismus?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Streben &lt;/strong&gt;nach &lt;strong&gt;kulturellem&lt;/strong&gt; und &lt;strong&gt;politischem Zusammenschluss &lt;/strong&gt;aller &lt;strong&gt;slawischen&lt;/strong&gt; &lt;strong&gt;Völker&lt;/strong&gt;. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Zerschlagung &lt;/strong&gt;von &lt;strong&gt;Österreich-Ungarn&lt;/strong&gt;.&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer waren die Entente-Mächte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Frankreich&lt;/li&gt;&lt;li&gt;Russland&lt;/li&gt;&lt;li&gt;Großbritannien&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer war Teil der Mittelmächte?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;K+K&lt;/li&gt;&lt;li&gt;Deutsches Kaiserreich&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der eiserne Ring?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Regierung &lt;/strong&gt;unter Eduard Graf von &lt;strong&gt;Taaffe &lt;/strong&gt;bildete &lt;strong&gt;gestützt &lt;/strong&gt;auf &lt;strong&gt;feudale&lt;/strong&gt; &lt;strong&gt;Kreise&lt;/strong&gt; den&lt;strong&gt; Eisernen Ring, &lt;/strong&gt;ab &lt;strong style="background-color: rgb(230, 238, 248); color: rgb(51, 51, 51);"&gt;1879&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Suchte &lt;strong&gt;Annäherung &lt;/strong&gt;an die &lt;strong&gt;katholisch&lt;/strong&gt;-&lt;strong&gt;konservativen Rechten&lt;/strong&gt; im &lt;strong&gt;Parlament&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;neue &lt;strong&gt;Gesprächsbasis &lt;/strong&gt;mit &lt;strong&gt;österr&lt;/strong&gt;. &lt;strong&gt;Bischöfen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie hängen die Maigesetze von 1868 und das Konkordat von 1855 zusammen? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Maigesetze &lt;/strong&gt;von &lt;strong&gt;1868 &lt;/strong&gt;sowie damit &lt;strong&gt;verbundene&lt;/strong&gt; &lt;strong&gt;Änderungen&lt;/strong&gt; des &lt;strong&gt;ABGB beendeten &lt;/strong&gt;das &lt;strong&gt;Konkordat &lt;/strong&gt;von &lt;strong&gt;1855&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eherecht &lt;/strong&gt;für Katholiken &lt;strong&gt;wiederhergestellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehesachen&lt;/strong&gt; wieder &lt;strong&gt;weltlicher&lt;/strong&gt; &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;zugeordnet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notzivilehe&lt;/strong&gt;, wenn&lt;strong&gt; &lt;/strong&gt;Kirche &lt;strong&gt;Trauung verweigert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reaktion &lt;/strong&gt;der &lt;strong&gt;Bevölkerung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bürgerlich&lt;/strong&gt;-&lt;strong&gt;liberal&lt;/strong&gt;: &lt;strong&gt;Zustimmung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ländliche &lt;/strong&gt;Regionen: &lt;strong&gt;Kritik&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1874 weitere Maigesetze: Verhältnis &lt;/strong&gt;von &lt;strong&gt;Staat &lt;/strong&gt;und &lt;strong&gt;Kirche &lt;/strong&gt;weiter &lt;strong&gt;zugunsten&lt;/strong&gt; l&lt;strong&gt;iberaler Öffnung konkretisiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Katholikengesetz &lt;/strong&gt;zur Regelung der &lt;strong&gt;äußeren Rechtsverhältnisse &lt;/strong&gt;der &lt;strong&gt;Kirche &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Religionsfonds&lt;/strong&gt;gesetz &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anerkennungs&lt;/strong&gt;gesetz &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wodurch wurde der Konstitutionalismus geprägt? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ol&gt;&lt;li&gt;&lt;strong&gt;Parlamentarismus &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Massenparteien &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kampf&lt;/strong&gt; um ein &lt;strong&gt;allgemeines&lt;/strong&gt; &lt;strong&gt;Wahlrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nationale Forderungen &lt;/strong&gt;(größte &lt;strong&gt;Belastung &lt;/strong&gt;der &lt;strong&gt;Innenpolitik&lt;/strong&gt;)&lt;/li&gt;&lt;/ol&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist die pragmatische Sanktion? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Von &lt;strong&gt;Kaiser Karl VI&lt;/strong&gt; &lt;strong&gt;1713 &lt;/strong&gt;veröffentlichte Urkunde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unteilbarkeit &lt;/strong&gt;und &lt;strong&gt;Untrennbarkeit &lt;/strong&gt;der habsburgerischen &lt;strong&gt;Erbländer &lt;/strong&gt;-&amp;gt; &lt;strong&gt;einheitliche&lt;/strong&gt; &lt;strong&gt;Erbfolge&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;außenpolitische &lt;strong&gt;Vorgeschichte&lt;/strong&gt;: der &lt;strong&gt;Spanische Erbfolgekrieg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Spanische &lt;strong&gt;männliche Linie &lt;/strong&gt;ausgestorben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anspruch erhoben:  &lt;strong&gt;testamentarische Nachfolger Bourbone&lt;/strong&gt; &lt;strong&gt;Philipp von Anjou&lt;/strong&gt; sowie &lt;strong&gt;Habsburger Kaiser&lt;/strong&gt; &lt;strong&gt;Leopold I&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ging um &lt;strong&gt;Vorherrschaft &lt;/strong&gt;in &lt;strong&gt;Europa&lt;/strong&gt;: Entweder &lt;strong&gt;Habsburger&lt;/strong&gt; &lt;strong&gt;oder Frankreich&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Von wann bis wann bestand die konstitutionelle Doppelmonarchie? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Auch &lt;strong&gt;Konstitutionalismus &lt;/strong&gt;genannt&lt;/li&gt;&lt;li&gt;Von&lt;strong&gt; Ö-U Ausgleich 1867&lt;/strong&gt; bis Zusammenbruch nach 1. WK &lt;strong&gt;1918&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der aufgeklärte Absolutismus?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verbindung&lt;/strong&gt; von &lt;strong&gt;Absolutismus &lt;/strong&gt;und &lt;strong&gt;Aufklärung &lt;/strong&gt;im &lt;strong&gt;18. Jahrhundert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Herrscher &lt;/strong&gt;handeln &lt;strong&gt;nach Grundsätzen&lt;/strong&gt; der &lt;strong&gt;Vernunft &lt;/strong&gt;und zum &lt;strong&gt;Wohl &lt;/strong&gt;der &lt;strong&gt;Untertanen&lt;/strong&gt; und des &lt;strong&gt;Landes&lt;/strong&gt;, &lt;strong&gt;nicht &lt;/strong&gt;nach &lt;strong&gt;eigenem Willen&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reformen&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;soziale Missstände &lt;/strong&gt;beseitigen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Wissenschaft&lt;/strong&gt;, &lt;strong&gt;Kultur&lt;/strong&gt;, &lt;strong&gt;Bildung&lt;/strong&gt;, &lt;strong&gt;Handel &lt;/strong&gt;und &lt;strong&gt;Gewerbe&lt;/strong&gt; &lt;strong&gt;fördern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erster Diener des Staates&lt;/strong&gt; - Kontrast zum Gottesgnadendum &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;In Ö&lt;/strong&gt; vor allem gezeigt durch &lt;strong&gt;Toleranzpolitik Joseph &lt;/strong&gt;II.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Obwohl &lt;strong&gt;Liberalisierung&lt;/strong&gt; der &lt;strong&gt;Religionspolitik weniger &lt;/strong&gt;aus &lt;strong&gt;idealistischen Gründen&lt;/strong&gt;, &lt;strong&gt;eher&lt;/strong&gt; zur &lt;strong&gt;Steigerung &lt;/strong&gt;der &lt;strong&gt;Wirtschaftskraft&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Obstruktionspolitik?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Trotz&lt;/strong&gt; &lt;strong&gt;Betonung&lt;/strong&gt; der &lt;strong&gt;Landtage &lt;/strong&gt;und &lt;strong&gt;Zugeständnisse &lt;/strong&gt;des &lt;strong&gt;Monarchen&lt;/strong&gt;, &lt;strong&gt;verweigerten&lt;/strong&gt; die &lt;strong&gt;Ungarn &lt;/strong&gt;die &lt;strong&gt;Beschickung &lt;/strong&gt;des &lt;strong&gt;Reichsrates&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ungarischer Landtag &lt;/strong&gt;(auf &lt;strong&gt;Basis &lt;/strong&gt;von &lt;strong&gt;Februarpatent&lt;/strong&gt; 1861 &lt;strong&gt;gewählt&lt;/strong&gt;) &lt;strong&gt;lehnt Zentralparlament ab &lt;/strong&gt;-&amp;gt; fordert &lt;strong&gt;Rückkehr &lt;/strong&gt;zur &lt;strong&gt;revolutionären Verfassung&lt;/strong&gt; von &lt;strong&gt;1848&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kroatien &lt;/strong&gt;und &lt;strong&gt;Siebenbürgerische Rumänen erhoffen &lt;/strong&gt;sich durch &lt;strong&gt;Annäherung&lt;/strong&gt; an &lt;strong&gt;Ungarn&lt;/strong&gt; &lt;strong&gt;Vorteile&lt;/strong&gt;, und &lt;strong&gt;tragen Obstruktionspolitik&lt;/strong&gt; &lt;strong&gt;mit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Auf Dauer schrumpfte Reichsrat&lt;/strong&gt; (mangels Entsendung) auf &lt;strong&gt;Versammlung &lt;/strong&gt;von Politikern der &lt;strong&gt;deutschen Verfassungspartei&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Monarch&lt;/strong&gt; &lt;strong&gt;bevorzugt &lt;/strong&gt;dann &lt;strong&gt;staatliche&lt;/strong&gt; &lt;strong&gt;Neugestaltung&lt;/strong&gt;, &lt;strong&gt;statt Zentralismus &lt;/strong&gt;oder &lt;strong&gt;Föderalismus&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Dualismus &lt;/strong&gt;mit Ungarn&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1865 Erklärung an &lt;/strong&gt;seine &lt;strong&gt;Völker&lt;/strong&gt;: &lt;strong&gt;Enttäuschung &lt;/strong&gt;über &lt;strong&gt;Verweigerung &lt;/strong&gt;der Entsendung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Deshalb&lt;/strong&gt;: &lt;strong&gt;Überarbeitung &lt;/strong&gt;von &lt;strong&gt;Februarpatent notwendig &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sowie &lt;strong&gt;Verhandlungen &lt;/strong&gt;mit &lt;strong&gt;Landtagen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundgesetz &lt;/strong&gt;über die &lt;strong&gt;Reichsvertretung &lt;/strong&gt;wurde daher in allen &lt;strong&gt;Ländern sistiert &lt;/strong&gt;(&lt;strong&gt;stillgelegt&lt;/strong&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weil: &lt;strong&gt;Kann nicht gelten&lt;/strong&gt;, &lt;strong&gt;während &lt;/strong&gt;es in einem anderen Land &lt;strong&gt;verhandelt wird&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einigung &lt;/strong&gt;mit den &lt;strong&gt;Landtagen&lt;/strong&gt; &lt;strong&gt;verzögerte &lt;/strong&gt;sich aufgrund &lt;strong&gt;militärischer Niederlage &lt;/strong&gt;gegen &lt;strong&gt;Preußen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Faktisch &lt;/strong&gt;kehrte &lt;strong&gt;Franz Joseph &lt;/strong&gt;damit zu &lt;strong&gt;absolutistischer &lt;/strong&gt;Herrschaft zurück&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Wie war die Rolle der Grundrechte im Neoabsolutismus? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Grundrechte&lt;/strong&gt;/Grundfreiheiten &lt;strong&gt;von Bürgern &lt;/strong&gt;immer wieder &lt;strong&gt;durch Kaiser&lt;/strong&gt; &lt;strong&gt;betont&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber &lt;strong&gt;kein Katalog &lt;/strong&gt;aufgezählter Rechte, sondern &lt;strong&gt;eher Staatsziele &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Inhaltlich&lt;/strong&gt; entweder gar &lt;strong&gt;nicht garantiert&lt;/strong&gt;, &lt;strong&gt;oder &lt;/strong&gt;mittels &lt;strong&gt;einfacher&lt;/strong&gt; &lt;strong&gt;Gesetze&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Was war der Februarpatent von 1861? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Ausführungsgesetz &lt;/strong&gt;zum &lt;strong&gt;Oktoberdiplom&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Änderte das Oktoberdiplom &lt;strong&gt;inhaltlich weitgehend&lt;/strong&gt; &lt;strong&gt;ab&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kombination&lt;/strong&gt; der Beilagen (&lt;strong&gt;Grundgesetze&lt;/strong&gt; + &lt;strong&gt;Wahlordnungen&lt;/strong&gt;) wurde als &lt;strong&gt;Verfassung&lt;/strong&gt; &lt;strong&gt;verkündet&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erste Verfassung &lt;/strong&gt;seit &lt;strong&gt;1849&lt;/strong&gt;, aber nur auf &lt;strong&gt;Gesetzgebung bezogen &lt;/strong&gt;(keine anderen konstitutionellen Elemente)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zuständigkeit&lt;/strong&gt; der &lt;strong&gt;Landesgesetzgebung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Landesfinanzen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Der &lt;strong&gt;Landwirtschaft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Öffentliches &lt;strong&gt;Bauwesen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Weitere Aufgaben &lt;/strong&gt;konnten den Ländern zugewiesen werden, &lt;strong&gt;wenn&lt;/strong&gt; &lt;strong&gt;Landesinteressen berührt &lt;/strong&gt;wurden&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;Landtage &lt;/strong&gt;wurden aus &lt;strong&gt;4 Kurien&lt;/strong&gt; gewählt (Großgrundbesitz, Handel+Gewerbe, Städte+Märkte, Landgemeinden)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;hoher Steuerzensus &lt;/strong&gt;-&amp;gt; nur wohlhabende Schichten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abgeordnete &lt;strong&gt;deutscher&lt;/strong&gt; &lt;strong&gt;Nationalität&lt;/strong&gt; wurden &lt;strong&gt;gefördert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reichsvertretung&lt;/strong&gt;: &lt;strong&gt;Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Besteht aus: &lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Herrenhaus&lt;/strong&gt;: Adel + Kleriker, vom &lt;strong&gt;Kaiser &lt;/strong&gt;ernannt&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Abgeordnetenhaus&lt;/strong&gt;: Aus &lt;strong&gt;Landtagen &lt;/strong&gt;entsandt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vom &lt;strong&gt;Kaiser&lt;/strong&gt; &lt;strong&gt;einberufen &lt;/strong&gt;1x &lt;strong&gt;Jährlich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompetenzbereich &lt;/strong&gt;des Reichsrates &lt;strong&gt;bestätigt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beratende &lt;/strong&gt;Funktion zu &lt;strong&gt;beschließender Funktion &lt;/strong&gt;gewandelt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Abhängig von &lt;strong&gt;Sanktion &lt;/strong&gt;des &lt;strong&gt;Kaisers &lt;/strong&gt;(Veto)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Weitere&lt;/strong&gt; &lt;strong&gt;Reichsvertretung&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;engerer&lt;/strong&gt; &lt;strong&gt;Reichstag &lt;/strong&gt;für Angelegenheiten in &lt;strong&gt;nicht ungarische &lt;/strong&gt;Länder&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des &lt;strong&gt;Kaisers &lt;/strong&gt;(Gesetze ohne Reichstag)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Alleinige Entscheidungsmacht &lt;/strong&gt;des &lt;strong&gt;Kaises &lt;/strong&gt;in Agenden wie &lt;strong&gt;Äußeres&lt;/strong&gt;, &lt;strong&gt;Kriegswesen&lt;/strong&gt;, &lt;strong&gt;Religion&lt;/strong&gt;, &lt;strong&gt;Strafrecht &lt;/strong&gt;(&lt;em&gt;Prärogativen der Krone)&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Reichsrat?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;In &lt;strong&gt;Märzverfassung&lt;/strong&gt; &lt;strong&gt;1849 &lt;/strong&gt;vorgesehen &lt;strong&gt;Reichstag &lt;/strong&gt;wurde &lt;strong&gt;nie umgesetzt &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zeigte &lt;strong&gt;fehlenden Willen &lt;/strong&gt;des Kaisers für &lt;strong&gt;konstitutionell Staatsführung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ursprünglich &lt;/strong&gt;als &lt;strong&gt;Beratungsorgan &lt;/strong&gt;vorgesehener &lt;strong&gt;Reichsrat &lt;/strong&gt;wurde &lt;strong&gt;verfassungswidrig aufgewertet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;hatte &lt;strong&gt;kein Initiativrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Stattdessen &lt;/strong&gt;konnten &lt;strong&gt;Kaiser &lt;/strong&gt;und &lt;strong&gt;Minister &lt;/strong&gt;die Kompetenz des &lt;strong&gt;Reichsrates in Anspruch nehmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;durfte zur &lt;strong&gt;Vorbereitung &lt;/strong&gt;der &lt;strong&gt;Beratung &lt;/strong&gt;um &lt;strong&gt;Mitwirkung&lt;/strong&gt; der &lt;strong&gt;Minister ersuchen&lt;/strong&gt;, diese waren aber &lt;strong&gt;nicht verpflichtet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie gliederte sich die Gewerbeordnung im Neoabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Gewerbeordnung von &lt;strong&gt;1859&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zeigte weiten Bogen &lt;/strong&gt;zwischen &lt;strong&gt;konservativer&lt;/strong&gt; und &lt;strong&gt;liberaler&lt;/strong&gt; &lt;strong&gt;Legislative &lt;/strong&gt;auf, da sie die &lt;strong&gt;Zunftordnung aufhob.&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sollte &lt;strong&gt;Betriebsamkeit &lt;/strong&gt;erleichtern.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kompromiss. Zunächst &lt;/strong&gt;von &lt;strong&gt;beiden Seiten angefeindet&lt;/strong&gt;, aber &lt;strong&gt;zunehmend &lt;/strong&gt;mit &lt;strong&gt;Wohlwollen &lt;/strong&gt;begrüßt&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Inhalt:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Keine Rechtszersplitterung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Beseitigung &lt;/strong&gt;des &lt;strong&gt;Konzessionssystems&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Nicht alle &lt;/strong&gt;wurden &lt;strong&gt;gewerbefrei&lt;/strong&gt;, &lt;strong&gt;aber nur &lt;/strong&gt;noch &lt;strong&gt;14 &lt;/strong&gt;im &lt;strong&gt;Gesetz&lt;/strong&gt; &lt;strong&gt;taxativ aufgezählte &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kaum &lt;/strong&gt;noch &lt;strong&gt;gesetzliche Preisbindung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Arbeitsverhältnisse &lt;/strong&gt;(Lehrlinge etc.; freie Vereinbarkeit)&lt;/li&gt;&lt;li&gt;Erste &lt;strong&gt;Ansätze &lt;/strong&gt;von &lt;strong&gt;Arbeitnehmerschutz &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Genossenschaftswesen&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Kulturkampf in Österreich?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Befasst sich mit der &lt;strong&gt;öffentlichen Austragung&lt;/strong&gt; über die &lt;strong&gt;Kritik &lt;/strong&gt;am &lt;strong&gt;Konkordat von 1855&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Kritik&lt;strong&gt; aus bürgerlich-liberalen Kreise&lt;/strong&gt;n&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verstärkt&lt;/strong&gt; durch die &lt;strong&gt;Niederlage &lt;/strong&gt;von &lt;strong&gt;1859 &lt;/strong&gt;im Sardinischen Krieg (2. Ital. Unabhängigkeitskrieg)&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Machte &lt;strong&gt;Notwendigkeit staatlicher Reformen&lt;/strong&gt; klar&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Nach &lt;strong&gt;weiterer&lt;/strong&gt; &lt;strong&gt;Niederlage&lt;/strong&gt; &lt;strong&gt;1866 (&lt;em&gt;Königgrätz&lt;/em&gt;)&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;klar, dass &lt;strong&gt;reaktionäre&lt;/strong&gt; und &lt;strong&gt;klerikale Linie nicht&lt;/strong&gt; &lt;strong&gt;haltbar&lt;/strong&gt; ist&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;außenpolitischer Misserfolg &lt;/strong&gt;kann &lt;strong&gt;nicht mehr &lt;/strong&gt;hinter &lt;strong&gt;Beschützerrolle &lt;/strong&gt;für &lt;strong&gt;deutsches Katholikentum versteckt &lt;/strong&gt;werden &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung &lt;/strong&gt;versucht &lt;strong&gt;Heiligen&lt;/strong&gt; &lt;strong&gt;Stuhl &lt;/strong&gt;von einer Lösung zu &lt;strong&gt;überzeugen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Praktische&lt;/strong&gt; &lt;strong&gt;Abkehr &lt;/strong&gt;vom &lt;strong&gt;Konkordat 1867 &lt;/strong&gt;durch &lt;strong&gt;Festlegung &lt;/strong&gt;der &lt;strong&gt;Staatsbürgerrechte &lt;/strong&gt;und &lt;strong&gt;Bestimmungen&lt;/strong&gt; über die &lt;strong&gt;richterliche Gewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Vorrangstellung &lt;/strong&gt;der Kirche &lt;strong&gt;de facto unmöglich &lt;/strong&gt;gemacht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Maigesetzen &lt;/strong&gt;von &lt;strong&gt;1868&lt;/strong&gt; &lt;strong&gt;endgültig beendet&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war das handelspolitische Königgrätz? &lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Die &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Konkurrenz &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zwischen &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Österreich&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Preußen &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;fügte Österreich &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;schwere wirtschaftliche Schäden &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;zu.&amp;nbsp;&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Preußen&lt;/strong&gt; zwang &lt;strong&gt;Staaten&lt;/strong&gt; des &lt;strong&gt;Deutschen Bundes &lt;/strong&gt;ab &lt;strong&gt;1862&lt;/strong&gt; in &lt;strong&gt;Zollverein &lt;/strong&gt;mit &lt;strong&gt;Frankreich &lt;/strong&gt;und &lt;strong&gt;Großbritannien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Silvesterpatente von 1851?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;31.12.1851&lt;/strong&gt; vom Kaiser erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;endete&lt;/strong&gt; formell die &lt;strong&gt;frühkonstitutionelle &lt;/strong&gt;Phase →&lt;strong&gt; keine&lt;/strong&gt; &lt;strong&gt;Verfassung&lt;/strong&gt; mehr → &lt;strong&gt;Absolutismus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ol&gt;&lt;li&gt;Patent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Märzverfassung &lt;/strong&gt;von 1849 &lt;strong&gt;außer Kraft&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ausdrücklich&lt;/strong&gt; &lt;strong&gt;bestätigt:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Gleichheit &lt;/strong&gt;aller Bürger vor dem Gesetz&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Aufhebung&lt;/strong&gt; der &lt;strong&gt;Untertänigkeit&lt;/strong&gt; der &lt;strong&gt;Bauern&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Patent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aufhebung &lt;/strong&gt;des &lt;strong&gt;Grundrechtspatents &lt;/strong&gt;von &lt;strong&gt;1849&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;bestätigt &lt;/strong&gt;aber &lt;strong&gt;ausdrücklich religiöse Grundrechte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;allerhöchstes Kabinettsschreiben&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Schreiben &lt;/strong&gt;von Kaiser &lt;strong&gt;an Ministerpräsident Schwarzenberg&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;36 Grundsätze &lt;/strong&gt;für organisatorische Einrichtungen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Umstrukturierung &lt;/strong&gt;der &lt;strong&gt;internen Verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Machtkonzentration &lt;/strong&gt;auf den &lt;strong&gt;Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Jurisdiktion &lt;/strong&gt;und &lt;strong&gt;Grundrechtsschutz&lt;/strong&gt; &lt;strong&gt;untergraben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Mitbestimmung &lt;/strong&gt;des &lt;strong&gt;Volkes ausgeschlossen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Einzug &lt;/strong&gt;von &lt;strong&gt;organisatorischen Ebenen &lt;/strong&gt;in der &lt;strong&gt;Verwaltung &lt;/strong&gt;von Stadt, Kreis, Bezirks- und Länderebene → Verringerung der Länder- und Gemeindeautonomie&lt;/li&gt;&lt;/ol&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Justizreformen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Richter&lt;/strong&gt; und &lt;strong&gt;Justizbeamte nicht &lt;/strong&gt;mehr &lt;strong&gt;unabhängig &lt;/strong&gt;→ befolgen allgemeine Vorschriften für Staatsbeamte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Trennung &lt;/strong&gt;von &lt;strong&gt;Verwaltung&lt;/strong&gt; und &lt;strong&gt;Gerichtsbarkeit &lt;/strong&gt;in erster &lt;strong&gt;Instanz aufgehoben&lt;/strong&gt; → Bezirksämter Entscheiden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Strafprozess: &lt;strong&gt;Inquisitorisches &lt;/strong&gt;Verfahren und &lt;strong&gt;keine öffentlichen&lt;/strong&gt; &lt;strong&gt;Prozesse&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber:&lt;strong&gt; Geplant &lt;/strong&gt;möglichst &lt;strong&gt;schnell einheitliches Strafrecht &lt;/strong&gt;für alle &lt;strong&gt;Kronländer &lt;/strong&gt;zu schaffen, sowie &lt;strong&gt;ABGB&lt;/strong&gt; in allen &lt;strong&gt;Kronländern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zusammengefasst:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Rückkehr zu &lt;strong&gt;absoluter Monarchie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine&lt;/strong&gt; repräsentative &lt;strong&gt;Mitbestimmung &lt;/strong&gt;des&lt;strong&gt; Volkes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Länder&lt;/strong&gt;- und &lt;strong&gt;Gemeindeautonomie&lt;/strong&gt; &lt;strong&gt;zurückgedrängt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Justizreformen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Rückbau &lt;/strong&gt;von &lt;strong&gt;Grundrechten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist der Neoabsolutismus?&lt;/p&gt;&lt;ul&gt;&lt;li&gt;zeitliche Einordnung&lt;/li&gt;&lt;li&gt;Oktoberdiplom&lt;/li&gt;&lt;li&gt;Februarpatent&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1851-1867&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Genauer Beginn &lt;/strong&gt;hängt ab was als &lt;strong&gt;entscheidend angesehen &lt;/strong&gt;wird:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verfassungswirklichkeit 1851&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für Patente von April und August spricht: &lt;strong&gt;offener Widerspruch &lt;/strong&gt;zur &lt;strong&gt;Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für Silvesterpatente spricht: &lt;strong&gt;Heben &lt;/strong&gt;formell von &lt;strong&gt;Verfassung 1849 auf&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Oktroyierte Märzverfassung&lt;/strong&gt; &lt;strong&gt;1849&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Für diese spricht: wurde &lt;strong&gt;nie umgesetzt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Das Neue: &lt;strong&gt;Scheinkonstitutionelle &lt;/strong&gt;Elemente und teilweise &lt;strong&gt;inhaltlich liberale Gesetzgebung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;→ &lt;strong&gt;Absolutheit &lt;/strong&gt;der Herrschaftsmacht &lt;strong&gt;gemildert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Merkmale:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Zentralismus&lt;/strong&gt;, ab 1860 durch neuständische Elemente erweitert&lt;/li&gt;&lt;li&gt;Versuch &lt;strong&gt;Nationalitätskonflikt einzuschränken&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;deutsche Amtssprache&lt;/strong&gt;, &lt;strong&gt;Betonung &lt;/strong&gt;der &lt;strong&gt;Länder&lt;/strong&gt; und ihrer &lt;strong&gt;Verfassungen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Wichtig &lt;strong&gt;neben &lt;/strong&gt;dem &lt;strong&gt;Kaiser&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beamtentum&lt;/strong&gt;, &lt;strong&gt;Heer&lt;/strong&gt;, &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Oktoberdiplom 1860&lt;/strong&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reorganisation &lt;/strong&gt;- Neubesetzung zugunsten Militär und Adel, keine tatsächlichen Reformen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweitern &lt;/strong&gt;der &lt;strong&gt;Kompetenzen &lt;/strong&gt;für den &lt;strong&gt;Reichsrat &lt;/strong&gt;(Steuer, Anleihen)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Versuch Adel &lt;/strong&gt;vor allem in &lt;strong&gt;Ungarn&lt;/strong&gt;, auf &lt;strong&gt;Seite des Kaisers&lt;/strong&gt; zu bekommen&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Februarpatent 1861&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;erstes Abkommen &lt;/strong&gt;vom &lt;strong&gt;Neoabsolutismus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ausführungsgesetz &lt;/strong&gt;für &lt;strong&gt;Oktoberdiplom &lt;/strong&gt;-&amp;gt; aber &lt;strong&gt;wandelt ab&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Grundgesetz über Reichsvertretung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Landesordnungen&lt;/em&gt;/&lt;em&gt;Landtagswahlordnungen&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;→ als Verfassung verkündet&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Landtage &lt;/strong&gt;aus &lt;strong&gt;4 Kurien&lt;/strong&gt; mit &lt;strong&gt;Steuerzensus&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reichsrat &lt;/strong&gt;aus &lt;strong&gt;Herren&lt;/strong&gt;- &amp;amp; &lt;strong&gt;Abgeordnetenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Veto des Kaisers &lt;/strong&gt;bei Gesetzen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Notverordnungsrecht &lt;/strong&gt;des Kaisers (Gesetze&lt;strong&gt; ohne Reichsrat&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;→ &lt;strong&gt;Schein&lt;/strong&gt;konstitutionalismus: &lt;strong&gt;Keine Grundrechte&lt;/strong&gt;, aber wichtige liberale Anliegen umgesetzt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schutz der &lt;strong&gt;persönlichen Freiheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schutz des &lt;strong&gt;Hausrechts&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kaiser beruft&lt;/strong&gt; sich auch auf &lt;strong&gt;andere&lt;/strong&gt; &lt;strong&gt;Rechte &lt;/strong&gt;(&lt;em&gt;Gleichheit&lt;/em&gt;, &lt;em&gt;Religionsausübung&lt;/em&gt;, ...) aber &lt;strong&gt;nicht in Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;strong&gt;Endgültiges Ende&lt;/strong&gt;: &lt;strong&gt;&lt;em&gt;Dezemberverfassung &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;1867&lt;/em&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welche Rolle spielte die Kirche im Neoabsolutismus? (gedrucktes Canossa)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Konkordat&lt;/strong&gt; von &lt;strong&gt;1855 &lt;/strong&gt;um sich in Europa als &lt;strong&gt;katholische Großmacht &lt;/strong&gt;zu &lt;strong&gt;profilieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Erhoffte Prestigegewinn &lt;/strong&gt;bei &lt;strong&gt;katholischen Fürsten &lt;/strong&gt;im Deutschen Bund, als &lt;strong&gt;Gegengewicht&lt;/strong&gt; zu &lt;strong&gt;Preußen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schulterschluss mit Kirche &lt;/strong&gt;soll &lt;strong&gt;legitimatorische Mängel &lt;/strong&gt;des &lt;strong&gt;Reichszentralismus verstecken &lt;/strong&gt;und über &lt;strong&gt;fehlende &lt;/strong&gt;demokratische/&lt;strong&gt;konstitutionelle Legitimation hinwegtäuschen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Katholischer Klerus ursprünglich &lt;/strong&gt;für &lt;strong&gt;nationale Bewegungen&lt;/strong&gt;, erst &lt;strong&gt;nach Konkordat &lt;/strong&gt;für &lt;strong&gt;absolutistischen Gesamtstaat&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Durch &lt;strong&gt;betonten Katholizismus &lt;/strong&gt;sollen &lt;strong&gt;nationale&lt;/strong&gt; &lt;strong&gt;Interessen negiert &lt;/strong&gt;werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Länder &lt;/strong&gt;der Monarchie &lt;strong&gt;durch neue &lt;/strong&gt;Form des &lt;strong&gt;Patriotismus verbunden&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kirche &lt;/strong&gt;in der &lt;strong&gt;Ausgestaltung &lt;/strong&gt;des &lt;strong&gt;Glaubens freie Hand&lt;/strong&gt; gelassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Eheangelegenheiten &lt;/strong&gt;der &lt;strong&gt;kirchlichen Gerichtsbarkeit &lt;/strong&gt;vorbehalten&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wer war (im Neoabsolutismus) die Zentralfigur der öffentlichen Verwaltung?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Der &lt;strong&gt;Gendarm&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Dem &lt;strong&gt;Einfluss des Innenministers entzogen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Umfassende &lt;/strong&gt;Rechte an Gendarm &lt;strong&gt;übertragen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie ist &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;(im Neoabsolutismus)&lt;/span&gt; die Stellung des Reichsrates?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Militärische Niederlagen&lt;/strong&gt; und &lt;strong&gt;Widerstand &lt;/strong&gt;gegen &lt;strong&gt;Silvesterpatente 1851 &lt;/strong&gt;zwingen &lt;strong&gt;Kaiser&lt;/strong&gt; zum &lt;strong&gt;erneuten Eingriff &lt;/strong&gt;in &lt;strong&gt;Organisation &lt;/strong&gt;der &lt;strong&gt;Staatsgewalt&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Entgegen erwarteter innenpolitischer Wende erweitert &lt;/strong&gt;er mit &lt;strong&gt;Patent &lt;/strong&gt;von &lt;strong&gt;März 1860 &lt;/strong&gt;den &lt;strong&gt;Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;außerordentliche &lt;/strong&gt;Reichsräte&lt;/li&gt;&lt;li class="ql-indent-1"&gt;alle der &lt;strong&gt;Monarchie&lt;/strong&gt; &lt;strong&gt;wohlgesonnen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;= &lt;strong&gt;verstärkter Reichsrat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;Aufgaben:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Agenden &lt;/strong&gt;des &lt;strong&gt;Staatshaushaltes&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;allgemeine &lt;strong&gt;wichtige&lt;/strong&gt; &lt;strong&gt;Gesetzesangelegenheiten&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von &lt;strong&gt;Landtagen eingebrachte Vorlagen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Erneute Kompetenzerweiterung &lt;/strong&gt;im &lt;strong&gt;Juli 1860 &lt;/strong&gt;erlaubt &lt;strong&gt;Sanierung &lt;/strong&gt;des schwer verschuldeten &lt;strong&gt;Staatshaushaltes gegen &lt;/strong&gt;den &lt;strong&gt;Willen der Länder&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die Stützen von Franz Joseph im Neoabsolutismus?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Beamtentum&lt;/li&gt;&lt;li&gt;Heer&lt;/li&gt;&lt;li&gt;Kirche&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wie wurde die aufgezwungene Märzverfassung 1849 bezeichnet?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;Oktroyierte &lt;/strong&gt;Märzverfassung 1849&lt;/p&gt;</t>
+    <t>&lt;p&gt;Was war der Pfrimer Putsch?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;1931&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Heimwehrführer Pfrimer &lt;/strong&gt;versuchte &lt;strong&gt;Putsch &lt;/strong&gt;in der &lt;strong&gt;Steiermark&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Unter Eindruck der &lt;strong&gt;Weltwirtschaftskrise&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Scheiterte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber: weitere &lt;strong&gt;Schwächung &lt;/strong&gt;des &lt;strong&gt;Staates&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Pippinische Schenkung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;754&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Papst&lt;/strong&gt; bat Pippin III das röm. Volk von &lt;strong&gt;Langobarden &lt;/strong&gt;zu &lt;strong&gt;befreien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Pippin siegte&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Papst &lt;/strong&gt;erhält &lt;strong&gt;erobertes Land&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundlage &lt;/strong&gt;für &lt;strong&gt;Kirchenstaat &lt;/strong&gt;im MA&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Pax Dei?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gottesfrieden&lt;/strong&gt;, im &lt;strong&gt;11 Jhdt &lt;/strong&gt;von &lt;strong&gt;Kirche eingeführt&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Bestimmte &lt;strong&gt;Personen &lt;/strong&gt;(&lt;em&gt;Geistliche&lt;/em&gt;, &lt;em&gt;Waisen&lt;/em&gt;, &lt;em&gt;Frauen&lt;/em&gt;) und bestimmte &lt;strong&gt;Orte &lt;/strong&gt;(&lt;em&gt;Kirchen&lt;/em&gt;, &lt;em&gt;Klöster&lt;/em&gt;) waren vor &lt;strong&gt;Übergriffen &lt;/strong&gt;zu &lt;strong&gt;Schützen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verstoß&lt;/strong&gt;: &lt;em&gt;Kirchenstrafe &lt;/em&gt;oder &lt;em&gt;Exkommunikation&lt;/em&gt; (-&amp;gt; wirtschaftlicher und persönlicher Ruin)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der 1. Landfriede?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1103, &lt;/strong&gt;verhängt von &lt;strong&gt;Heinrich IV&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;4 jähriger Frieden&lt;/strong&gt; für ganzes Land &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eindämmung &lt;strong&gt;Faust- und Fehderecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verbot von Gewalt zur Durchsetzung eigener Ansprüche&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Landfriedengerichte&lt;/strong&gt;: &lt;strong&gt;Peinliche&lt;/strong&gt; &lt;strong&gt;Strafe&lt;/strong&gt; bei Widersetzung &lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Privilegium Minus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;1156&lt;/em&gt;, Frühestes &lt;/strong&gt;Ö &lt;strong&gt;Reichsdokument&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Urkunde &lt;/strong&gt;von &lt;strong&gt;Kaiser Friedrich I&lt;/strong&gt; an &lt;strong&gt;Herzog Heinrich II &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Personenverbandsstaat &lt;/strong&gt;zu &lt;strong&gt;Territorialstaat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö &lt;strong&gt;unabhängig&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Umwandlung &lt;strong&gt;Markgrafschaft Ostarrichi &lt;/strong&gt;in &lt;strong&gt;territoriales Herzogtum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Vorrechte &lt;/strong&gt;für Herzog&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Aufwertung &lt;/strong&gt;des &lt;strong&gt;Landesfürstentums&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reduktion &lt;/strong&gt;der &lt;strong&gt;Lehenspflichten &lt;/strong&gt;(-&amp;gt; &lt;em&gt;Hoffahrt &lt;/em&gt;nur nach &lt;em&gt;Bayern&lt;/em&gt;, &lt;em&gt;Heerfahrt &lt;/em&gt;nur in &lt;em&gt;Nachbarländer&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;weibliche Erbfolge &lt;/strong&gt;möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ad-hoc-Nachfolgeregelung &lt;/strong&gt;bei Kinderlosigkeit&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Oberster Gerichtsherr &lt;/strong&gt;(keine Ausübung der Gerichtsbarkeit ohne Zustimmung)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Sachsenspiegel?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1220&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Wichtigstes Rechtsbuch &lt;/strong&gt;des MA&lt;/li&gt;&lt;li&gt;&lt;strong&gt;König &lt;/strong&gt;gibt &lt;strong&gt;Land &lt;/strong&gt;und &lt;strong&gt;Ämter &lt;/strong&gt;and &lt;strong&gt;Kronvasallen&lt;/strong&gt;, diese geben weiter an &lt;strong&gt;Untervasallen &lt;/strong&gt;und diese zur Bearbeitung an &lt;strong&gt;unfreie&lt;/strong&gt; &lt;strong&gt;Bauern&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Heerschildsordnung&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;König&lt;/strong&gt;, &lt;strong&gt;geistliche&lt;/strong&gt; Fürsten, &lt;strong&gt;weltliche &lt;/strong&gt;Fürsten, &lt;strong&gt;freie &lt;/strong&gt;Herren, &lt;strong&gt;Lehensmannen &lt;/strong&gt;d. Freien, &lt;strong&gt;Lehensmannen &lt;/strong&gt;d. &lt;strong&gt;fünften &lt;/strong&gt;Heerschilds&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Hexenhammer?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1486&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Werk zur &lt;strong&gt;Legitimation &lt;/strong&gt;der &lt;strong&gt;Hexenverfolgung &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Beschrieb &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Wirkung&lt;/strong&gt; der &lt;strong&gt;Hexerei &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie &lt;strong&gt;Ausrottung &lt;/strong&gt;und &lt;strong&gt;Bestrafung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von Dominikanermönch &lt;strong&gt;Heinrich&lt;/strong&gt; &lt;strong&gt;Kramer &lt;/strong&gt;(Institoris)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Reichstag zu Worms? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1495&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Reichsreform &lt;/strong&gt;des hl. röm. Reich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;ewiger Landfriede&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ständiges &lt;strong&gt;Reichskammergericht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Exekutionsordnung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichssteuer&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Privilegium Maius?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1358 -&amp;gt;&lt;/strong&gt; &lt;strong&gt;Reaktion &lt;/strong&gt;auf Nicht-nennung in &lt;strong&gt;Goldener Bulle&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Fälschung &lt;/strong&gt;des &lt;strong&gt;Privilegium&lt;/strong&gt; &lt;strong&gt;Minus &lt;/strong&gt;mit weiteren &lt;strong&gt;Freiheitsbriefen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Ziele:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unabhängigkeit &lt;/strong&gt;der &lt;strong&gt;Habsburgerischen Länder von Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ehrenstellung &lt;/strong&gt;des Herzogs -&amp;gt; &lt;strong&gt;Erzherzog&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gleichstellung &lt;/strong&gt;mit &lt;strong&gt;Kurfürsten &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;weitere &lt;strong&gt;Reduktion &lt;/strong&gt;der &lt;strong&gt;Lehenspflichten&lt;/strong&gt;: &lt;strong&gt;keine Hoffahrt&lt;/strong&gt;, &lt;strong&gt;Heerfahrt&lt;/strong&gt; nur für &lt;strong&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Karl IV&lt;/strong&gt; &lt;strong&gt;verweigerte Anerkennung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erst im &lt;strong&gt;15 Jhdt &lt;/strong&gt;von &lt;strong&gt;Habsburger &lt;/strong&gt;röm. deutsch. König (dann Kaiser) &lt;strong&gt;Friedrich III &lt;/strong&gt;(für eigenes Haus) anerkannt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Vertrag zu Brüssel?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;1522&lt;/li&gt;&lt;li&gt;Nach Erbfolgestreit -&amp;gt; Aufteilung der Habsburger in spanische und österr. Linie&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Wormser Edikt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;Reichsacht &lt;/strong&gt;von Kaiser&lt;strong&gt; Karl V&lt;/strong&gt; gegen &lt;strong&gt;Martin&lt;/strong&gt; &lt;strong&gt;Luther 1521&lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die 95 Thesen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1517&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Martin &lt;strong&gt;Luther&lt;/strong&gt; -&amp;gt; primär gegen &lt;strong&gt;Ablasshandel&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Constitutio Criminalis Carolina?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1532&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Neue &lt;strong&gt;Strafrechtsordnung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Erlaubt &lt;strong&gt;Folter &lt;/strong&gt;und &lt;strong&gt;Todesstrafe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;-&amp;gt; &lt;strong&gt;Hexenprozesse&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Augsburger Interim?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1548&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Sieg von Kaiser &lt;strong&gt;Karl V über Protestanten &lt;/strong&gt;im &lt;strong&gt;Schmalkaldischen&lt;/strong&gt; Krieg&lt;/li&gt;&lt;li&gt;Eigene &lt;strong&gt;Reichsreligionsordnung &lt;/strong&gt;durch Kaiser &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Priesterehe &lt;/strong&gt;+ &lt;strong&gt;Laienkelch &lt;/strong&gt;gestattet&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Sonst &lt;/strong&gt;aber &lt;strong&gt;katholische Tradition&lt;/strong&gt; verbindlich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Reformationszeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1517-1648&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Spaltung&lt;/strong&gt; der &lt;strong&gt;Kirche ausgehend &lt;/strong&gt;von Martin &lt;strong&gt;Luther &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der 7 Jährige Krieg?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1756-1763&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Versuch &lt;strong&gt;Rückeroberung&lt;/strong&gt; &lt;strong&gt;Schelsiens &lt;/strong&gt;unter Maria Theresia&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Scheitert &lt;/strong&gt;-&amp;gt; &lt;strong&gt;schwächt&lt;/strong&gt; Staat&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Pariser Frieden?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1814&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Neuordnung Europas &lt;/strong&gt;durch 4 Siegermächte (&lt;strong&gt;Ö, RU, Preußen, England&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Karlsbader Beschlüsse?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1819&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ermordung von Schriftsteller &lt;/strong&gt;Kotzebue durch &lt;strong&gt;Burschenschafter &lt;/strong&gt;Karl Sand&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Metternich&lt;/strong&gt; &lt;strong&gt;behauptet&lt;/strong&gt; &lt;strong&gt;Umsturzversuch &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;4 Gesetze&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verbot &lt;/strong&gt;polit. &lt;strong&gt;Parteien&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abschaffung &lt;/strong&gt;Vereins- und &lt;strong&gt;Versammlungsfreiheit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwachte&lt;/strong&gt; &lt;strong&gt;Unis&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zensur &lt;/strong&gt;der &lt;strong&gt;Presse&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Welche Drei Revolutionen gab es in Wien 1848?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Märzerhebungen&lt;/strong&gt; &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Folge&lt;/strong&gt;: &lt;strong&gt;Pillersdorfer &lt;/strong&gt;Verfassung 1848&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Maiunruhen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Defizite &lt;/strong&gt;in &lt;strong&gt;Pillersd&lt;/strong&gt;. Verfassung (&lt;em&gt;fehlendes Stimmrecht &lt;/em&gt;für &lt;em&gt;Tage&lt;/em&gt;/&lt;em&gt;Wochenlöhner&lt;/em&gt;, &lt;em&gt;Dienstboten&lt;/em&gt;, ... )&lt;/li&gt;&lt;li&gt;Oktobererhebung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ermodung Kriegsminister&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Verlegung Reichstag &lt;/strong&gt;nach Kremsier&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;blutig Niedergeschlagen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die "Frage an Österreich"?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nov 1848&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Durch &lt;strong&gt;Revolution Machtverschiebung &lt;/strong&gt;in Ländern des &lt;strong&gt;dt. Bundes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bund soll &lt;strong&gt;konstitutioneller Bundesstaat &lt;/strong&gt;werden&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Großdeutsche Lösung&lt;/strong&gt;: Umfasst &lt;strong&gt;alle deutschsprachigen&lt;/strong&gt; &lt;strong&gt;Gebiete&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;hätte Teilung Ös erfordert&lt;/strong&gt; wegen Mehrheiten von &lt;strong&gt;Nationalitäten in Ö Kronländern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: &lt;strong&gt;Unteilbarkeit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Also wurde &lt;strong&gt;kleindeutsche Lösung ohne Ö&lt;/strong&gt; verfolgt&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Märzpatent?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1860&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erweiterung&lt;/strong&gt; des &lt;strong&gt;Reichsrats&lt;/strong&gt;: &lt;strong&gt;verstärkter &lt;/strong&gt;Reichsrat&lt;/li&gt;&lt;li&gt;neue &lt;strong&gt;Kompetenz&lt;/strong&gt;: &lt;strong&gt;Beratung &lt;/strong&gt;bei &lt;strong&gt;Gesetzgebungsangelegenheiten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Sistierungspatent?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1865&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Neuverhandlung &lt;/strong&gt;des &lt;strong&gt;Silvesterpatents 1861 &lt;/strong&gt;mit &lt;strong&gt;Landtagen &lt;/strong&gt;von &lt;strong&gt;Ungarn &lt;/strong&gt;und &lt;strong&gt;Kroatien&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Dafür &lt;strong&gt;Sistierung &lt;/strong&gt;(&lt;strong&gt;Unterbrechung&lt;/strong&gt;) des &lt;strong&gt;&lt;em&gt;GG &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;über Reichsvertretung&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Zweibund?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1872&lt;/strong&gt; - &lt;strong&gt;Bündnis &lt;/strong&gt;mit &lt;strong&gt;Preußen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Besetzung &lt;/strong&gt;und &lt;strong&gt;Verwaltung Bosniens&lt;/strong&gt; und &lt;strong&gt;Herzegowinas &lt;/strong&gt;durch &lt;strong&gt;Ö&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was passierte 1905/6?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;nach &lt;strong&gt;Badenischer Sprachenverordnung &lt;/strong&gt;(zweite &lt;strong&gt;Amtsprache&lt;/strong&gt; &lt;strong&gt;Tschechisch &lt;/strong&gt;für Beamte) &lt;/li&gt;&lt;li&gt;-&amp;gt; &lt;strong&gt;Ausschreitungen &lt;/strong&gt;(&lt;strong&gt;Zustrom tschechischer&lt;/strong&gt; &lt;strong&gt;Beamter &lt;/strong&gt;in deutschen Gebieten &lt;strong&gt;befürchtet&lt;/strong&gt;)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was passierte 1893?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Regierung &lt;/strong&gt;legt &lt;strong&gt;Entwurf &lt;/strong&gt;für &lt;strong&gt;Wahlverordnung &lt;/strong&gt;des &lt;strong&gt;Abgeordnetenhauses &lt;/strong&gt;Vor&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Allgemeines Wahlrecht ohne Zensus&lt;/strong&gt; in Kurien der &lt;strong&gt;Stadt&lt;/strong&gt;- und &lt;strong&gt;Landgemeinden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Folge: &lt;strong&gt;Amtsenthebung &lt;/strong&gt;der Regierung &lt;strong&gt;Taafe&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das 14-Punkte Programm?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1918 &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von amerikanischem Präsident &lt;strong&gt;Wilson&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Grundzüge&lt;/strong&gt; einer &lt;strong&gt;Friedensordnung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Völkerbund?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Gegründet &lt;strong&gt;1920&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;58 Mitglieder - &lt;strong&gt;Friedenssicherung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren die Lausanner Protokolle? &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;em&gt;1932&lt;/em&gt;&lt;/li&gt;&lt;li&gt;Neuerlicher &lt;strong&gt;Kredit &lt;/strong&gt;vom &lt;strong&gt;Völkerbund &lt;/strong&gt;an Ö, Höhe&lt;strong&gt; 300 Mio Schilling&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verweis &lt;/strong&gt;auf &lt;strong&gt;Genfer &lt;/strong&gt;Protokolle: &lt;strong&gt;Verzicht &lt;/strong&gt;auf &lt;strong&gt;Anschluss&lt;/strong&gt; an Deutsches Reich&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Novemberpogrom?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1938&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;17j Jude&lt;/strong&gt; &lt;strong&gt;tötet &lt;/strong&gt;aus &lt;strong&gt;Rache Botschaftssekräter &lt;/strong&gt;in Paris&lt;/li&gt;&lt;li class="ql-indent-1"&gt;"&lt;em&gt;endgültiger Beweis für j. Weltverschwörung&lt;/em&gt;"&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Göbbels&lt;/strong&gt; ordnet &lt;strong&gt;Racheaktion &lt;/strong&gt;an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Pogrome &lt;/strong&gt;im &lt;strong&gt;gesamten &lt;/strong&gt;Reich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zusätzlich per &lt;strong&gt;VO Sühneleistung &lt;/strong&gt;von &lt;strong&gt;1 Mrd Reichsmark von dt. Juden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Danach&lt;/strong&gt;: systematische &lt;strong&gt;Deportation&lt;/strong&gt; von &lt;strong&gt;Juden&lt;/strong&gt; in &lt;strong&gt;KZ&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Ermächtigungsgesetz/Aktion T4&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;1939&lt;/li&gt;&lt;li&gt;Euthanasieprogramm &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Methodische Tötung "unwerten" Lebens&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Geisteskranke, Alte, chronisch Kranke&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Ottonisch-Salische Reichskirchensystem?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;bis &lt;strong&gt;1000 &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Um &lt;strong&gt;Einfluss &lt;/strong&gt;der &lt;strong&gt;Stammesherzogtümer&lt;/strong&gt; zu &lt;strong&gt;reduzieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kirche &lt;/strong&gt;als &lt;strong&gt;Gegengewicht &lt;/strong&gt;in &lt;strong&gt;Reichsverfassung &lt;/strong&gt;eingebaut&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bischöfe &lt;/strong&gt;wurden "&lt;strong&gt;Reichsbeamte&lt;/strong&gt;" und &lt;strong&gt;stützten&lt;/strong&gt; &lt;strong&gt;König&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Aufgebaut&lt;strong&gt; &lt;/strong&gt;von &lt;strong&gt;Otto I &lt;/strong&gt;durch &lt;strong&gt;Schenkungen&lt;/strong&gt; an die &lt;strong&gt;Kirche&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;dem kam zugute: &lt;strong&gt;keine Erblichkeit &lt;/strong&gt;bei Geistlichen -&amp;gt; &lt;strong&gt;Lehen &lt;/strong&gt;können nach Ableben &lt;strong&gt;erneut&lt;/strong&gt; &lt;strong&gt;vergeben &lt;/strong&gt;werden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Personalhoheit&lt;/strong&gt; bei &lt;strong&gt;Bischofswahlen &lt;/strong&gt;(&lt;strong&gt;&lt;em&gt;Laieninvestitur&lt;/em&gt;&lt;/strong&gt;)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unzufriedenheit &lt;/strong&gt;in Kirche darüber führte zu &lt;strong&gt;Investiturstreit&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war ein Lehen?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;ein &lt;strong&gt;weltliches&lt;/strong&gt; &lt;strong&gt;Gut&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stück &lt;strong&gt;Land&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;politisches &lt;strong&gt;Amt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Recht &lt;/strong&gt;(&lt;em&gt;fischen&lt;/em&gt;, &lt;em&gt;jagen&lt;/em&gt;, Steuern eintreiben) oder andere &lt;strong&gt;Werte &lt;/strong&gt;von &lt;strong&gt;erheblicher&lt;/strong&gt; &lt;strong&gt;Dauer&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von &lt;strong&gt;Lehnsherr &lt;/strong&gt;(Eigentümer) an &lt;strong&gt;Lehensmann &lt;/strong&gt;gegeben &lt;/li&gt;&lt;li class="ql-indent-1"&gt;meist &lt;strong&gt;erblich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;An &lt;strong&gt;Bedingungen &lt;/strong&gt;geknüpft - z.B. &lt;strong&gt;Treueversprechen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was waren Hierokratismus und Dualismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beschreiben das &lt;strong&gt;Verhältnis &lt;/strong&gt;zwischen &lt;strong&gt;geistlicher &lt;/strong&gt;(&lt;em&gt;sacerdotium&lt;/em&gt;) und &lt;strong&gt;weltlicher &lt;/strong&gt;(&lt;em&gt;regnum&lt;/em&gt;) &lt;strong&gt;Gewalt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;siehe auch &lt;strong&gt;Zweischwertgleichnis&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dualismus&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;weltliche Macht&lt;/strong&gt; hat ein &lt;strong&gt;selbständiges&lt;/strong&gt; &lt;strong&gt;Recht &lt;/strong&gt;mit &lt;strong&gt;Pflicht zur Kooperation&lt;/strong&gt; mit der geistlichen&lt;/li&gt;&lt;li&gt;&lt;em&gt;Hierokratismus&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;die &lt;strong&gt;weltliche Macht&lt;/strong&gt; wird &lt;strong&gt;von &lt;/strong&gt;der &lt;strong&gt;geistlichen &lt;/strong&gt;Macht &lt;strong&gt;absorbiert&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;der &lt;strong&gt;Kaiser&lt;/strong&gt; ist also &lt;strong&gt;nur&lt;/strong&gt; ein &lt;strong&gt;Beauftragter&lt;/strong&gt; des &lt;strong&gt;Papstes&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das Zweischwertergleichnis?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;allegorische&lt;/strong&gt; &lt;strong&gt;Auslegung &lt;/strong&gt;der Begriffe Hierokratismus und Dualismus&lt;/li&gt;&lt;li&gt;&lt;em style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Hierokratismus &lt;/em&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Schwabenspiegel&lt;/strong&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;)&lt;/span&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Gott gibt &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;beide Schwerter&lt;/strong&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt; (weltlich+geistlich) an &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Papst&lt;/strong&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;, Papst gibt das &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;weltliche&lt;/strong&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;weiter&lt;/strong&gt;&lt;span style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt; an den &lt;/span&gt;&lt;strong style="color: rgb(171, 127, 242); background-color: rgb(40, 45, 88);"&gt;Kaiser&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiser muss&lt;/strong&gt; also Papst &lt;strong&gt;folgen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Dualismus &lt;/em&gt;(&lt;strong&gt;Sachsenspiegel&lt;/strong&gt;):&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gott &lt;/strong&gt;gibt &lt;strong&gt;beiden Machtträgern&lt;/strong&gt; unmittelbar&lt;strong&gt; je ein Schwert&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Stellung der Landtage in der frühen Neuzeit?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Herzstück landständischer&lt;/strong&gt; &lt;strong&gt;Autonomie&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Landesfürst &lt;/strong&gt;musste &lt;strong&gt;wirtschaftliche&lt;/strong&gt; und &lt;strong&gt;gesellschaftliche&lt;/strong&gt; &lt;strong&gt;Verhältnisse&lt;/strong&gt; im Land &lt;strong&gt;verhandeln&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;v. a. in&lt;strong&gt;&lt;em&gt; &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;finanziellen &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Krisen&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zustimmung&lt;/strong&gt; der &lt;strong&gt;Landesstände &lt;/strong&gt;über &lt;strong&gt;Art &lt;/strong&gt;und &lt;strong&gt;Ausmaß &lt;/strong&gt;der &lt;strong&gt;aufzubringenden Mittel &lt;/strong&gt;notwendig&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wie entwickelten sich die Landstände?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Landesherren versuchten &lt;/strong&gt;stets &lt;strong&gt;Landesherrschaft auszubauen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Landsässige &lt;/strong&gt;&lt;em&gt;Herren&lt;/em&gt;, &lt;em&gt;Ritter&lt;/em&gt;, &lt;em&gt;Städte&lt;/em&gt;, ... versuchten ihre &lt;strong&gt;politische&lt;/strong&gt; &lt;strong&gt;Autonomie &lt;/strong&gt;zu &lt;strong&gt;Sichern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Zusammenschlüsse  entwickelten &lt;/strong&gt;sich zu &lt;strong&gt;organisierten&lt;/strong&gt; &lt;strong&gt;Verbänden&lt;/strong&gt; -&amp;gt; den &lt;em&gt;Landständen&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Deutsche Bund / die Deutsche Bundesakte &lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;1815 Einigung &lt;/strong&gt;über dt. &lt;strong&gt;Bundesakte&lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;40 souveräne Staaten&lt;/li&gt;&lt;li&gt;&lt;em&gt;Gründen Deutschen Bund&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Ziel&lt;/em&gt;:&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Erhaltung &lt;strong&gt;äußerer &lt;/strong&gt;und &lt;strong&gt;innerer Sicherheit&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Unabhängigkeit&lt;/strong&gt; und &lt;strong&gt;Unverletzbarkeit &lt;/strong&gt;der einzelnen Staaten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Zweck&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Konzept der &lt;strong&gt;dynastischen Legitimität&lt;/strong&gt;: Erhaltung des &lt;strong&gt;Absolutismus&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Organe&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Bundestag (&lt;em&gt;Bundesversammlung&lt;/em&gt;)&lt;/strong&gt;: &lt;strong&gt;Beschlussfassendes &lt;/strong&gt;Organ&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gesandten &lt;/strong&gt;der Mitgliedsländer&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ö hat Vorsitz&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gemeinsame &lt;/strong&gt;Bundes&lt;strong&gt;verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;aber &lt;strong&gt;keine Bundesjustiz &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Untergang&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Machtverschiebungen &lt;/strong&gt;nach Revolutionsjahr &lt;strong&gt;1848&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;1866 &lt;/em&gt;&lt;strong&gt;Niederlage &lt;/strong&gt;Ö gegen Preußen in Schlacht von &lt;strong&gt;Königgrätz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö &lt;strong&gt;muss Auflösung zustimmen&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Gegner Ös gründen &lt;strong&gt;Norddeutschen &lt;/strong&gt;Bund&lt;/li&gt;&lt;li&gt;&lt;em&gt;1871 &lt;/em&gt;&lt;strong&gt;deutsche&lt;/strong&gt; &lt;strong&gt;Einigung &lt;/strong&gt;-&amp;gt; Gründung des &lt;strong&gt;dt. Reichs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Verurteilung der Geschwister Scholl?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Widerstandsgruppe "&lt;strong&gt;Die weiße Rose&lt;/strong&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;bestand aus &lt;strong&gt;Studierenden&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Flugblätter &lt;/strong&gt;zu wahrem &lt;strong&gt;Charakter &lt;/strong&gt;des &lt;strong&gt;Nationalsozialismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Widerstandsaufrufe&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verurteilt &lt;/strong&gt;vor &lt;strong&gt;Volksgerichtshof&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;1943 hingerichtet &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war das B-VG 1920&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;em&gt;Oktober 1920&lt;/em&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Inhalt&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;föderalistischer &lt;/strong&gt;Bundesstaat&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Gesetzgebung&lt;/strong&gt; nach Grundsätzen &lt;strong&gt;mittelbarer Demokratie&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;allgemeines&lt;/em&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;,&lt;/span&gt; &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;gleiches&lt;/em&gt;, &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;geheimes &lt;/em&gt;und &lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;direktes&lt;/em&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;em&gt;Verhältni&lt;/em&gt;swahlrecht&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;NR &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;wählte &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;BReg &lt;/strong&gt;und konnte sie &lt;strong&gt;entheben&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Kompetenzkompetenz &lt;/strong&gt;beim Bund&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Gerichtsbarkeit Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Rest aufgeteilt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Generalklausel für Länder&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Geprägt &lt;/strong&gt;von Prinzip der &lt;strong&gt;Rechtsstaatlichkeit&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Legalitätsprinzip &lt;/strong&gt;-&amp;gt; staatl. Verwaltung nur aufgrund der Gesetze&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Keine Einigung&lt;/em&gt;&lt;em&gt; &lt;/em&gt;bei &lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Grundrechten&lt;/span&gt; -&amp;gt; daher von &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;1867 übernommen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Josephinismus?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Reformen &lt;/strong&gt;Joseph II im &lt;strong&gt;18 JH&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Setzte Reformen von &lt;strong&gt;Maria Theresia fort&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;andere Anschauungen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Reformen als &lt;strong&gt;Aufklärerisch angesehen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;nicht ideologisch &lt;/strong&gt;inspiriert&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem aber: Nach Gesichtspunkten der &lt;strong&gt;Nützlichkeit für den Staat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Anschluss?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Im &lt;em&gt;März 1938&lt;/em&gt;: &lt;strong&gt;Machtzunahme &lt;/strong&gt;der &lt;strong&gt;Nationalsozialisten &lt;/strong&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;nachdem &lt;strong&gt;Seyß-Inquart Innenminister&lt;/strong&gt; wurde (Berchtesgadener Abkommen)&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Schuschnigg &lt;/strong&gt;kündigt als &lt;strong&gt;letztes&lt;/strong&gt; &lt;strong&gt;Mittel Volksabstimmung &lt;/strong&gt;über &lt;strong&gt;Unabhängigkeit &lt;/strong&gt;an&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Unternehmen Otto&lt;/em&gt;: plant &lt;strong&gt;Einmarsch &lt;/strong&gt;der &lt;strong&gt;deutschen &lt;/strong&gt;Truppen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ultimatum &lt;/strong&gt;Hitlers an &lt;strong&gt;Schuschnigg &lt;/strong&gt;für Rücktritt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schuschnigg &lt;strong&gt;gibt nach&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Seyß-Inquart&lt;/strong&gt; wurde &lt;strong&gt;Bundeskanzler&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einmarsch &lt;/strong&gt;der Truppen begann am&lt;strong&gt; selben Tag&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Seyß-Inquart unterzeichnet „&lt;em&gt;Gesetz über Wiedervereinigung Österreichs mit dem Deutschen Reich&lt;/em&gt;“&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war der Staatsgerichtshof, was das Reichsgericht?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;Beide &lt;strong&gt;1867 eingerichtet&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;&lt;em&gt;Staatsgerichtshof&lt;/em&gt;&lt;/strong&gt;: Für &lt;strong&gt;Ministeranklage&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Reichsgericht&lt;/em&gt;: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;vor allem &lt;strong&gt;Kompetenzkonflikte &lt;/strong&gt;zw &lt;strong&gt;Gerichten &lt;/strong&gt;und &lt;strong&gt;Verwaltungsbehörden &lt;/strong&gt;und zw &lt;strong&gt;Länder&lt;/strong&gt; und &lt;strong&gt;Regierung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;deklaratorische&lt;/strong&gt; &lt;strong&gt;Prüfung&lt;/strong&gt; der &lt;strong&gt;Gesetze &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Heilige Allianz?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nach &lt;/strong&gt;dem &lt;strong&gt;Wiener Kongress &lt;em&gt;1815&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;wurde der Deutsche Bund gegründet&lt;/li&gt;&lt;li&gt;Zusätzlich &lt;strong&gt;Gründung der Hl. Allianz&lt;/strong&gt;: &lt;em&gt;Russland, Preußen, Österreich&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;gegenseitiger Schutz &lt;/strong&gt;vor &lt;strong&gt;Revolutionen &lt;/strong&gt;im jeweiligen Land&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Wann wurde der Schilling eingeführt?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;strong&gt;1.1.1925 &lt;/strong&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was war die Pillersdorfersche Verfassung?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Kontext&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Entstand unter Druck der &lt;strong&gt;Märzrevolution 1848&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Inhaltlich &lt;strong&gt;Innenminister Pillersdorf verantwortlich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Erlassen &lt;/em&gt;im &lt;em&gt;April&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Novelle &lt;/em&gt;im &lt;em&gt;Mai&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em&gt;Aufgehoben Juni&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;em&gt;Inhalt&lt;/em&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Früh&lt;/strong&gt;konstitutionell&lt;/li&gt;&lt;li&gt;&lt;em&gt;Gesetzgebung&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;em&gt;tag&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Senat &lt;/strong&gt;+ &lt;strong&gt;Abgeordnetenhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;kein &lt;/strong&gt;Selbstversammlungsrecht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Absolutes &lt;/strong&gt;Veto des Kaisers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kein Notverordnungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Wahlrecht&lt;/em&gt;: &lt;strong&gt;Wahlmänner&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;keine&lt;/strong&gt; &lt;strong&gt;Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Gerichtsbarkeit&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Öffentlichkeit &lt;/strong&gt;+ &lt;strong&gt;Mündlichkeit &lt;/strong&gt;der Verfahren&lt;/li&gt;&lt;li&gt;&lt;em&gt;Grundrechte&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht durchsetzbar &lt;/strong&gt;-&amp;gt; nur &lt;strong&gt;Staatsziele&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Geltungsbereich&lt;/em&gt;: &lt;strong&gt;nicht &lt;/strong&gt;für &lt;strong&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
   <si>
     <t>&lt;p&gt;Was ist der Kremsierer Entwurf?&amp;nbsp;&lt;/p&gt;</t>
   </si>
   <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Blutige Unruhen&lt;/strong&gt; infolge der &lt;strong&gt;Ermordung &lt;/strong&gt;des &lt;strong&gt;Kriegsministers&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiserlicher &lt;/strong&gt;Hof nach &lt;strong&gt;Olmütz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichstag &lt;/strong&gt;nach &lt;strong&gt;Kremsier&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;um &lt;strong&gt;Einfluss &lt;/strong&gt;der &lt;strong&gt;Revolution &lt;/strong&gt;zu &lt;strong&gt;fliehen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Durch erste &lt;strong&gt;Erfolge&lt;/strong&gt; der &lt;strong&gt;Gegenrevolution rückte &lt;/strong&gt;Franz Josef von der ursprünglich &lt;strong&gt;konstitutionsfreundlichen &lt;/strong&gt;Linie &lt;strong&gt;ab&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiser löste März 1849 &lt;/strong&gt;Kremsierer &lt;strong&gt;Reichstag &lt;/strong&gt;auf&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Bevor&lt;/strong&gt; &lt;strong&gt;Verfassungsentwurf verabschiedet &lt;/strong&gt;werden konnte&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Nach Auflösung &lt;/strong&gt;des Reichstags erließ der &lt;strong&gt;Kaiser &lt;/strong&gt;eine &lt;strong&gt;eigene Verfassung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Oktroyierte &lt;/strong&gt;(aufgezwungene) &lt;strong&gt;Märzverfassung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die Pillersdorfsche Verfassung?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Märzrevolution 1848 &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Studenten&lt;/strong&gt; + &lt;strong&gt;Bürger &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Petition &lt;/strong&gt;an Kaiser für überfällige &lt;strong&gt;Reformen &lt;/strong&gt;wie &lt;strong&gt;Aufhebung der Zensur&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Demonstranten stürmen &lt;/strong&gt;nach Enttäuschung über Behandlung durch &lt;strong&gt;NÖ Landtag &lt;/strong&gt;das &lt;strong&gt;Landhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Staatsmacht &lt;/strong&gt;versucht &lt;strong&gt;Metternichs&lt;/strong&gt; &lt;strong&gt;Repressionspolitik&lt;/strong&gt; aufrechtzuerhalten -&amp;gt; &lt;strong&gt;direkter&lt;/strong&gt; &lt;strong&gt;Widerspruch &lt;/strong&gt;zu den &lt;strong&gt;Forderungen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Nachdem &lt;strong&gt;Arbeiter &lt;/strong&gt;sich dem &lt;strong&gt;Protest&lt;/strong&gt; &lt;strong&gt;angeschlossen &lt;/strong&gt;haben -&amp;gt; &lt;strong&gt;Druck &lt;/strong&gt;auf &lt;strong&gt;Kaiser &lt;/strong&gt;steigt -&amp;gt; bringt &lt;strong&gt;Metternich &lt;/strong&gt;zum &lt;strong&gt;Rücktritt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kaiser &lt;/strong&gt;verspricht Konstitution zu erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Beteiligung &lt;/strong&gt;des &lt;strong&gt;Bürgertums &lt;/strong&gt;in Form von Beratungen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Innenminister Franz Freiherr von Pillersdorf &lt;/strong&gt;konzipiert &lt;strong&gt;Verfassung &lt;/strong&gt;nach &lt;strong&gt;belgischem&lt;/strong&gt; &lt;strong&gt;Vorbild&lt;/strong&gt;.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Verfassung &lt;/strong&gt;vom &lt;strong&gt;Kaiser &lt;/strong&gt;am 25. &lt;strong&gt;April&lt;/strong&gt; &lt;strong&gt;1848 &lt;/strong&gt;in Kraft gesetzt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bereits &lt;strong&gt;im Mai &lt;/strong&gt;zum &lt;strong&gt;Provisorium erklärt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Im&lt;strong&gt; Juni zurückgenommen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Frühkonstitutionelle &lt;/strong&gt;Elemente:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verfassung oktroyiert (aufgezwungen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Senat/Oberhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kein Selbstversammlungsrecht&lt;/strong&gt; des Parlaments&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Absolutes Vetorecht &lt;/strong&gt;des Monarchen -&amp;gt; Zentraler Träger der Staatsgewalten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine Trennung &lt;/strong&gt;von &lt;strong&gt;Gesetzgebung &lt;/strong&gt;und &lt;strong&gt;Vollziehung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Konstitutionelle Elemente:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Abgeordnetenhaus &lt;/strong&gt;mit &lt;strong&gt;Wahlberechtigung &lt;/strong&gt;ab 24. Lebensjahr &lt;strong&gt;ohne Steuerzensus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Parlament &lt;/strong&gt;hat &lt;strong&gt;Gesetzesinitiative&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unabhängige Richter&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Grundrechtskatalog&amp;nbsp;&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war der Rheinbund? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1806&lt;/strong&gt;: Zusammenschluss von &lt;strong&gt;16 deutschen Fürsten&lt;/strong&gt; unter dem &lt;strong&gt;Protektorat Napoleons&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit Gründung des Staatenbundes &lt;strong&gt;Austritt aus Hl. Röm Reich Deutscher Nation&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Rheinbund blieb &lt;/strong&gt;faktisch ein &lt;strong&gt;militärisches Zweckbündnis &lt;/strong&gt;zwischen &lt;strong&gt;Rheinbundstaaten&lt;/strong&gt; und &lt;strong&gt;Napoleons Frankreich&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ausbau in &lt;strong&gt;Bundesstaat &lt;/strong&gt;mit gemeinsamen Organen &lt;strong&gt;scheitert &lt;/strong&gt;am &lt;strong&gt;Widerstand &lt;/strong&gt;der Mitglieder&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Ende &lt;strong&gt;1813 &lt;/strong&gt;nach &lt;strong&gt;Niederlage Napoleons &lt;/strong&gt;in &lt;strong&gt;Völkerschlacht&lt;/strong&gt; &lt;strong&gt;bei Leipzig&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der &lt;strong&gt;deutsche Bund&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Wie &lt;strong&gt;handelte &lt;/strong&gt;er? &lt;/p&gt;&lt;p&gt;Wann &lt;strong&gt;ging &lt;/strong&gt;er &lt;strong&gt;unter&lt;/strong&gt;? &lt;/p&gt;&lt;p&gt;Wann kann es zur &lt;strong&gt;Einigung&lt;/strong&gt;?&amp;nbsp;&lt;/p&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1804 &lt;/strong&gt;erklärte sich &lt;strong&gt;Franz II &lt;/strong&gt;unter Eindruck der Kaiserkrönung Napoleons zum&lt;strong&gt; Kaiser von Österreich&lt;/strong&gt;, da er einen Machtverlust im Hl. Röm. Reich antizipierte.&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Juli 1806&lt;/strong&gt;: &lt;strong&gt;Rheinbund &lt;/strong&gt;zwischen 16 deutsche Fürsten unter Protektorat Napoleons geschlossen.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;August 1806&lt;/strong&gt;: &lt;strong&gt;Napoleon fordert Niederlegung &lt;/strong&gt;der &lt;strong&gt;Kaiserkrone des Hl. Röm. Reichs &lt;/strong&gt;von Franz II -&amp;gt; &lt;strong&gt;Franz II kommt dem nach &lt;/strong&gt;-&amp;gt; Bleibt aber Kaiser von Ö!&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit Niederlegung des Kaiseramts:&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Entbindung &lt;/strong&gt;der &lt;strong&gt;Reichsstände &lt;/strong&gt;vom &lt;strong&gt;Reich &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Institutionelles&lt;/strong&gt; &lt;strong&gt;Ende &lt;/strong&gt;des &lt;strong&gt;HRRDN &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Rechtlich &lt;/strong&gt;war das Ende&lt;strong&gt; unzulässig&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-3"&gt;Erfordert &lt;strong&gt;Abdankung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-3"&gt;Erfordert &lt;strong&gt;Einbindung &lt;/strong&gt;des &lt;strong&gt;Reichstages&lt;/strong&gt;/der &lt;strong&gt;Kurfürsten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Folge: &lt;strong&gt;de facto&lt;/strong&gt; Untergang, aber &lt;strong&gt;nicht&lt;em&gt; &lt;/em&gt;&lt;/strong&gt;&lt;em&gt;de iure&lt;/em&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Juni &lt;strong&gt;1815&lt;/strong&gt;: Einigung über &lt;strong&gt;deutsche Bundesakte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Völkerrechtlicher Vertrag &lt;/strong&gt;zwischen &lt;strong&gt;40 souveränen&lt;/strong&gt; &lt;strong&gt;Staaten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Begründete &lt;/strong&gt;den &lt;strong&gt;Deutschen Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sowohl &lt;strong&gt;Bund &lt;/strong&gt;als &lt;strong&gt;Gliedstaaten &lt;/strong&gt;waren &lt;strong&gt;selbständige Völkerrechtssubjekte &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kein Rechtsnachfolger &lt;/strong&gt;des &lt;strong&gt;HRRDN &lt;/strong&gt;oder des &lt;strong&gt;Rheinbundes&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;originäre Gründung &lt;/strong&gt;mit dem &lt;strong&gt;Ziel restaurative Beschlüsse &lt;/strong&gt;des Wiener Kongresses &lt;strong&gt;umzusetzen &lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Handlung:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Erster &lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;verfassungsrechtlicher &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Grundsatz (&lt;em&gt;Wiener Schlussakte&lt;/em&gt;):&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; &lt;/span&gt;Erhaltung der &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;äußeren&lt;/strong&gt;&lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt; und &lt;/span&gt;&lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;inneren Sicherheit Deutschlands&lt;/strong&gt;, &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Unabhängigkeit&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;und &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Unverletzlichkeit &lt;/strong&gt;der einzelnen &lt;span style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;deutschen&lt;/span&gt; &lt;strong style="color: rgb(56, 190, 155); background-color: rgba(0, 0, 0, 0);"&gt;Staaten&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;beschlussfähiges &lt;/strong&gt;Organ: &lt;strong&gt;Bundestag &lt;/strong&gt;aus Gesandten der Mitgliedsländer, &lt;strong&gt;Vorsitz hatte Ö&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Keine&lt;/strong&gt; gemeinsame &lt;strong&gt;Bundesjustiz&lt;/strong&gt;, nur &lt;strong&gt;gemeinsame Verwaltung&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;politisches&lt;strong&gt; &lt;/strong&gt;Konzept&lt;strong&gt;: dynastische Legitimität -&amp;gt; Absolutismus &lt;/strong&gt;einzige &lt;strong&gt;legitime Staatsform&lt;/strong&gt; im Bund&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Vorbereitung des Untergangs:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolution 1848 &lt;/strong&gt;-&amp;gt; revolutionäre Verwerfungen -&amp;gt; &lt;strong&gt;Vorparlamente&lt;/strong&gt; und &lt;strong&gt;Verfassungen &lt;/strong&gt;in manchen Gliedstaaten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Bund &lt;strong&gt;bestand de iure&lt;/strong&gt; &lt;strong&gt;weiter&lt;/strong&gt;, überlebte Revolution -&amp;gt; Versuch der &lt;strong&gt;Auflösung &lt;/strong&gt;durch &lt;strong&gt;Erzherzog Johann scheitert &lt;/strong&gt;an Gliedstaaten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1850&lt;/strong&gt;: &lt;strong&gt;Ö&lt;/strong&gt; versucht Bund in &lt;strong&gt;ursprünglicher Gestalt &lt;/strong&gt;wiederherzustellen -&amp;gt; &lt;strong&gt;scheitert &lt;/strong&gt;an integration aller Länder&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Preußen verhinderten &lt;/strong&gt;selbst "überlebenswichtige" &lt;strong&gt;Organisationsreformen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Untergang &lt;em&gt;1866&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Niederlage&lt;/strong&gt; &lt;strong&gt;Ö&lt;/strong&gt; gegen Preußen in &lt;strong&gt;Schlacht von Königgrätz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ende &lt;/strong&gt;des deutschen Bundes&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ö muss Auflösung zustimmen&lt;/strong&gt; -&amp;gt; Ende der Wiener Schlussakte&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Einigung &lt;em&gt;1871&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vorher: Gegner Ös gründen &lt;strong&gt;norddeutschen&lt;/strong&gt; &lt;strong&gt;Bund&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Daraus 1871 &lt;strong&gt;deutsche Einigung &lt;/strong&gt;-&amp;gt; Gründung des &lt;strong&gt;Deutschen Reichs&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Reichsdeputationshauptschluss?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Abfindung &lt;/strong&gt;der &lt;strong&gt;weltlichen &lt;/strong&gt;Fürsten für &lt;strong&gt;linksrheinische Gebietsverluste &lt;/strong&gt;an&lt;strong&gt; Frankreich&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Geschah durch:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Säkularisation kirchlicher &lt;/strong&gt;Herrschaften&lt;/li&gt;&lt;li class="ql-indent-1"&gt;und &lt;strong&gt;Mediatisierung&lt;/strong&gt; &lt;strong&gt;kleinerer&lt;/strong&gt; &lt;strong&gt;weltlicher &lt;/strong&gt;Herrschaften &lt;/li&gt;&lt;li class="ql-indent-1"&gt;bisheriger Reichsstände &lt;strong&gt;rechts&lt;/strong&gt; &lt;strong&gt;des  Rheins&lt;/strong&gt; &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Mediatisierung?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;"&lt;strong&gt;Mittelbarmachung&lt;/strong&gt;" im Hl. Röm Reich&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Verlust der selbständigen Herrschaft&lt;/strong&gt; (&lt;em&gt;Souveränität&lt;/em&gt;) der Grafen und Fürsten, v.A. kleinerer Reichsstände&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Unterordnung &lt;/strong&gt;unter &lt;strong&gt;größere Territorien&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was wurde auf dem Wiener Kongress geregelt?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;territoriale &lt;/strong&gt;und &lt;strong&gt;politische&lt;/strong&gt; &lt;strong&gt;Neuordnung Kontinentaleuropas&lt;/strong&gt;. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;revolutionären Bestrebungen &lt;/strong&gt;+ &lt;strong&gt;napoleonischen Kriege &lt;/strong&gt;-&amp;gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;&lt;em&gt;kleinere&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;&lt;strong&gt;&lt;em&gt;Mächte&lt;/em&gt;&lt;/strong&gt;&lt;em&gt; &lt;/em&gt;untergegangen, &lt;em&gt;Europa &lt;/em&gt;in &lt;em&gt;Chaos&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nach &lt;strong&gt;Niederlage Napoleons&lt;/strong&gt;: &lt;strong&gt;Aufteilung &lt;/strong&gt;der Gebiete unter Siegermächten.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Zur Lösung: &lt;strong&gt;Wiener Kongress &lt;/strong&gt;unter &lt;strong&gt;Leitung&lt;/strong&gt; &lt;strong&gt;Metternichs &lt;/strong&gt;von &lt;strong&gt;November 1814 bis Juni 1815&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Neben territorialer Neuordnung &lt;strong&gt;auch&lt;/strong&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionäre Ideen &lt;/strong&gt;(Freiheit, Gleichheit, Brüderlichkeit) &lt;strong&gt;klein &lt;/strong&gt;halten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Absolutistische Machtgefüge stabilisieren &lt;/strong&gt;/ neu aufbauen.&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Auseinandersetzung mit Gedankengut &lt;/strong&gt;der Aufklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Aber mit &lt;strong&gt;Ziel&lt;/strong&gt; des &lt;strong&gt;Neuaufbaus &lt;/strong&gt;des &lt;strong&gt;Absolutismus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;strong&gt;Verwerfen &lt;/strong&gt;der &lt;strong&gt;Ziele &lt;/strong&gt;und &lt;strong&gt;Methoden &lt;/strong&gt;der Revolution&lt;/li&gt;&lt;li class="ql-indent-1"&gt;-&amp;gt; &lt;strong&gt;freiwillige Übernahme &lt;/strong&gt;weniger &lt;strong&gt;Resultate &lt;/strong&gt;um erneute &lt;strong&gt;Revolution &lt;/strong&gt;zu &lt;strong&gt;verhindern&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Aber: &lt;strong&gt;Erstes Mal &lt;/strong&gt;"&lt;em&gt;europäischer Gedanke&lt;/em&gt;"&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Lösung&lt;/strong&gt; der Probleme &lt;strong&gt;durch Gemeinschaft &lt;/strong&gt;/ &lt;strong&gt;Zusammenhelfen &lt;/strong&gt;der &lt;strong&gt;Staaten&lt;/strong&gt;/Königshäuser&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was waren die innenpolitischen Folgen der Jakobinerprozesse?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Aufdeckung der Verschwörung&lt;/strong&gt; gemeinsam mit &lt;strong&gt;Hinrichtung Ludwig XVI und Marie Antionette &lt;/strong&gt;führte endgültig zu &lt;strong&gt;reaktionärer Linie&lt;/strong&gt; Franz II&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Hetze &lt;/strong&gt;gegen alle, die &lt;strong&gt;nicht seiner Meinung &lt;/strong&gt;folgten&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Intellektuelle &lt;/strong&gt;und &lt;strong&gt;Beamte&lt;/strong&gt; denen man &lt;strong&gt;Sympathie für&lt;/strong&gt; &lt;strong&gt;Aufklärung &lt;/strong&gt;nachsagte -&amp;gt; aus &lt;strong&gt;öffentlichem Leben entfernt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Revolutionäre Propaganda&lt;/strong&gt; und &lt;strong&gt;Geheimbünde verboten&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Jakobinerprozesse &lt;/strong&gt;waren eine &lt;strong&gt;Bruchstelle &lt;/strong&gt;in der &lt;strong&gt;aufgeklärten&lt;/strong&gt; &lt;strong&gt;Entwicklung der Ö. Politik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anpassung &lt;/strong&gt;des Strafrechts &lt;strong&gt;ermöglichte Todesstrafe&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;1795 &lt;/strong&gt;neue &lt;strong&gt;General-Zensurverordnung&lt;/strong&gt; um &lt;strong&gt;öffentliche Meinungsbildung &lt;/strong&gt;zu &lt;strong&gt;beeinflussen&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was ist das Toleranzpatent von Joseph II? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Am 13.10.&lt;strong&gt;1781&lt;/strong&gt; von&lt;strong&gt; Joseph II&lt;/strong&gt; für Ö erlassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur&lt;strong&gt; eines von vielen&lt;/strong&gt;, da die &lt;strong&gt;Maßnahmen &lt;/strong&gt;auch &lt;strong&gt;Länderweise erlassen &lt;/strong&gt;werden mussten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Betraf:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;evangelische Bekenntnisse &lt;/strong&gt;(&lt;em&gt;Augsburgerisch &lt;/em&gt;und &lt;em&gt;Helvetisch&lt;/em&gt;)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;nicht unierte&lt;/strong&gt;, &lt;strong&gt;orthodoxe &lt;/strong&gt;Christen&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Erlaubt &lt;/strong&gt;wurde&lt;/li&gt;&lt;li class="ql-indent-1"&gt;das &lt;strong&gt;Privatexercicium &lt;/strong&gt;(nicht-öffentliche Religionsausübung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Errichtung &lt;/strong&gt;von &lt;strong&gt;Bethäusern &lt;/strong&gt;und &lt;strong&gt;Kirchen&lt;/strong&gt;, solange &lt;strong&gt;nicht nach außen als solche erkennbar&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Weitere &lt;strong&gt;Ausübung &lt;/strong&gt;und &lt;strong&gt;regulative Eingriffe &lt;/strong&gt;in &lt;strong&gt;Ausgstaltung&lt;/strong&gt; der &lt;strong&gt;Religion &lt;/strong&gt;wurden unter &lt;strong&gt;staatliche Aufsicht &lt;/strong&gt;gestellt, z.B.: die &lt;strong&gt;Schulmeister&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Juden&lt;/strong&gt; waren &lt;strong&gt;nicht umfasst&lt;/strong&gt;, wurden a&lt;strong&gt;ber besser gestellt&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Niederlassung &lt;/strong&gt;in &lt;strong&gt;Gemeinden &lt;/strong&gt;die ihnen bisher verboten waren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zugang zu vielen &lt;strong&gt;Gewerben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Möglichkeit des &lt;strong&gt;Studiums&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Joseph &lt;/strong&gt;II verstand (gegenüber kath. Kirche) sich als &lt;strong&gt;oberster&lt;/strong&gt; &lt;strong&gt;Kirchenherr &lt;/strong&gt;des Staates&lt;/li&gt;&lt;li class="ql-indent-1"&gt;wollte &lt;strong&gt;staatliche Verwaltung &lt;/strong&gt;und &lt;strong&gt;Kontrolle &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;= Josephinisches Staatskirchentum&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Gründe &lt;/strong&gt;für Toleranzpatent:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nur &lt;strong&gt;teilweise &lt;/strong&gt;aus &lt;strong&gt;liberaler&lt;/strong&gt; &lt;strong&gt;religiöser Haltung &lt;/strong&gt;von Joseph II&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;vielmehr&lt;/strong&gt;: &lt;strong&gt;wirtschaftliche Wachstumschancen &lt;/strong&gt;durch Anpassungen&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Beseitigung &lt;/strong&gt;des &lt;strong&gt;kirchlichen Einflusses &lt;/strong&gt;auf die &lt;strong&gt;Ehe&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Auflösung &lt;/strong&gt;von &lt;strong&gt;Klöstern &lt;/strong&gt;die sich&lt;strong&gt; nicht Unterricht, Krankenpflege, Landwirtschaft oder Gewerbe &lt;/strong&gt;widmeten&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Das &lt;strong&gt;Vermögen &lt;/strong&gt;ging in &lt;strong&gt;Religionsfond&lt;/strong&gt;, der die &lt;strong&gt;Pfarren &lt;/strong&gt;&lt;strong style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;finanzierte &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;und &lt;/span&gt;bis ins 20. Jahrhundert bestand&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was war die Jakobinerverschwörung?&amp;nbsp;&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;1793/1794&amp;nbsp;&lt;/strong&gt;formierten sich in Ö die &lt;strong&gt;Jakobiner&lt;/strong&gt; aus &lt;strong&gt;Schriftstellern&lt;/strong&gt;, &lt;strong&gt;Intellektuellen &lt;/strong&gt;und &lt;strong&gt;Beamten &lt;/strong&gt;die &lt;strong&gt;Joseph II &lt;/strong&gt;und &lt;strong&gt;Leopold II wohlgesonnen &lt;/strong&gt;gegenüberstanden&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem &lt;strong&gt;diejenigen&lt;/strong&gt;, die an den &lt;strong&gt;Reformen &lt;/strong&gt;von &lt;strong&gt;Joseph II mitgewirkt &lt;/strong&gt;haben und von der &lt;strong&gt;Restaurationspolitik&lt;/strong&gt; &lt;strong&gt;von Franz II enttäuscht&lt;/strong&gt; waren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Sie organisierten sich im &lt;strong&gt;geheimen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Standen im &lt;strong&gt;Austausch mit französischen&lt;/strong&gt; Jakobinern&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Die &lt;strong&gt;Komplotte &lt;/strong&gt;kamen aber&lt;strong&gt; nie zur Ausführung&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Die &lt;strong&gt;österr&lt;/strong&gt;. &lt;strong&gt;Jakobiner &lt;/strong&gt;versuchten (anders als Josephinismus) die &lt;strong&gt;Revolution&lt;/strong&gt; &lt;strong&gt;von Unten &lt;/strong&gt;(mittels unterer Gesellschaftsschichten) vorzubereiten&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Auch in &lt;strong&gt;Ungarn &lt;/strong&gt;gab es eine &lt;strong&gt;Bewegung &lt;/strong&gt;für &lt;strong&gt;politisch-soziale Reformen im Habsburgerreich&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;sowie für &lt;strong&gt;nationale Unabhängigkeit&lt;/strong&gt; &lt;strong&gt;Ungarns&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;von &lt;strong&gt;Machtübernahme &lt;/strong&gt;durch &lt;strong&gt;Franz II &lt;/strong&gt;enttäuscht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;→ Forderungen radikaler: vollständige Umgestaltung der Gesellschaft&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der &lt;span style="background-color: rgb(255, 255, 255); color: rgba(0, 0, 0, 0.87);"&gt;Pauperismus?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;Verelendung &lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;großer &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;Bevölkerungsteile &lt;/strong&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;unmittelbar &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;vor der Industrialisierung &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;zunehmender Verarmung &lt;/span&gt;&lt;strong style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 36);"&gt;vor allem der Arbeiterschicht&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was versteht man unter der Stagnation im Vormärz und was erhofften sich die Menschen und worin wurden sie enttäuscht? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Vormärz: &lt;strong&gt;1792 &lt;/strong&gt;bis &lt;strong&gt;1848 &lt;/strong&gt;- &lt;strong&gt;Französische Revolution &lt;/strong&gt;bis &lt;strong&gt;Märzrevolution&lt;/strong&gt;.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Motivation der franz. Revolution: Befreiung von autoritären Herrschern, Einkehr der Grundsätze der Aufklärung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;In Ö gaben sich &lt;strong&gt;Joseph II und Leopold II&lt;/strong&gt; als &lt;strong&gt;aufgeklärt &lt;/strong&gt;und konnten sich mit &lt;strong&gt;Teilen &lt;/strong&gt;der &lt;strong&gt;revolutionären Ideen identifizieren&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Franz II&lt;/strong&gt; - &lt;strong&gt;Gegner der Revolution&lt;/strong&gt; und der &lt;strong&gt;innerstaatlichen&lt;/strong&gt; &lt;strong&gt;Öffnungstendenzen seiner Vorgänger&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Mit &lt;strong&gt;Amtsantritt &lt;/strong&gt;startete &lt;strong&gt;Stagnation &lt;/strong&gt;(Ende der Zeit der Reformen)&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Striktes Festhalten an der &lt;strong&gt;monarchischen Legitimität &lt;/strong&gt;zur &lt;strong&gt;Unterdrückung liberaler, konstitutioneller &lt;/strong&gt;und &lt;strong&gt;nationaler Bewegungen &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Österreich als &lt;strong&gt;Obrigkeits&lt;/strong&gt;-, &lt;strong&gt;Zensur&lt;/strong&gt;-, &lt;strong&gt;Überwachungsstaat&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Der &lt;strong&gt;Reformzeit&lt;/strong&gt; unter Joseph II und Leopold II &lt;strong&gt;folgte&lt;/strong&gt; also der &lt;strong&gt;Vormärz &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Vor allem die &lt;strong&gt;Neuordnung&lt;/strong&gt; &lt;strong&gt;Europas &lt;/strong&gt;am &lt;strong&gt;Wiener&lt;/strong&gt; &lt;strong&gt;Kongress 1815 &lt;/strong&gt;mit &lt;strong&gt;Metternich's Stabilitätssystem (U&lt;/strong&gt;nterdrückung der&lt;strong&gt; &lt;/strong&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Demokratie, Presse-, Meinungs- und Versammlungsfreiheit&lt;/span&gt;&lt;strong&gt;) &lt;/strong&gt;prägte die Zeit bis zur Revolution 1848 &lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Worin wurden die Leute enttäuscht?&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung der autoritären&lt;/strong&gt; &lt;strong&gt;Strukturen&lt;/strong&gt; und &lt;strong&gt;Einführung eines Verfassungsstaates&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung&lt;/strong&gt; des &lt;strong&gt;Pauperismus &lt;/strong&gt;und des &lt;strong&gt;Massenelends&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Überwindung &lt;/strong&gt;der &lt;strong&gt;drangsalierenden Auflagen&lt;/strong&gt;, die durch das &lt;strong&gt;Metternichsche Stabilitätssystem &lt;/strong&gt;über ganz Europa lagen&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war der Zollunionsplan?&amp;nbsp;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;ab &lt;strong&gt;1929 &lt;/strong&gt;wurde die Schaffung eines&lt;strong&gt; einheitlichen deutsch-österreichischen Zoll- und Wirtschaftsgebietes &lt;/strong&gt;gefordert.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Von Deutscher Seite als Reaktion auf &lt;strong&gt;französischen Vorschlag eines europäischen Staatenbundes &lt;/strong&gt;vertreten.&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Eine solche europ. Verbindung hätte den &lt;strong&gt;politischen und territorialen Status der europ. Staaten festgesetzt &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Ende der Deutschen Revisions- und Großmachtpolitk&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Um dies zu verhindern: &lt;strong&gt;Deutschland&lt;/strong&gt; strebt &lt;strong&gt;Großmachtstellung &lt;/strong&gt;an, &lt;strong&gt;Ö als Sprungbrett&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Geheime Verhandlungen&lt;/strong&gt; werden &lt;strong&gt;publik&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;französische Regierung sieht&lt;strong&gt; Zollunion als Vorstufe des Anschlusses&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Stellt  Ö ein &lt;strong&gt;Ultimatum&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;IGH in Den Haag entscheidet: &lt;/li&gt;&lt;li class="ql-indent-1"&gt;Zollunion &lt;strong&gt;nicht gegen Anschlussverbot&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber &lt;strong&gt;gegen Genfer Protokolle&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Als &lt;strong&gt;1931 &lt;/strong&gt;zur &lt;strong&gt;politischen Krise &lt;/strong&gt;die &lt;strong&gt;Bankenkrise &lt;/strong&gt;kam, &lt;strong&gt;verzichtete &lt;/strong&gt;Ö auf den Plan.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Was sind die Genfer-Protokolle? &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Österreichische Wirtschaft konnte Strukturprobleme infolge des 1. Weltkriegs nicht bewältigen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Konnte sich nicht an neue Gegebenheiten anpassen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö blieb &lt;strong&gt;Agrar&lt;/strong&gt;/&lt;strong&gt;Industriestaat&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;ökonomische Stabilisierung nicht möglich&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Andauernde&lt;/strong&gt; &lt;strong&gt;Inflation &lt;/strong&gt;-&amp;gt; &lt;strong&gt;Ö vor Zusammenbruch&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Situation der Bürger ebenfalls stetig verschlechternd&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Regierung reduziert Steuern&lt;/li&gt;&lt;li&gt;Regierung will &lt;strong&gt;Auslandskredite &lt;/strong&gt;nehmen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Andere &lt;strong&gt;Nationalbanken verweigern&lt;/strong&gt; aufgrund der &lt;strong&gt;Abwertung &lt;/strong&gt;der Ö Währung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Ö an Völkerbund verwiesen&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Ententmächte &lt;/strong&gt;von Seipel &lt;strong&gt;überzeugt&lt;/strong&gt; von negativen Folgen von &lt;strong&gt;politischer Instabilität&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Anleihen: &lt;strong&gt;650 Mio Goldkronen&lt;/strong&gt; vom Völkerbund&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Verbürgt von &lt;strong&gt;England,&lt;/strong&gt; &lt;strong&gt;Italien, Tschechoslovakei, Frankreich&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Drei Genfer Protokolle&lt;/strong&gt; legen &lt;strong&gt;Bedingungen der&lt;/strong&gt; &lt;strong&gt;Anleihe &lt;/strong&gt;fest:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erneute Verpflichtung von Ö zur&lt;strong&gt; Unabhängigkeit iSd Vertrag von St Germain&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anschlussverbot &lt;/strong&gt;bekräftigt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;20 Jahre&lt;/strong&gt; &lt;strong&gt;keine &lt;/strong&gt;finanzielle/wirtschaftliche Verpflichtungen die &lt;strong&gt;Unabhängigkeit konterkarieren&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Austerityprogramm &lt;/strong&gt;zur Sanierung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Kontrolle durch Generalkommissar &lt;/strong&gt;rund &lt;strong&gt;Kontrollkommitee&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Regierung &lt;/strong&gt;durch Verfassungsänderung &lt;strong&gt;bevollmächtigt&lt;/strong&gt;, &lt;strong&gt;Sanierungsmaßnahmen &lt;/strong&gt;auch &lt;strong&gt;ohne Parlament &lt;/strong&gt;durchführen zu können&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;Durchführung des Sanierungsprogramms durch das sog. &lt;strong&gt;Wiederaufbaugesetz: &lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verwaltungs&lt;strong&gt;reform&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Einsparungsmaßnahmen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Einnahmeerhöhung durch &lt;strong&gt;Steuern&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Insgesamt&lt;strong&gt;:&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Entscheidende &lt;strong&gt;Beschränkungen&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Geringe Investitionsausgaben&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;Rücksichtslose &lt;strong&gt;Ausgabenreduktion&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;1924 &lt;/strong&gt;Einführung des&lt;strong&gt; Schillings&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Weltwirtschaftskrise &lt;/strong&gt;Ende der &lt;strong&gt;1920er &lt;/strong&gt;taucht Problem &lt;strong&gt;erneut &lt;/strong&gt;auf. &lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Lausanner Protokolle&lt;/strong&gt; mit Verweis auf Genfer Protokolle durchgesetzt&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Nahezu &lt;strong&gt;dasselbe&lt;/strong&gt; &lt;strong&gt;Programm &lt;/strong&gt;in Höhe von &lt;strong&gt;300 Mio Schilling&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Welchen Zeitraum umfasst das Mittelalter?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;500-1500 n. Chr.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die 5 Inhalte des Privilegium &lt;strong&gt;Minus&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Beibehaltung des Herzogstitel&lt;/strong&gt; und damit Umwandlung der Mark Österreich in ein (Territoriales) Herzogtum &lt;/li&gt;&lt;li&gt;&lt;strong&gt;Stellung der Herzogs als Reichsfürst &lt;/strong&gt;(=Ö erlangte die Reichsunmittelbarkeit) mit beschränkter Vasallenpflicht: Hoffart nur nach Bayern, Heerfahrt nur für benachbarte Länder (=gesteigertes Ansehen der Fürsten)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Stellung des Herzogs als oberster Gerichtsherr&lt;/strong&gt; (seine Zustimmung war nötig)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Bestimmung des Herzogtum als Weiberlehen&lt;/strong&gt; (=Anerkennung des subsidiären Erbrechts der Frau)&lt;/li&gt;&lt;li&gt;&lt;strong&gt;Ad-hoc-Nachfolgeregelung&lt;/strong&gt; (=Mitbelehnung der Herzogin) und das Recht bei Kinderlosigkeit seinen Nachfolger selbst zu bestimmen.&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;libertas affectandi?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Freies Verfügungsrecht über Länder&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Verkauf&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Schenkung&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Erbvertrag (kann bei Kinderlosigkeit eigenen Nachfolger bestimmen) &lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was war die Situation vor der Vergabe des Privilegium &lt;strong&gt;Minus&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Politische Konflikte zwischen Welfern und Staufern&lt;/li&gt;&lt;li&gt;Staufer (Konrad III)&amp;nbsp;wurde anstatt Welfer (Heinrich der Stolze) zum König&lt;/li&gt;&lt;li&gt;er entzog den Welfern das Herzogtum Bayern und übergab es seinem Stiefbruder (Babenberger Leopold IV) nach dessen Tod fiel es an seinen Bruder Heinrich II&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;War hat das Privilegium &lt;strong&gt;Minus &lt;/strong&gt;warum vergeben?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Friedrich Barbarossa wollte Konflikte zwischen Welfern und Staufern ausräumen&lt;/li&gt;&lt;li&gt;Heinrich II gab das Herzogtum Bayern an Friedrich zurück, dieser gab Bayern an die Welfer zurück.&lt;/li&gt;&lt;li&gt;Dafür bekam Heinrich II das Privilegium Minus&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wo wurde das &lt;strong&gt;subsidiäre Erbrecht&lt;/strong&gt; zum ersten Mal verankert?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;im Privilegium Minus&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Kann man in das Original des Privilegium &lt;strong&gt;Minus &lt;/strong&gt;Einsicht nehmen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, es wurde zerstört.&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das früheste Österreichische Reichsdokument?&lt;/p&gt;&lt;p&gt;Welche Umwandlung leitet es ein?&lt;/p&gt;&lt;p&gt;Wodurch wurde die Umwandlung ermöglicht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Privilegium Minus&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Übergang vom frühmittelalterlichen &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Personenverbandsstaat&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; zum spätmittelalterlichen &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Territorialstaat&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Herauslösung der Markgrafschaft Ostarrichi und Umwandlung in ein selbständiges Territorialherzogtum&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(112, 48, 160);"&gt;Was war das ersturkundlich verfassungsähnliche Dokument Österreichs?&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="color: rgb(112, 48, 160);"&gt;Welche Verfassungsdokumente folgten?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;P&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;rivilegium Minus&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Danach: pragmatische Sanktion 1713, &lt;/span&gt;&lt;span style="background-color: rgb(255, 255, 255); color: rgb(32, 33, 34);"&gt;Österreichisch-Ungarischen Ausgleich 1866 und Dezemberverfassung 1867&lt;/span&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Wann wurde das Privilegium &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Minus &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;eingeführt?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;1156&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das subsidiäre Erbrecht der Frau?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Außerordentliches Erbrecht der Frau&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist das Privilegium &lt;strong&gt;Maius&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Österreichischer Freiheitsbrief&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Wann wurde das&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; Privilegium &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Maius &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;verfasst?&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;strong&gt;1358&amp;nbsp;&lt;/strong&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Woraus bestand das &lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Privilegium &lt;/span&gt;&lt;strong&gt;Maius&lt;/strong&gt;?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Setzt sich zusammen aus 5 Dokumenten: Fälschung und Erweiterung des Privilegium minus und drei neue Freiheitsbriefe&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind die durch das &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Privilegium &lt;/span&gt;&lt;strong&gt;Maius &lt;/strong&gt;verliehenen Rechte?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Minimierung der Lehenspflichten&lt;/strong&gt;: Keine Hoffahrtspflicht, Heerfahrtspflicht nur für Ungarn&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ausbau der Landeshoheit&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;:&lt;/span&gt; Reichslehen sind Herzog unterstellt, er ist auch oberster Gerichtsherr&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Erbfolge und Verfügungsrecht&lt;/strong&gt;: &lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;libertas affectandi, &lt;/span&gt;Primogeniturprinzip (&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;Männliche Erben und subsidiär älteste Tochter)&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Rangerhöhung&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;:&lt;/span&gt; Herzog bekommt in der Rangordnung nach Kürfürsten den ersten Platz; und &lt;strong&gt;Titel Erzherzog&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;War das Privilegium &lt;strong&gt;Maius &lt;/strong&gt;sofort gültig?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Nein, Kaiser verweigerte Anerkennung; Erst im 15 JH (Habsburger Friedrich) und nochmal Kaiser Friedrich III bestätigt (mit Zustimmung der Kurfürsten)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was wurde beim Privilegium &lt;strong&gt;Maius &lt;/strong&gt;gefälscht?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Das Privilegium Minus (erweitert und Unterschrift des Kaiser Friedrich II)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(112, 48, 160); background-color: rgb(40, 45, 88);"&gt;Wann war das Privilegium &lt;/span&gt;&lt;strong style="color: rgb(112, 48, 160); background-color: rgb(40, 45, 88);"&gt;Maius &lt;/strong&gt;&lt;span style="color: rgb(112, 48, 160); background-color: rgb(40, 45, 88);"&gt;wieder von Bedeutung?&lt;/span&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; &lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Pragmatische Sanktion 1713 (Erweiterung des Privilegium Maius)&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Warum wurde das Privilegium &lt;strong&gt;Maius &lt;/strong&gt;erlassen?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Wahrscheinlich die Missachtung der Habsburger in der Goldenen Bulle 1356&lt;/li&gt;&lt;li&gt;Ziel war es die &lt;strong&gt;Unabhängigkeit sämtlicher Habsburgischen Länder&lt;/strong&gt; von jeder Einmischung der kaiserlichen Gewalt und die besondere &lt;strong&gt;Ehrenstellung des Herzogs &lt;/strong&gt;am kaiserlichen Hof&lt;/li&gt;&lt;/ul&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was sind Kurfürsten (in Hinsicht auf die Goldene Bulle)?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Ein bevorrechteter Kreis von &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Königswählern &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;(&lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Erzbischofe&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;, &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Pfalzgrafen&lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt; und &lt;/span&gt;&lt;strong style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;Herzoge &lt;/strong&gt;&lt;span style="color: rgb(238, 236, 246); background-color: rgb(40, 45, 88);"&gt;ohne Bayern)&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;Was ist die goldene Bulle?&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>&lt;ul&gt;&lt;li&gt;Die goldene Bulle war ein in Urkundenform verfasstes &lt;strong&gt;kaiserliches Gesetzbuch&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;von &lt;strong&gt;1356-1806&lt;/strong&gt; das &lt;strong&gt;wichtigste der Grundgesetze &lt;/strong&gt;des Heiligen Römischen Reichs&lt;/li&gt;&lt;li&gt;Es regelte vor allem die Modalitäten der &lt;strong&gt;Wahl und der Krönung der römisch-deutschen Könige und Kaiser&lt;/strong&gt; durch die Kurfürsten. &lt;/li&gt;&lt;li&gt;&lt;strong&gt;schriftliche&lt;/strong&gt; &lt;strong&gt;Fixierung &lt;/strong&gt;des sich gewohnheitsrechtlich herausgebildeten Wahlrechts. &lt;/li&gt;&lt;li&gt;Aktiv &lt;strong&gt;wahlberechtigt &lt;/strong&gt;waren ausschließlich die drei geistlichen und die vier weltlichen Kurfürsten. &lt;/li&gt;&lt;li&gt;Festgelegt wurden das &lt;strong&gt;Majoritätsprinzip &lt;/strong&gt;und der Grundsatz der &lt;strong&gt;örtlichen und zeitlichen Einheit&lt;/strong&gt; der Wahl.&lt;/li&gt;&lt;li&gt;Dieses Gesetz machte das Reich zu einem&lt;strong&gt; föderalen Staatsgebilde&lt;/strong&gt; und blieb bis zum Ende 1806 bestehen. &lt;/li&gt;&lt;li&gt;Die Goldene Bulle diente vor allem dazu, das römische bzw. &lt;strong&gt;päpstliche Einmischen zu unterbinden&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;Der &lt;strong&gt;König war oberster Lehnsherr&lt;/strong&gt; des Reiches, führte den Oberbefehl über das Reichsheer und verfügte über die Regalien (nutzbare königliche Hoheitsrechte).&amp;nbsp;&lt;/li&gt;&lt;/ul&gt;</t>
+    <t>&lt;p&gt;&lt;em&gt;Oktobererhebungen &lt;/em&gt;&lt;span style="background-color: rgb(40, 45, 88); color: rgb(238, 236, 246);"&gt;1848&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Kaiserlicher &lt;/strong&gt;Hof nach &lt;strong&gt;Olmütz&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Reichstag &lt;/strong&gt;nach &lt;strong&gt;Kremsier&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;um &lt;strong&gt;Einfluss &lt;/strong&gt;der &lt;strong&gt;Revolution &lt;/strong&gt;zu &lt;strong&gt;fliehen &lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Entwurf &lt;/em&gt;-&amp;gt; weil &lt;strong&gt;vor Kundmachung &lt;/strong&gt;Reichstag &lt;strong&gt;aufgelöst&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Inhalt&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Hochkonstitutionell&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gesetzgebung&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;em&gt;tag&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Volks &lt;/strong&gt;+&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Länder&lt;/strong&gt;kammer&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Selbstversammlungsrecht&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Suspensives &lt;/strong&gt;Veto des Kaisers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Kein Notverordnungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Wahlrecht&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;direkt&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;niedriger &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Steuerzensus&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;volle Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichtsbarkeit&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;unabhängig&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundrechte&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechte &lt;strong&gt;Katalog&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Durchsetzbar&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Geltungsbereich&lt;/em&gt;: &lt;strong&gt;nicht &lt;/strong&gt;für &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;Was ist die oktroyierte Märzverfassung von &lt;strong&gt;1849&lt;/strong&gt;?&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>&lt;ul&gt;&lt;li&gt;&lt;strong&gt;Herrscherwechsel &lt;/strong&gt;Dezember &lt;strong&gt;1848 &lt;/strong&gt;-&amp;gt; Franz Joseph&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Auflösung &lt;/strong&gt;des Reichstages in &lt;strong&gt;Kremsier&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;oktroyiert &lt;/strong&gt;Märzverfassung&lt;/li&gt;&lt;/ul&gt;&lt;p&gt;&lt;br&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Inhalt&lt;/span&gt;&lt;/p&gt;&lt;ul&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Früh&lt;/strong&gt;&lt;strong&gt;konstitutionell&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: wird &lt;strong&gt;nie&lt;/strong&gt; &lt;strong&gt;umgesetzt&lt;/strong&gt; -&amp;gt; &lt;strong&gt;Kaiser &lt;/strong&gt;regiert &lt;strong&gt;absolut&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gesetzgebung&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Reichs&lt;em&gt;tag&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;Ober + Unterhaus&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-2"&gt;&lt;strong&gt;&lt;em&gt;nie eingerichtet!&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;kein &lt;/strong&gt;&lt;strong&gt;Selbstversammlungsrecht&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Absolutes &lt;/strong&gt;Veto des Kaisers&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;&lt;em&gt;Notverordnungsrecht&lt;/em&gt;&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em&gt;Wahlrecht&lt;/em&gt;: &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;direkt&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;, &lt;/span&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;hoher &lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Steuerzensus&lt;/span&gt;&lt;/li&gt;&lt;li&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;keine&lt;/strong&gt;&lt;strong&gt; &lt;/strong&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Gewaltenteilung&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Gerichtsbarkeit&lt;/em&gt;:&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Öffentlichkeit &lt;/strong&gt;+ &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Mündlichkeit&lt;/strong&gt;&lt;span style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt; &lt;/span&gt;der Verfahren&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Anklageprinzip&lt;/strong&gt;&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Grundrechte&lt;/em&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;Grundrechte&lt;strong&gt;patent&lt;/strong&gt;&lt;/li&gt;&lt;li class="ql-indent-1"&gt;&lt;strong&gt;Durchsetzbar&lt;/strong&gt; vor Reichsgericht&lt;/li&gt;&lt;li class="ql-indent-1"&gt;aber: konnten in &lt;strong&gt;Krise ausgesetzt&lt;/strong&gt; werden&lt;/li&gt;&lt;li&gt;&lt;em style="background-color: rgba(0, 0, 0, 0); color: rgb(171, 127, 242);"&gt;Geltungsbereich&lt;/em&gt;: &lt;strong&gt;inkl&lt;/strong&gt;. &lt;strong style="background-color: rgba(0, 0, 0, 0); color: rgb(56, 190, 155);"&gt;Ungarn&lt;/strong&gt;&lt;/li&gt;&lt;/ul&gt;</t>
   </si>
 </sst>
 </file>
@@ -1294,7 +1648,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B149"/>
+  <dimension ref="A1:B208"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="2" width="20" customWidth="1"/>
@@ -2492,6 +2846,478 @@
         <v>297</v>
       </c>
     </row>
+    <row r="150" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A150" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="B150" s="2" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A151" s="2" t="s">
+        <v>300</v>
+      </c>
+      <c r="B151" s="2" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A152" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B152" s="2" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A153" s="2" t="s">
+        <v>304</v>
+      </c>
+      <c r="B153" s="2" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="154" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A154" s="2" t="s">
+        <v>306</v>
+      </c>
+      <c r="B154" s="2" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A155" s="2" t="s">
+        <v>308</v>
+      </c>
+      <c r="B155" s="2" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A156" s="2" t="s">
+        <v>310</v>
+      </c>
+      <c r="B156" s="2" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A157" s="2" t="s">
+        <v>312</v>
+      </c>
+      <c r="B157" s="2" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A158" s="2" t="s">
+        <v>314</v>
+      </c>
+      <c r="B158" s="2" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A159" s="2" t="s">
+        <v>316</v>
+      </c>
+      <c r="B159" s="2" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A160" s="2" t="s">
+        <v>318</v>
+      </c>
+      <c r="B160" s="2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="161" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A161" s="2" t="s">
+        <v>320</v>
+      </c>
+      <c r="B161" s="2" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A162" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B162" s="2" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A163" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="B163" s="2" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A164" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="B164" s="2" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A165" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="B165" s="2" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="166" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A166" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="B166" s="2" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="167" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A167" s="2" t="s">
+        <v>332</v>
+      </c>
+      <c r="B167" s="2" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="168" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A168" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="B168" s="2" t="s">
+        <v>335</v>
+      </c>
+    </row>
+    <row r="169" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A169" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="B169" s="2" t="s">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="170" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A170" s="2" t="s">
+        <v>338</v>
+      </c>
+      <c r="B170" s="2" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="171" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A171" s="2" t="s">
+        <v>340</v>
+      </c>
+      <c r="B171" s="2" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="172" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A172" s="2" t="s">
+        <v>342</v>
+      </c>
+      <c r="B172" s="2" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="173" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A173" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B173" s="2" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="174" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A174" s="2" t="s">
+        <v>346</v>
+      </c>
+      <c r="B174" s="2" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="175" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A175" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B175" s="2" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="176" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A176" s="2" t="s">
+        <v>350</v>
+      </c>
+      <c r="B176" s="2" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="177" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A177" s="2" t="s">
+        <v>352</v>
+      </c>
+      <c r="B177" s="2" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="178" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A178" s="2" t="s">
+        <v>354</v>
+      </c>
+      <c r="B178" s="2" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="179" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A179" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="B179" s="2" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="180" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A180" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="B180" s="2" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="181" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A181" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="B181" s="2" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="182" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A182" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="B182" s="2" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="183" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A183" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="B183" s="2" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="184" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A184" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="B184" s="2" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="185" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A185" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="B185" s="2" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="186" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A186" s="2" t="s">
+        <v>370</v>
+      </c>
+      <c r="B186" s="2" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="187" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A187" s="2" t="s">
+        <v>372</v>
+      </c>
+      <c r="B187" s="2" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="188" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A188" s="2" t="s">
+        <v>374</v>
+      </c>
+      <c r="B188" s="2" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="189" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A189" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="B189" s="2" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="190" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A190" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="B190" s="2" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="191" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A191" s="2" t="s">
+        <v>380</v>
+      </c>
+      <c r="B191" s="2" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="192" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A192" s="2" t="s">
+        <v>382</v>
+      </c>
+      <c r="B192" s="2" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="193" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A193" s="2" t="s">
+        <v>384</v>
+      </c>
+      <c r="B193" s="2" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="194" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A194" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="B194" s="2" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="195" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A195" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="B195" s="2" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A196" s="2" t="s">
+        <v>390</v>
+      </c>
+      <c r="B196" s="2" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="197" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A197" s="2" t="s">
+        <v>392</v>
+      </c>
+      <c r="B197" s="2" t="s">
+        <v>393</v>
+      </c>
+    </row>
+    <row r="198" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A198" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="B198" s="2" t="s">
+        <v>395</v>
+      </c>
+    </row>
+    <row r="199" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A199" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="B199" s="2" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="200" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A200" s="2" t="s">
+        <v>398</v>
+      </c>
+      <c r="B200" s="2" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="201" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A201" s="2" t="s">
+        <v>400</v>
+      </c>
+      <c r="B201" s="2" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="202" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A202" s="2" t="s">
+        <v>402</v>
+      </c>
+      <c r="B202" s="2" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A203" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="B203" s="2" t="s">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="204" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A204" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="B204" s="2" t="s">
+        <v>407</v>
+      </c>
+    </row>
+    <row r="205" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A205" s="2" t="s">
+        <v>408</v>
+      </c>
+      <c r="B205" s="2" t="s">
+        <v>409</v>
+      </c>
+    </row>
+    <row r="206" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="B206" s="2" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="207" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A207" s="2" t="s">
+        <v>412</v>
+      </c>
+      <c r="B207" s="2" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="208" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="B208" s="2" t="s">
+        <v>415</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>